<commit_message>
loading scada data lazyly and using remc avc pnt in scada report
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="regional_profile" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="257">
   <si>
     <t>name</t>
   </si>
@@ -104,27 +104,18 @@
     <t>dummy</t>
   </si>
   <si>
-    <t>WREMCPRI.SCADA01.00045859</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00032758</t>
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00045850</t>
   </si>
   <si>
-    <t>WREMCPRI.SCADA01.00045861</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00032759</t>
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00045848</t>
   </si>
   <si>
-    <t>WREMCPRI.SCADA01.00045860</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00032413</t>
   </si>
   <si>
@@ -284,52 +275,34 @@
     <t>WREMCPRI.SCADA01.00032726</t>
   </si>
   <si>
-    <t>WREMCPRI.SCADA01.00031527</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00046640</t>
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00046641</t>
   </si>
   <si>
-    <t>WREMCPRI.SCADA01.00045864</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00030482</t>
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00045845</t>
   </si>
   <si>
-    <t>WREMCPRI.SCADA01.00045863</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00037226</t>
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00045846</t>
   </si>
   <si>
-    <t>WREMCPRI.SCADA01.00045862</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00030481</t>
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00045847</t>
   </si>
   <si>
-    <t>WREMCPRI.SCADA01.00045865</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00045558</t>
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00045844</t>
-  </si>
-  <si>
-    <t>WREMCPRI.SCADA01.00045866</t>
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00032415</t>
@@ -1207,7 +1180,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,7 +1215,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>19</v>
@@ -1250,7 +1223,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -1258,7 +1231,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -1266,7 +1239,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -1274,7 +1247,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -1282,7 +1255,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -1290,7 +1263,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>19</v>
@@ -1298,16 +1271,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B9" s="4">
         <v>14848.26</v>
       </c>
+      <c r="C9" t="s">
+        <v>196</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>5</v>
@@ -1315,16 +1291,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B10" s="4">
         <v>6588.0749999999998</v>
       </c>
+      <c r="C10" t="s">
+        <v>191</v>
+      </c>
       <c r="D10" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>5</v>
@@ -1338,12 +1317,14 @@
         <f>SUM(B9:B10)</f>
         <v>21436.334999999999</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" t="s">
+        <v>186</v>
+      </c>
       <c r="D11" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>5</v>
@@ -1351,7 +1332,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
@@ -1359,7 +1340,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
@@ -1393,24 +1374,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -1418,7 +1399,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -1426,7 +1407,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -1434,7 +1415,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -1442,7 +1423,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -1450,7 +1431,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -1458,58 +1439,58 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C8" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D9" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
@@ -1517,58 +1498,58 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D12" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
         <v>65</v>
-      </c>
-      <c r="B13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C13" t="s">
-        <v>220</v>
-      </c>
-      <c r="D13" t="s">
-        <v>218</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
@@ -1576,53 +1557,53 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C16" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D16" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C17" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D17" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1652,10 +1633,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -1666,7 +1647,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -1674,7 +1655,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -1682,7 +1663,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -1690,7 +1671,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -1698,7 +1679,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -1706,7 +1687,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
@@ -1714,52 +1695,52 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1769,86 +1750,86 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1858,64 +1839,64 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1945,21 +1926,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -1967,7 +1948,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -1975,7 +1956,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -1983,7 +1964,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -1991,7 +1972,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -1999,52 +1980,52 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C7" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -2052,52 +2033,52 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
         <v>65</v>
-      </c>
-      <c r="B12" t="s">
-        <v>217</v>
-      </c>
-      <c r="C12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -2105,47 +2086,47 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C16" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2175,12 +2156,12 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -2188,7 +2169,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -2196,7 +2177,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -2204,7 +2185,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -2212,35 +2193,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2272,7 +2253,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -2280,7 +2261,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -2288,7 +2269,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -2296,7 +2277,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -2304,7 +2285,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -2312,7 +2293,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -2320,46 +2301,46 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -2367,74 +2348,74 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>253</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -2442,60 +2423,60 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -2503,35 +2484,35 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2565,21 +2546,21 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -2587,7 +2568,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -2595,58 +2576,58 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -2654,58 +2635,58 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>259</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -2714,58 +2695,58 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
@@ -2773,7 +2754,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -2784,7 +2765,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
@@ -2795,13 +2776,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2829,15 +2810,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>15</v>
@@ -2848,7 +2829,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>16</v>
@@ -2859,7 +2840,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>16</v>
@@ -2888,7 +2869,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2931,12 +2912,12 @@
         <v>11</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>19</v>
@@ -2944,7 +2925,7 @@
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>19</v>
@@ -2952,7 +2933,7 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>19</v>
@@ -2960,7 +2941,7 @@
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>19</v>
@@ -2968,7 +2949,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>19</v>
@@ -2976,80 +2957,80 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1">
         <v>250</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>95</v>
+      <c r="C7" t="s">
+        <v>140</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1">
         <v>184.5</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>92</v>
+      <c r="C8" t="s">
+        <v>160</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1">
         <f>SUM(B7:B8)</f>
         <v>434.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>19</v>
@@ -3057,138 +3038,138 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11" s="4">
         <v>250</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>89</v>
+      <c r="C11" t="s">
+        <v>165</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" s="4">
         <v>226.8</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>86</v>
+      <c r="C12" t="s">
+        <v>175</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B13" s="4">
         <v>200</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>83</v>
+      <c r="C13" t="s">
+        <v>170</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B14" s="4">
         <v>176.4</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>80</v>
+      <c r="C14" t="s">
+        <v>180</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" s="4">
         <f>SUM(B11:B14)</f>
         <v>853.19999999999993</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -3196,7 +3177,7 @@
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>19</v>
@@ -3204,94 +3185,94 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B18" s="4">
         <v>250</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F18" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B19" s="4">
         <v>250</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="F19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B20" s="4">
         <v>250</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
+      <c r="C20" t="s">
+        <v>155</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B21" s="4">
         <f>SUM(B18:B20)</f>
@@ -3301,16 +3282,16 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
@@ -3319,7 +3300,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B23" s="4">
         <f>B21</f>
@@ -3357,7 +3338,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B25" s="4">
         <f>SUM(B23:B24)</f>
@@ -3367,15 +3348,15 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3403,8 +3384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3440,18 +3421,18 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>19</v>
@@ -3459,7 +3440,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>19</v>
@@ -3467,7 +3448,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>19</v>
@@ -3475,7 +3456,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>19</v>
@@ -3483,76 +3464,82 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4">
         <v>2248</v>
       </c>
+      <c r="C6" t="s">
+        <v>221</v>
+      </c>
       <c r="D6" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4">
         <v>6265</v>
       </c>
+      <c r="C7" t="s">
+        <v>226</v>
+      </c>
       <c r="D7" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4">
         <f>SUM(B6:B7)</f>
         <v>8513</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>19</v>
@@ -3560,74 +3547,80 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" s="4">
         <v>1388</v>
       </c>
+      <c r="C10" t="s">
+        <v>211</v>
+      </c>
       <c r="D10" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" s="4">
         <v>4953</v>
       </c>
+      <c r="C11" t="s">
+        <v>216</v>
+      </c>
       <c r="D11" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" s="4">
         <f>SUM(B10:B11)</f>
         <v>6341</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>19</v>
@@ -3635,74 +3628,80 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B14" s="4">
         <v>2202.0749999999998</v>
       </c>
+      <c r="C14" t="s">
+        <v>201</v>
+      </c>
       <c r="D14" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B15" s="4">
         <v>2442.56</v>
       </c>
+      <c r="C15" t="s">
+        <v>206</v>
+      </c>
       <c r="D15" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4">
         <f>SUM(B14:B15)</f>
         <v>4644.6350000000002</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>19</v>
@@ -3710,7 +3709,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B18" s="4">
         <f>B7+B11+B15</f>
@@ -3725,7 +3724,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B19" s="4">
         <f>B6+B10+B14</f>
@@ -3740,22 +3739,22 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
         <v>19498.634999999998</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>19</v>
@@ -3787,10 +3786,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
@@ -3798,7 +3797,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
@@ -3806,7 +3805,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -3814,7 +3813,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>19</v>
@@ -3822,7 +3821,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>19</v>
@@ -3830,13 +3829,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -3844,13 +3843,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
@@ -3858,13 +3857,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>5</v>
@@ -3872,7 +3871,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -3880,7 +3879,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
@@ -3914,16 +3913,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -3931,7 +3930,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>19</v>
@@ -3939,7 +3938,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3951,7 +3950,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3963,7 +3962,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -3975,7 +3974,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3987,7 +3986,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3999,7 +3998,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -4011,7 +4010,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -4023,7 +4022,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -4038,16 +4037,16 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D11" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E11" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>5</v>
@@ -4058,16 +4057,16 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D12" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E12" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>5</v>
@@ -4075,19 +4074,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D13" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E13" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>5</v>
@@ -4095,19 +4094,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D14" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E14" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>5</v>
@@ -4115,19 +4114,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>5</v>
@@ -4135,19 +4134,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E16" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>5</v>
@@ -4162,8 +4161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4181,16 +4180,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -4198,7 +4197,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>19</v>
@@ -4206,7 +4205,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -4218,7 +4217,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -4230,7 +4229,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -4242,7 +4241,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -4256,16 +4255,16 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>5</v>
@@ -4276,16 +4275,16 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E8" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>5</v>
@@ -4293,19 +4292,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D9" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E9" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>5</v>
@@ -4313,19 +4312,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>5</v>
@@ -4333,19 +4332,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E11" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>5</v>
@@ -4353,19 +4352,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E12" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>5</v>
@@ -4401,19 +4400,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -4424,7 +4423,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>19</v>
@@ -4432,7 +4431,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -4445,7 +4444,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -4458,7 +4457,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -4471,7 +4470,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4"/>
       <c r="D6" s="4"/>
@@ -4483,7 +4482,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B7" s="4"/>
       <c r="D7" s="4"/>
@@ -4495,70 +4494,70 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F9" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -4571,122 +4570,122 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E12" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C13" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F13" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F14" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D15" t="s">
-        <v>187</v>
-      </c>
-      <c r="E15" t="s">
-        <v>188</v>
-      </c>
-      <c r="F15" t="s">
-        <v>189</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -4699,96 +4698,96 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F18" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E19" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F19" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F20" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="H21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -4801,22 +4800,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E23" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
@@ -4824,22 +4823,22 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C24" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F24" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
@@ -4847,22 +4846,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E25" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F25" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
@@ -4896,36 +4895,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -4933,7 +4932,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -4941,7 +4940,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
@@ -4949,7 +4948,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
         <v>19</v>
@@ -4957,7 +4956,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
@@ -4965,7 +4964,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
         <v>19</v>
@@ -4973,7 +4972,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -4981,7 +4980,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G9" t="s">
         <v>19</v>
@@ -4989,7 +4988,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G10" t="s">
         <v>19</v>
@@ -4997,7 +4996,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G11" t="s">
         <v>19</v>
@@ -5005,7 +5004,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G12" t="s">
         <v>19</v>
@@ -5013,7 +5012,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
@@ -5021,7 +5020,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
@@ -5029,7 +5028,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
@@ -5037,82 +5036,82 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C16" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D16" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E16" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F16" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I16" t="s">
         <v>2</v>
       </c>
       <c r="J16" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C17" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D17" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E17" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F17" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I17" t="s">
         <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
@@ -5120,82 +5119,82 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D20" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E20" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F20" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I20" t="s">
         <v>2</v>
       </c>
       <c r="J20" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" t="s">
+        <v>209</v>
+      </c>
+      <c r="E21" t="s">
+        <v>210</v>
+      </c>
+      <c r="F21" t="s">
+        <v>211</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
         <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>216</v>
-      </c>
-      <c r="C21" t="s">
-        <v>217</v>
-      </c>
-      <c r="D21" t="s">
-        <v>218</v>
-      </c>
-      <c r="E21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F21" t="s">
-        <v>220</v>
-      </c>
-      <c r="G21" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" t="s">
-        <v>68</v>
       </c>
       <c r="I21" t="s">
         <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G23" t="s">
         <v>19</v>
@@ -5203,82 +5202,82 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C24" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D24" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E24" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="F24" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I24" t="s">
         <v>2</v>
       </c>
       <c r="J24" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C25" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D25" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E25" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F25" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I25" t="s">
         <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G27" t="s">
         <v>19</v>
@@ -5286,7 +5285,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="G28" t="s">
         <v>13</v>
@@ -5295,12 +5294,12 @@
         <v>2</v>
       </c>
       <c r="J28" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="G29" t="s">
         <v>13</v>
@@ -5309,18 +5308,18 @@
         <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="G30" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="J30" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -5351,13 +5350,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -5368,7 +5367,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -5376,7 +5375,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -5384,7 +5383,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -5392,7 +5391,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -5400,7 +5399,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -5408,7 +5407,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -5416,58 +5415,58 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5478,98 +5477,98 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D15" t="s">
-        <v>187</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -5580,73 +5579,73 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D20" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rmse perc formula change, num err blks formula change
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="regional_profile" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="322">
   <si>
     <t>name</t>
   </si>
@@ -1383,7 +1383,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,22 +1816,23 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1839,64 +1840,72 @@
         <v>96</v>
       </c>
       <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="4"/>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="4"/>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="4"/>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -1904,16 +1913,19 @@
         <v>120</v>
       </c>
       <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1921,37 +1933,41 @@
         <v>140</v>
       </c>
       <c r="C9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1959,16 +1975,19 @@
         <v>145</v>
       </c>
       <c r="C12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1976,16 +1995,19 @@
         <v>155</v>
       </c>
       <c r="C13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" t="s">
         <v>156</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1993,16 +2015,19 @@
         <v>150</v>
       </c>
       <c r="C14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" t="s">
         <v>151</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2010,37 +2035,41 @@
         <v>160</v>
       </c>
       <c r="C15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
         <v>161</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="4"/>
+      <c r="E17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -2048,16 +2077,19 @@
         <v>130</v>
       </c>
       <c r="C18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" t="s">
         <v>131</v>
       </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
       <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -2065,16 +2097,19 @@
         <v>125</v>
       </c>
       <c r="C19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" t="s">
         <v>126</v>
       </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
       <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -2082,25 +2117,31 @@
         <v>135</v>
       </c>
       <c r="C20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" t="s">
         <v>136</v>
       </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
       <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>87</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2109,22 +2150,23 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2132,56 +2174,59 @@
         <v>96</v>
       </c>
       <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2189,16 +2234,19 @@
         <v>206</v>
       </c>
       <c r="C7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" t="s">
         <v>207</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
       <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2206,35 +2254,38 @@
         <v>201</v>
       </c>
       <c r="C8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" t="s">
         <v>202</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
       <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -2242,16 +2293,19 @@
         <v>196</v>
       </c>
       <c r="C11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" t="s">
         <v>197</v>
       </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
       <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2259,35 +2313,38 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" t="s">
         <v>192</v>
       </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
       <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -2295,16 +2352,19 @@
         <v>186</v>
       </c>
       <c r="C15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" t="s">
         <v>187</v>
       </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
       <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
@@ -2312,23 +2372,26 @@
         <v>181</v>
       </c>
       <c r="C16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" t="s">
         <v>182</v>
       </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
       <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>26</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3744,7 +3807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -5263,7 +5326,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D25"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5760,7 +5823,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
actual data taken from scada file
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="regional_profile" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="334">
   <si>
     <t>name</t>
   </si>
@@ -995,6 +995,57 @@
   </si>
   <si>
     <t>Maharashtra Solar Forecast R16</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00032415</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00045558</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00030481</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00037226</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00030482</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00046640</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00032758</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00032759</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00032413</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00045841</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00045838</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00045839</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00045630</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00045129</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00037566</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00037565</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00034364</t>
   </si>
 </sst>
 </file>
@@ -1367,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,7 +1519,7 @@
         <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>327</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>61</v>
@@ -1488,7 +1539,7 @@
         <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>167</v>
+        <v>328</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>62</v>
@@ -1508,7 +1559,7 @@
         <v>164</v>
       </c>
       <c r="D11" t="s">
-        <v>162</v>
+        <v>326</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>63</v>
@@ -3800,7 +3851,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3899,7 +3950,7 @@
         <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>317</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>69</v>
@@ -3928,7 +3979,7 @@
         <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>318</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>68</v>
@@ -3981,7 +4032,7 @@
         <v>143</v>
       </c>
       <c r="D11" t="s">
-        <v>141</v>
+        <v>319</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>67</v>
@@ -4010,7 +4061,7 @@
         <v>153</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>320</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>66</v>
@@ -4039,7 +4090,7 @@
         <v>148</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>321</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>65</v>
@@ -4068,7 +4119,7 @@
         <v>158</v>
       </c>
       <c r="D14" t="s">
-        <v>156</v>
+        <v>322</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>64</v>
@@ -4130,7 +4181,7 @@
         <v>128</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>323</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>18</v>
@@ -4159,7 +4210,7 @@
         <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>324</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>19</v>
@@ -4188,7 +4239,7 @@
         <v>133</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>325</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>20</v>
@@ -4259,7 +4310,8 @@
         <v>12</v>
       </c>
       <c r="B24" s="4">
-        <v>1360.8</v>
+        <f>B15+B9</f>
+        <v>1360.9</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24"/>
@@ -4277,7 +4329,8 @@
         <v>79</v>
       </c>
       <c r="B25" s="4">
-        <v>2110.8000000000002</v>
+        <f>B24+B23</f>
+        <v>2110.9</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -4319,8 +4372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4410,7 +4463,7 @@
         <v>199</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>329</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>28</v>
@@ -4439,7 +4492,7 @@
         <v>204</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
+        <v>330</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>27</v>
@@ -4493,7 +4546,7 @@
         <v>189</v>
       </c>
       <c r="D10" t="s">
-        <v>187</v>
+        <v>331</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>70</v>
@@ -4522,7 +4575,7 @@
         <v>194</v>
       </c>
       <c r="D11" t="s">
-        <v>192</v>
+        <v>332</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>71</v>
@@ -4545,7 +4598,8 @@
         <v>54</v>
       </c>
       <c r="B12" s="4">
-        <v>6411.39</v>
+        <f>B10+B11</f>
+        <v>6411.3899999999994</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>26</v>
@@ -4573,7 +4627,7 @@
         <v>179</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>333</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>72</v>
@@ -4602,7 +4656,7 @@
         <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>182</v>
+        <v>333</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>73</v>
@@ -4625,6 +4679,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="4">
+        <f>B15+B14</f>
         <v>3952.05</v>
       </c>
       <c r="F16" s="4" t="s">

</xml_diff>

<commit_message>
mp solar pnt change
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="regional_profile" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="335">
   <si>
     <t>name</t>
   </si>
@@ -1046,6 +1046,9 @@
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00034364</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00034363</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1077,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1082,12 +1085,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1101,6 +1119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4372,8 +4391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4626,8 +4645,8 @@
       <c r="C14" t="s">
         <v>179</v>
       </c>
-      <c r="D14" t="s">
-        <v>333</v>
+      <c r="D14" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
change in installed capacity
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1525,7 +1525,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="4">
-        <v>15176</v>
+        <v>15184</v>
       </c>
       <c r="C9" t="s">
         <v>174</v>
@@ -1545,7 +1545,7 @@
         <v>89</v>
       </c>
       <c r="B10" s="4">
-        <v>5949</v>
+        <v>5983</v>
       </c>
       <c r="C10" t="s">
         <v>169</v>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="B11" s="4">
         <f>B10+B9</f>
-        <v>21125</v>
+        <v>21167</v>
       </c>
       <c r="C11" t="s">
         <v>164</v>
@@ -4413,7 +4413,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4580,7 +4580,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="4">
-        <v>1411</v>
+        <v>1445</v>
       </c>
       <c r="C10" t="s">
         <v>189</v>
@@ -4609,7 +4609,7 @@
         <v>53</v>
       </c>
       <c r="B11" s="4">
-        <v>5000</v>
+        <v>5008</v>
       </c>
       <c r="C11" t="s">
         <v>194</v>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="B12" s="4">
         <f>B10+B11</f>
-        <v>6411</v>
+        <v>6453</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>26</v>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="B18" s="4">
         <f>B7+B11+B15</f>
-        <v>13677</v>
+        <v>13685</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="B19" s="4">
         <f>B6+B10+B14</f>
-        <v>5199</v>
+        <v>5233</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -4773,7 +4773,7 @@
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
-        <v>18876</v>
+        <v>18918</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
minor name change of Inox
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.60\d$\wrldc_remc_reports_generator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\Python Projects\remc_report_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A16C06-4735-42C1-9C76-E6BB98A695E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -36,7 +35,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">remc_graph_data!$A$1:$C$56</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="347">
   <si>
     <t>name</t>
   </si>
@@ -1084,12 +1083,15 @@
   </si>
   <si>
     <t>REMC Report/WR</t>
+  </si>
+  <si>
+    <t>Inox (Dayapar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1142,7 +1144,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1453,7 +1455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1500,7 +1502,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1826,7 +1828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2086,7 +2088,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -2420,7 +2422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -2672,7 +2674,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
@@ -2768,7 +2770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3059,7 +3061,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -3337,7 +3339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -3975,7 +3977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4083,10 +4085,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -4259,11 +4261,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4493,7 +4495,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>346</v>
       </c>
       <c r="B13" s="4">
         <v>200</v>
@@ -4808,7 +4810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5195,7 +5197,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5320,7 +5322,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5587,7 +5589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5805,7 +5807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6302,7 +6304,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
minor changes in graph headings
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="14" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -758,39 +758,21 @@
     <t>Regional Actual</t>
   </si>
   <si>
-    <t>Regional Actual Prev</t>
-  </si>
-  <si>
     <t>Regional Solar Actual</t>
   </si>
   <si>
-    <t>Regional Solar Actual Prev</t>
-  </si>
-  <si>
     <t>Regional Wind Actual</t>
   </si>
   <si>
-    <t>Regional Wind Actual Prev</t>
-  </si>
-  <si>
     <t>ISTS Solar Actual</t>
   </si>
   <si>
-    <t>ISTS Solar Actual Prev</t>
-  </si>
-  <si>
     <t>ISTS Wind Actual</t>
   </si>
   <si>
-    <t>ISTS Wind Actual Prev</t>
-  </si>
-  <si>
     <t>ISTS Renewable Actual</t>
   </si>
   <si>
-    <t>ISTS Renewable Actual Prev</t>
-  </si>
-  <si>
     <t>OKWPL_RE-WIND_WIND_Act,RPL_SECI-II_RE-WIND_WIND_Act</t>
   </si>
   <si>
@@ -800,9 +782,6 @@
     <t>Bachau Pooling Actual</t>
   </si>
   <si>
-    <t>Bachau Pooling Actual Prev</t>
-  </si>
-  <si>
     <t>GIWEL_SECI-II_RE-WIND_WIND_16,GIWEL_SECI-III_RE-WIND_WIND_16,IWISL-WIND_WIND_16,AGEMPL-WIND_WIND_16</t>
   </si>
   <si>
@@ -812,9 +791,6 @@
     <t>Bhuj Pooling Actual</t>
   </si>
   <si>
-    <t>Bhuj Pooling Actual Prev</t>
-  </si>
-  <si>
     <t>Arinsun_RUMS-SOLAR_SOLAR_16,Acme_RUMS-SOLAR_SOLAR_16,Mahindra_RUMS-SOLAR_SOLAR_16</t>
   </si>
   <si>
@@ -824,15 +800,9 @@
     <t>Rewa Pooling Actual</t>
   </si>
   <si>
-    <t>Rewa Pooling Actual Prev</t>
-  </si>
-  <si>
     <t>Gujarat Renewable Actual</t>
   </si>
   <si>
-    <t>Gujarat Renewable Actual Prev</t>
-  </si>
-  <si>
     <t>Gujarat_Gujarat_WIND _16,Gujarat_Gujarat_SOLAR _16</t>
   </si>
   <si>
@@ -842,33 +812,18 @@
     <t>Gujarat Wind Actual</t>
   </si>
   <si>
-    <t>Gujarat Wind Actual Prev</t>
-  </si>
-  <si>
     <t>Gujarat Solar Actual</t>
   </si>
   <si>
-    <t>Gujarat Solar Actual Prev</t>
-  </si>
-  <si>
     <t>Madhya Pradesh Renewable Actual</t>
   </si>
   <si>
-    <t>Madhya Pradesh Renewable Actual Prev</t>
-  </si>
-  <si>
     <t>Madhya Pradesh Wind Actual</t>
   </si>
   <si>
-    <t>Madhya Pradesh Wind Actual Prev</t>
-  </si>
-  <si>
     <t>Madhya Pradesh Solar Actual</t>
   </si>
   <si>
-    <t>Madhya Pradesh Solar Actual Prev</t>
-  </si>
-  <si>
     <t>Madhya Pradesh_Madhya Pradesh_WIND _16,Madhya Pradesh_Madhya Pradesh_SOLAR _16</t>
   </si>
   <si>
@@ -878,21 +833,12 @@
     <t>Maharashtra Renewable Actual</t>
   </si>
   <si>
-    <t>Maharashtra Renewable Actual Prev</t>
-  </si>
-  <si>
     <t>Maharashtra Wind Actual</t>
   </si>
   <si>
-    <t>Maharashtra Wind Actual Prev</t>
-  </si>
-  <si>
     <t>Maharashtra Solar Actual</t>
   </si>
   <si>
-    <t>Maharashtra Solar Actual Prev</t>
-  </si>
-  <si>
     <t>Maharastra_Maharastra_WIND _16,Maharastra_Maharastra_SOLAR _16</t>
   </si>
   <si>
@@ -1086,6 +1032,60 @@
   </si>
   <si>
     <t>Inox (Dayapar)</t>
+  </si>
+  <si>
+    <t>Regional Actual for previous day</t>
+  </si>
+  <si>
+    <t>Regional Solar Actual for previous day</t>
+  </si>
+  <si>
+    <t>Regional Wind Actual for previous day</t>
+  </si>
+  <si>
+    <t>ISTS Renewable Actual for previous day</t>
+  </si>
+  <si>
+    <t>ISTS Solar Actual for previous day</t>
+  </si>
+  <si>
+    <t>ISTS Wind Actual for previous day</t>
+  </si>
+  <si>
+    <t>Bachau Pooling Actual for previous day</t>
+  </si>
+  <si>
+    <t>Bhuj Pooling Actual for previous day</t>
+  </si>
+  <si>
+    <t>Rewa Pooling Actual for previous day</t>
+  </si>
+  <si>
+    <t>Gujarat Renewable Actual for previous day</t>
+  </si>
+  <si>
+    <t>Gujarat Wind Actual for previous day</t>
+  </si>
+  <si>
+    <t>Gujarat Solar Actual for previous day</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh Renewable Actual for previous day</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh Wind Actual for previous day</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh Solar Actual for previous day</t>
+  </si>
+  <si>
+    <t>Maharashtra Renewable Actual for previous day</t>
+  </si>
+  <si>
+    <t>Maharashtra Wind Actual for previous day</t>
+  </si>
+  <si>
+    <t>Maharashtra Solar Actual for previous day</t>
   </si>
 </sst>
 </file>
@@ -1466,34 +1466,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="B3" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="B4" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -3342,8 +3342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3367,24 +3367,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="C2" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3395,579 +3395,579 @@
         <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>237</v>
+        <v>329</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>162</v>
       </c>
       <c r="C5" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C7" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>239</v>
+        <v>330</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C8" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>171</v>
       </c>
       <c r="C9" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>172</v>
       </c>
       <c r="C10" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>241</v>
+        <v>331</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>172</v>
       </c>
       <c r="C11" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>247</v>
+        <v>332</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>243</v>
+        <v>333</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>245</v>
+        <v>334</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C21" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C22" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>251</v>
+        <v>335</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C23" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C24" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C25" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>255</v>
+        <v>336</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C26" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C27" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C28" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>259</v>
+        <v>337</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C29" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C30" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="C31" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>261</v>
+        <v>338</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="C32" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>201</v>
       </c>
       <c r="C33" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>202</v>
       </c>
       <c r="C34" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>265</v>
+        <v>339</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>202</v>
       </c>
       <c r="C35" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>196</v>
       </c>
       <c r="C36" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>197</v>
       </c>
       <c r="C37" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>267</v>
+        <v>340</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>197</v>
       </c>
       <c r="C38" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C39" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C40" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>269</v>
+        <v>341</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C41" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>181</v>
       </c>
       <c r="C42" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>182</v>
       </c>
       <c r="C43" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>271</v>
+        <v>342</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>176</v>
       </c>
       <c r="C45" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>177</v>
       </c>
       <c r="C46" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>273</v>
+        <v>343</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>177</v>
       </c>
       <c r="C47" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="C48" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="C49" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>277</v>
+        <v>344</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="C50" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>191</v>
       </c>
       <c r="C51" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>192</v>
       </c>
       <c r="C52" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>279</v>
+        <v>345</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>192</v>
       </c>
       <c r="C53" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>186</v>
       </c>
       <c r="C54" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>187</v>
       </c>
       <c r="C55" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>281</v>
+        <v>346</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>187</v>
       </c>
       <c r="C56" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -4004,10 +4004,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -4015,7 +4015,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -4026,10 +4026,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -4037,7 +4037,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="B5" t="s">
         <v>74</v>
@@ -4048,10 +4048,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -4059,7 +4059,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -4070,10 +4070,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="B8" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -4189,7 +4189,7 @@
         <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>61</v>
@@ -4209,7 +4209,7 @@
         <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>62</v>
@@ -4230,7 +4230,7 @@
         <v>164</v>
       </c>
       <c r="D11" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>63</v>
@@ -4364,7 +4364,7 @@
         <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>69</v>
@@ -4393,7 +4393,7 @@
         <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>68</v>
@@ -4446,7 +4446,7 @@
         <v>143</v>
       </c>
       <c r="D11" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>67</v>
@@ -4475,7 +4475,7 @@
         <v>153</v>
       </c>
       <c r="D12" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>66</v>
@@ -4495,7 +4495,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="B13" s="4">
         <v>200</v>
@@ -4504,7 +4504,7 @@
         <v>148</v>
       </c>
       <c r="D13" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>65</v>
@@ -4533,7 +4533,7 @@
         <v>158</v>
       </c>
       <c r="D14" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>64</v>
@@ -4553,17 +4553,17 @@
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="B15" s="2">
         <v>214</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>5</v>
@@ -4622,7 +4622,7 @@
         <v>128</v>
       </c>
       <c r="D19" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>18</v>
@@ -4651,7 +4651,7 @@
         <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>19</v>
@@ -4680,7 +4680,7 @@
         <v>133</v>
       </c>
       <c r="D21" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>20</v>
@@ -4904,7 +4904,7 @@
         <v>199</v>
       </c>
       <c r="D6" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>28</v>
@@ -4933,7 +4933,7 @@
         <v>204</v>
       </c>
       <c r="D7" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>27</v>
@@ -4987,7 +4987,7 @@
         <v>189</v>
       </c>
       <c r="D10" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>70</v>
@@ -5016,7 +5016,7 @@
         <v>194</v>
       </c>
       <c r="D11" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>71</v>
@@ -5068,7 +5068,7 @@
         <v>179</v>
       </c>
       <c r="D14" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>72</v>
@@ -5097,7 +5097,7 @@
         <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>73</v>
@@ -5200,8 +5200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added alfnar and renew ap2 in configg
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="14" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="scada_graph_data" sheetId="17" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">remc_graph_data!$A$1:$C$56</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="362">
   <si>
     <t>name</t>
   </si>
@@ -1086,6 +1086,51 @@
   </si>
   <si>
     <t>Maharashtra Solar Actual for previous day</t>
+  </si>
+  <si>
+    <t>AlfanarWind_SECI-III-WIND_WIND_AVC</t>
+  </si>
+  <si>
+    <t>Renew(AP2)</t>
+  </si>
+  <si>
+    <t>AlfanarWind_SECI-III-WIND_WIND_R0</t>
+  </si>
+  <si>
+    <t>AlfanarWind_SECI-III-WIND_WIND_16</t>
+  </si>
+  <si>
+    <t>AlfanarWind_SECI-III-WIND_WIND_Act</t>
+  </si>
+  <si>
+    <t>AlfanarWind_SECI-III-WIND_WIND_CUF</t>
+  </si>
+  <si>
+    <t>RWE_AP2_SECI-III-WIND_WIND_R0</t>
+  </si>
+  <si>
+    <t>RWE_AP2_SECI-III-WIND_WIND_16</t>
+  </si>
+  <si>
+    <t>RWE_AP2_SECI-III-WIND_WIND_Act</t>
+  </si>
+  <si>
+    <t>RWE_AP2_SECI-III-WIND_WIND_CUF</t>
+  </si>
+  <si>
+    <t>RWE_AP2_SECI-III-WIND_WIND_AVC</t>
+  </si>
+  <si>
+    <t>AlfanarWind_SECI-III-WIND_WIND</t>
+  </si>
+  <si>
+    <t>RWE_AP2_SECI-III-WIND_WIND</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00047399</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00046369</t>
   </si>
 </sst>
 </file>
@@ -1503,10 +1548,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,78 +1776,78 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>315</v>
+      </c>
+      <c r="B16" t="s">
+        <v>350</v>
+      </c>
+      <c r="C16" t="s">
+        <v>347</v>
+      </c>
+      <c r="D16" t="s">
+        <v>351</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="A17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" t="s">
+        <v>354</v>
+      </c>
+      <c r="C17" t="s">
+        <v>357</v>
+      </c>
+      <c r="D17" t="s">
+        <v>355</v>
+      </c>
       <c r="E17" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>49</v>
+      <c r="A19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -1813,12 +1858,52 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>82</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F23" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2089,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,78 +2407,78 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>315</v>
+      </c>
+      <c r="B16" t="s">
+        <v>350</v>
+      </c>
+      <c r="C16" t="s">
+        <v>347</v>
+      </c>
+      <c r="D16" t="s">
+        <v>351</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="A17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" t="s">
+        <v>354</v>
+      </c>
+      <c r="C17" t="s">
+        <v>357</v>
+      </c>
+      <c r="D17" t="s">
+        <v>355</v>
+      </c>
       <c r="E17" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>49</v>
+      <c r="A19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -2404,20 +2489,61 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" t="s">
+        <v>121</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="F21" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="4"/>
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2426,7 +2552,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2678,7 +2804,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2771,10 +2897,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2944,60 +3070,60 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>315</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>358</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>76</v>
+      <c r="A16" t="s">
+        <v>348</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>359</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>216</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
+        <v>82</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>87</v>
+      <c r="A18" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>215</v>
-      </c>
-      <c r="D18" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D19" t="s">
         <v>49</v>
@@ -3005,53 +3131,81 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>215</v>
       </c>
       <c r="D20" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>76</v>
+      <c r="A21" t="s">
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>225</v>
+        <v>82</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>94</v>
+      <c r="A23" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>224</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>95</v>
       </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3342,8 +3496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3981,7 +4135,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,7 +4243,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4262,10 +4416,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,7 +4712,9 @@
       <c r="B15" s="2">
         <v>214</v>
       </c>
-      <c r="C15"/>
+      <c r="C15" t="s">
+        <v>347</v>
+      </c>
       <c r="D15" t="s">
         <v>316</v>
       </c>
@@ -4579,82 +4735,82 @@
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="4">
-        <f>SUM(B11:B15)</f>
-        <v>1140</v>
-      </c>
-      <c r="D16"/>
+      <c r="A16" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" s="2">
+        <v>72.5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>357</v>
+      </c>
+      <c r="D16" t="s">
+        <v>360</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>361</v>
+      </c>
       <c r="F16" s="4" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="F17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="B17" s="4">
+        <f>SUM(B11:B16)</f>
+        <v>1212.5</v>
+      </c>
+      <c r="D17"/>
+      <c r="F17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="4"/>
+      <c r="F18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="4">
-        <v>250</v>
-      </c>
-      <c r="C19" t="s">
-        <v>128</v>
-      </c>
-      <c r="D19" t="s">
-        <v>305</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="4">
         <v>250</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>5</v>
@@ -4671,19 +4827,19 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B21" s="4">
         <v>250</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>5</v>
@@ -4700,59 +4856,69 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B22" s="4">
-        <f>SUM(B19:B21)</f>
-        <v>750</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+        <v>250</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>307</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F22" s="4" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23"/>
+        <v>50</v>
+      </c>
+      <c r="B23" s="4">
+        <f>SUM(B20:B22)</f>
+        <v>750</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
-        <v>17</v>
+        <v>82</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="4">
-        <f>B22</f>
-        <v>750</v>
-      </c>
-      <c r="C24" s="4"/>
+        <v>76</v>
+      </c>
       <c r="D24"/>
-      <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4" t="s">
-        <v>3</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B25" s="4">
-        <f>B16+B9</f>
-        <v>1602.1</v>
+        <f>B23</f>
+        <v>750</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25"/>
@@ -4762,46 +4928,65 @@
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="B26" s="4">
-        <f>B25+B24</f>
-        <v>2352.1</v>
+        <f>B17+B9</f>
+        <v>1674.6</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="D26"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>77</v>
+        <v>13</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="B27" s="4">
+        <f>B26+B25</f>
+        <v>2424.6</v>
+      </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>17</v>
+        <v>80</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
+      <c r="A28" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5593,7 +5778,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5808,10 +5993,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6105,98 +6290,98 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>315</v>
+      </c>
+      <c r="B16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C16" t="s">
+        <v>350</v>
+      </c>
+      <c r="D16" t="s">
+        <v>351</v>
+      </c>
+      <c r="E16" t="s">
+        <v>352</v>
+      </c>
+      <c r="F16" t="s">
+        <v>347</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="A17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C17" t="s">
+        <v>354</v>
+      </c>
+      <c r="D17" t="s">
+        <v>355</v>
+      </c>
+      <c r="E17" t="s">
+        <v>356</v>
+      </c>
+      <c r="F17" t="s">
+        <v>357</v>
+      </c>
       <c r="G17" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" t="s">
-        <v>128</v>
-      </c>
-      <c r="G18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" t="s">
-        <v>122</v>
-      </c>
-      <c r="F19" t="s">
-        <v>123</v>
-      </c>
-      <c r="G19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" t="s">
-        <v>49</v>
+      <c r="A19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C20" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
@@ -6207,94 +6392,146 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" t="s">
+        <v>123</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="H21" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="2" t="s">
-        <v>17</v>
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" t="s">
-        <v>112</v>
-      </c>
-      <c r="F23" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>5</v>
+        <v>82</v>
+      </c>
+      <c r="H23" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" t="s">
-        <v>108</v>
-      </c>
-      <c r="G24" t="s">
-        <v>5</v>
+      <c r="A24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>95</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>99</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>100</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" t="s">
         <v>101</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>102</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F27" t="s">
         <v>103</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G27" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
alfanar ic changed to 234
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -1533,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4448,8 +4448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4740,7 +4740,7 @@
         <v>358</v>
       </c>
       <c r="B15" s="2">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="C15" t="s">
         <v>335</v>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="B17" s="4">
         <f>SUM(B11:B16)</f>
-        <v>1212.5</v>
+        <v>1232.5</v>
       </c>
       <c r="D17"/>
       <c r="F17" s="4" t="s">
@@ -4967,7 +4967,7 @@
       </c>
       <c r="B26" s="4">
         <f>B17+B9</f>
-        <v>1674.6</v>
+        <v>1694.6</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26"/>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="B27" s="4">
         <f>B26+B25</f>
-        <v>2424.6</v>
+        <v>2444.6</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>

</xml_diff>

<commit_message>
renew ap2 installed capacity increased
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -1533,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4448,7 +4448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -4769,7 +4769,7 @@
         <v>359</v>
       </c>
       <c r="B16" s="2">
-        <v>72.5</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>344</v>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="B17" s="4">
         <f>SUM(B11:B16)</f>
-        <v>1232.5</v>
+        <v>1255</v>
       </c>
       <c r="D17"/>
       <c r="F17" s="4" t="s">
@@ -4967,7 +4967,7 @@
       </c>
       <c r="B26" s="4">
         <f>B17+B9</f>
-        <v>1694.6</v>
+        <v>1717.1</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26"/>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="B27" s="4">
         <f>B26+B25</f>
-        <v>2444.6</v>
+        <v>2467.1</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>

</xml_diff>

<commit_message>
zero avc bug fixed
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\Python Projects\remc_report_generator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -4272,8 +4272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4367,7 +4367,7 @@
         <v>79</v>
       </c>
       <c r="B9" s="4">
-        <v>15344</v>
+        <v>15491</v>
       </c>
       <c r="C9" t="s">
         <v>164</v>
@@ -4387,7 +4387,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="4">
-        <v>6013</v>
+        <v>6157</v>
       </c>
       <c r="C10" t="s">
         <v>159</v>
@@ -4408,7 +4408,7 @@
       </c>
       <c r="B11" s="4">
         <f>B10+B9</f>
-        <v>21357</v>
+        <v>21648</v>
       </c>
       <c r="C11" t="s">
         <v>154</v>
@@ -4448,8 +4448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4711,7 +4711,7 @@
         <v>357</v>
       </c>
       <c r="B14" s="4">
-        <v>176</v>
+        <v>176.4</v>
       </c>
       <c r="C14" t="s">
         <v>148</v>
@@ -4740,7 +4740,7 @@
         <v>358</v>
       </c>
       <c r="B15" s="2">
-        <v>234</v>
+        <v>234.6</v>
       </c>
       <c r="C15" t="s">
         <v>335</v>
@@ -4769,7 +4769,7 @@
         <v>359</v>
       </c>
       <c r="B16" s="2">
-        <v>95</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
         <v>344</v>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="B17" s="4">
         <f>SUM(B11:B16)</f>
-        <v>1255</v>
+        <v>1331</v>
       </c>
       <c r="D17"/>
       <c r="F17" s="4" t="s">
@@ -4967,7 +4967,7 @@
       </c>
       <c r="B26" s="4">
         <f>B17+B9</f>
-        <v>1717.1</v>
+        <v>1793.1</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26"/>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="B27" s="4">
         <f>B26+B25</f>
-        <v>2467.1</v>
+        <v>2543.1</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>

</xml_diff>

<commit_message>
config change for installed capacity
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\Python Projects\remc_report_generator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.60\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9491D0-D90E-43AF-B02A-185E8E738481}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -36,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">remc_graph_data!$A$1:$C$56</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1185,7 +1186,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1238,7 +1239,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1296,7 +1297,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1348,7 +1349,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1549,7 +1550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1596,7 +1597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2055,7 +2056,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -2421,7 +2422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2681,7 +2682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -3056,7 +3057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -3308,7 +3309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
@@ -3404,7 +3405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3723,7 +3724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -4001,7 +4002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -4639,7 +4640,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4747,11 +4748,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4845,7 +4846,7 @@
         <v>79</v>
       </c>
       <c r="B9" s="4">
-        <v>15491</v>
+        <v>15614</v>
       </c>
       <c r="C9" t="s">
         <v>164</v>
@@ -4865,7 +4866,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="4">
-        <v>6157</v>
+        <v>6382</v>
       </c>
       <c r="C10" t="s">
         <v>159</v>
@@ -4886,7 +4887,7 @@
       </c>
       <c r="B11" s="4">
         <f>B10+B9</f>
-        <v>21648</v>
+        <v>21996</v>
       </c>
       <c r="C11" t="s">
         <v>154</v>
@@ -4923,11 +4924,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5247,7 +5248,7 @@
         <v>359</v>
       </c>
       <c r="B16" s="2">
-        <v>192</v>
+        <v>243</v>
       </c>
       <c r="C16" t="s">
         <v>344</v>
@@ -5277,7 +5278,7 @@
       </c>
       <c r="B17" s="4">
         <f>SUM(B11:B16)</f>
-        <v>1368.4</v>
+        <v>1419.4</v>
       </c>
       <c r="D17"/>
       <c r="F17" s="4" t="s">
@@ -5445,7 +5446,7 @@
       </c>
       <c r="B26" s="4">
         <f>B17+B9</f>
-        <v>1830.5</v>
+        <v>1881.5</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26"/>
@@ -5464,7 +5465,7 @@
       </c>
       <c r="B27" s="4">
         <f>B26+B25</f>
-        <v>2580.5</v>
+        <v>2631.5</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -5503,11 +5504,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5591,7 +5592,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="4">
-        <v>2248</v>
+        <v>2492</v>
       </c>
       <c r="C6" t="s">
         <v>189</v>
@@ -5620,7 +5621,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="4">
-        <v>6265</v>
+        <v>6299</v>
       </c>
       <c r="C7" t="s">
         <v>194</v>
@@ -5650,7 +5651,7 @@
       </c>
       <c r="B8" s="4">
         <f>SUM(B6:B7)</f>
-        <v>8513</v>
+        <v>8791</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>26</v>
@@ -5674,7 +5675,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="4">
-        <v>1460</v>
+        <v>1580</v>
       </c>
       <c r="C10" t="s">
         <v>179</v>
@@ -5703,7 +5704,7 @@
         <v>47</v>
       </c>
       <c r="B11" s="4">
-        <v>5008</v>
+        <v>5010</v>
       </c>
       <c r="C11" t="s">
         <v>184</v>
@@ -5733,7 +5734,7 @@
       </c>
       <c r="B12" s="4">
         <f>B10+B11</f>
-        <v>6468</v>
+        <v>6590</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>26</v>
@@ -5755,7 +5756,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="4">
-        <v>1555</v>
+        <v>1560</v>
       </c>
       <c r="C14" t="s">
         <v>169</v>
@@ -5784,7 +5785,7 @@
         <v>52</v>
       </c>
       <c r="B15" s="4">
-        <v>2418</v>
+        <v>2424</v>
       </c>
       <c r="C15" t="s">
         <v>174</v>
@@ -5814,7 +5815,7 @@
       </c>
       <c r="B16" s="4">
         <f>B15+B14</f>
-        <v>3973</v>
+        <v>3984</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>26</v>
@@ -5837,7 +5838,7 @@
       </c>
       <c r="B18" s="4">
         <f>B7+B11+B15</f>
-        <v>13691</v>
+        <v>13733</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
@@ -5852,7 +5853,7 @@
       </c>
       <c r="B19" s="4">
         <f>B6+B10+B14</f>
-        <v>5263</v>
+        <v>5632</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -5867,7 +5868,7 @@
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
-        <v>18954</v>
+        <v>19365</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>74</v>
@@ -6138,11 +6139,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6440,7 +6441,7 @@
         <v>359</v>
       </c>
       <c r="B16" s="2">
-        <v>192</v>
+        <v>243</v>
       </c>
       <c r="C16" t="s">
         <v>347</v>
@@ -6464,7 +6465,7 @@
       </c>
       <c r="B17" s="4">
         <f>SUM(B11:B16)</f>
-        <v>1368.4</v>
+        <v>1419.4</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>76</v>
@@ -6623,7 +6624,7 @@
       </c>
       <c r="B26" s="4">
         <f>B17+B9</f>
-        <v>1830.5</v>
+        <v>1881.5</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>13</v>
@@ -6640,7 +6641,7 @@
       </c>
       <c r="B27" s="4">
         <f>B26+B25</f>
-        <v>2580.5</v>
+        <v>2631.5</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
@@ -6670,7 +6671,7 @@
         <v>23</v>
       </c>
       <c r="B29" s="4">
-        <v>2248</v>
+        <v>2492</v>
       </c>
       <c r="C29" t="s">
         <v>307</v>
@@ -6693,7 +6694,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="4">
-        <v>6265</v>
+        <v>6299</v>
       </c>
       <c r="C30" t="s">
         <v>308</v>
@@ -6717,7 +6718,7 @@
       </c>
       <c r="B31" s="4">
         <f>SUM(B29:B30)</f>
-        <v>8513</v>
+        <v>8791</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
@@ -6747,7 +6748,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="4">
-        <v>1460</v>
+        <v>1580</v>
       </c>
       <c r="C33" t="s">
         <v>301</v>
@@ -6770,7 +6771,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="4">
-        <v>5008</v>
+        <v>5010</v>
       </c>
       <c r="C34" t="s">
         <v>302</v>
@@ -6794,7 +6795,7 @@
       </c>
       <c r="B35" s="4">
         <f>B33+B34</f>
-        <v>6468</v>
+        <v>6590</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
@@ -6824,7 +6825,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="4">
-        <v>1555</v>
+        <v>1560</v>
       </c>
       <c r="C37" t="s">
         <v>304</v>
@@ -6847,7 +6848,7 @@
         <v>52</v>
       </c>
       <c r="B38" s="4">
-        <v>2418</v>
+        <v>2424</v>
       </c>
       <c r="C38" t="s">
         <v>303</v>
@@ -6871,7 +6872,7 @@
       </c>
       <c r="B39" s="4">
         <f>B38+B37</f>
-        <v>3973</v>
+        <v>3984</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>76</v>
@@ -6900,7 +6901,7 @@
       </c>
       <c r="B41" s="4">
         <f>B30+B34+B38</f>
-        <v>13691</v>
+        <v>13733</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>13</v>
@@ -6917,7 +6918,7 @@
       </c>
       <c r="B42" s="4">
         <f>B29+B33+B37</f>
-        <v>5263</v>
+        <v>5632</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>13</v>
@@ -6934,7 +6935,7 @@
       </c>
       <c r="B43" s="4">
         <f>SUM(B41:B42)</f>
-        <v>18954</v>
+        <v>19365</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>74</v>
@@ -6961,7 +6962,7 @@
         <v>79</v>
       </c>
       <c r="B45" s="4">
-        <v>15491</v>
+        <v>15614</v>
       </c>
       <c r="C45" t="s">
         <v>299</v>
@@ -6975,7 +6976,7 @@
         <v>80</v>
       </c>
       <c r="B46" s="4">
-        <v>6157</v>
+        <v>6382</v>
       </c>
       <c r="C46" t="s">
         <v>300</v>
@@ -6990,7 +6991,7 @@
       </c>
       <c r="B47" s="4">
         <f>B46+B45</f>
-        <v>21648</v>
+        <v>21996</v>
       </c>
       <c r="C47" t="s">
         <v>298</v>
@@ -7282,7 +7283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7407,7 +7408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7674,7 +7675,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7892,7 +7893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
minor changes in versions
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wrldc_remc_reports_generator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\Python Projects\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BA5D4F-7A01-43D3-B7B3-A283A683A061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="11" activeTab="17"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -36,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">remc_graph_data!$A$1:$C$56</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1185,7 +1186,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1238,7 +1239,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1549,7 +1550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1596,7 +1597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2055,7 +2056,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2421,7 +2422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2681,7 +2682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -3056,7 +3057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -3308,7 +3309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
@@ -3404,7 +3405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3723,7 +3724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -4001,11 +4002,11 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4643,7 +4644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4751,7 +4752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4927,7 +4928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -5507,7 +5508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6142,7 +6143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
@@ -7288,7 +7289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7413,7 +7414,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7680,7 +7681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7898,7 +7899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
rangdhesa solar stations added
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.60\d$\wrldc_remc_reports_generator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656AE231-8201-449C-8EF9-BA6F421F7B3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="16" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -34,10 +33,10 @@
     <sheet name="scada_graph_data" sheetId="17" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">remc_graph_data!$A$1:$C$56</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="407">
   <si>
     <t>name</t>
   </si>
@@ -1181,12 +1180,99 @@
   </si>
   <si>
     <t>AWEK1L-WIND</t>
+  </si>
+  <si>
+    <t>TPREL_RSP</t>
+  </si>
+  <si>
+    <t>TPREL_RSP-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00056861</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00056231</t>
+  </si>
+  <si>
+    <t>GIPCL_RSP</t>
+  </si>
+  <si>
+    <t>GIPCL_RSP-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00056860</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00056233</t>
+  </si>
+  <si>
+    <t>ESPL_RSP</t>
+  </si>
+  <si>
+    <t>ESPL_RSP-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00056862</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00056232</t>
+  </si>
+  <si>
+    <t>Radhaneshda Pooling</t>
+  </si>
+  <si>
+    <t>Radhaneshda</t>
+  </si>
+  <si>
+    <t>TPREL_RSP-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>TPREL_RSP-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>TPREL_RSP-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>TPREL_RSP-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>GIPCL_RSP-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>GIPCL_RSP-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>GIPCL_RSP-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>GIPCL_RSP-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>ESPL_RSP-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>ESPL_RSP-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>ESPL_RSP-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>ESPL_RSP-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>TPREL_RSP-SOLAR_SOLAR</t>
+  </si>
+  <si>
+    <t>GIPCL_RSP-SOLAR_SOLAR</t>
+  </si>
+  <si>
+    <t>ESPL_RSP-SOLAR_SOLAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1239,7 +1325,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1550,7 +1636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1597,7 +1683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2056,11 +2142,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2416,13 +2502,93 @@
         <v>43</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C25" t="s">
+        <v>379</v>
+      </c>
+      <c r="D25" t="s">
+        <v>394</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" t="s">
+        <v>397</v>
+      </c>
+      <c r="C26" t="s">
+        <v>383</v>
+      </c>
+      <c r="D26" t="s">
+        <v>398</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B27" t="s">
+        <v>401</v>
+      </c>
+      <c r="C27" t="s">
+        <v>387</v>
+      </c>
+      <c r="D27" t="s">
+        <v>402</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>390</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="E28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2682,11 +2848,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3048,7 +3214,86 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="4"/>
       <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C25" t="s">
+        <v>379</v>
+      </c>
+      <c r="D25" t="s">
+        <v>394</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" t="s">
+        <v>397</v>
+      </c>
+      <c r="C26" t="s">
+        <v>383</v>
+      </c>
+      <c r="D26" t="s">
+        <v>398</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B27" t="s">
+        <v>401</v>
+      </c>
+      <c r="C27" t="s">
+        <v>387</v>
+      </c>
+      <c r="D27" t="s">
+        <v>402</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>390</v>
+      </c>
+      <c r="E28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>391</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3057,7 +3302,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -3309,7 +3554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
@@ -3405,11 +3650,11 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3686,35 +3931,96 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>404</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>405</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>406</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>390</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>83</v>
       </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>84</v>
       </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>85</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3724,7 +4030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -4002,7 +4308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -4644,7 +4950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -4752,11 +5058,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4928,11 +5234,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5425,81 +5731,195 @@
       </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>378</v>
       </c>
       <c r="B25" s="4">
-        <f>B23</f>
-        <v>750</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25"/>
-      <c r="E25" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D25" t="s">
+        <v>380</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>381</v>
+      </c>
       <c r="F25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>391</v>
+      </c>
       <c r="H25" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" s="4">
+        <v>100</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="D26" t="s">
+        <v>384</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B27" s="4">
+        <v>200</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="D27" t="s">
+        <v>388</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>390</v>
+      </c>
+      <c r="B28" s="2">
+        <f>SUM(B25:B27)</f>
+        <v>400</v>
+      </c>
+      <c r="D28"/>
+      <c r="F28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29"/>
+      <c r="F29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="4">
+        <f>B23+B28</f>
+        <v>1150</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B31" s="4">
         <f>B17+B9</f>
         <v>2305</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4" t="s">
+      <c r="G31" s="4"/>
+      <c r="H31" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="4">
-        <f>B26+B25</f>
-        <v>3055</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
+      <c r="B32" s="4">
+        <f>B31+B30</f>
+        <v>3455</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5508,7 +5928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6143,11 +6563,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6607,187 +7027,185 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B25" s="4">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>380</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" s="4">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
+        <v>384</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B27" s="4">
+        <v>200</v>
+      </c>
+      <c r="C27" t="s">
+        <v>388</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>390</v>
+      </c>
+      <c r="B28" s="2">
+        <f>SUM(B25:B27)</f>
+        <v>400</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B30" s="4">
         <f>B23</f>
         <v>750</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4" t="s">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B31" s="4">
         <f>B17+B9</f>
         <v>2305</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="4">
-        <f>B26+B25</f>
-        <v>3055</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="4">
-        <v>3703</v>
-      </c>
-      <c r="C29" t="s">
-        <v>299</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="4">
-        <v>6471</v>
-      </c>
-      <c r="C30" t="s">
-        <v>300</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="4">
-        <f>SUM(B29:B30)</f>
-        <v>10174</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="B32" s="4">
+        <f>B31+B30</f>
+        <v>3055</v>
+      </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="G32" s="2" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="4">
-        <v>1580</v>
-      </c>
-      <c r="C33" t="s">
-        <v>293</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>366</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B34" s="4">
-        <v>5010</v>
+        <v>3703</v>
       </c>
       <c r="C34" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>367</v>
+        <v>22</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>366</v>
@@ -6795,76 +7213,76 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B35" s="4">
-        <f>B33+B34</f>
-        <v>6590</v>
-      </c>
-      <c r="C35" s="4"/>
+        <v>6471</v>
+      </c>
+      <c r="C35" t="s">
+        <v>300</v>
+      </c>
       <c r="D35" s="4" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B36" s="4">
+        <f>SUM(B34:B35)</f>
+        <v>10174</v>
+      </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="4">
-        <v>1560</v>
-      </c>
-      <c r="C37" t="s">
-        <v>296</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>366</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B38" s="4">
-        <v>2416</v>
+        <v>1580</v>
       </c>
       <c r="C38" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>367</v>
+        <v>49</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>366</v>
@@ -6872,210 +7290,290 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B39" s="4">
-        <f>B38+B37</f>
-        <v>3976</v>
+        <v>5010</v>
+      </c>
+      <c r="C39" t="s">
+        <v>294</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="B40" s="4">
+        <f>B38+B39</f>
+        <v>6590</v>
+      </c>
+      <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" s="4">
-        <f>B30+B34+B38</f>
-        <v>13897</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>13</v>
+      <c r="A41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E41" s="4"/>
-      <c r="F41" s="4" t="s">
-        <v>367</v>
-      </c>
+      <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>78</v>
+      <c r="A42" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="B42" s="4">
-        <f>B29+B33+B37</f>
-        <v>6843</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="4"/>
+        <v>1560</v>
+      </c>
+      <c r="C42" t="s">
+        <v>296</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="F42" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="G42" s="4"/>
+      <c r="G42" s="2" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>75</v>
+      <c r="A43" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B43" s="4">
-        <f>SUM(B41:B42)</f>
-        <v>20740</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
+        <v>2416</v>
+      </c>
+      <c r="C43" t="s">
+        <v>295</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>367</v>
+      </c>
       <c r="G43" s="2" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="B44" s="4">
+        <f>B43+B42</f>
+        <v>3976</v>
+      </c>
       <c r="D44" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="D45" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="4">
+        <f>B35+B39+B43</f>
+        <v>13897</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="G46" s="4"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="4">
+        <f>B34+B38+B42</f>
+        <v>6843</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="4">
+        <f>SUM(B46:B47)</f>
+        <v>20740</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="D49" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B50" s="4">
         <f>regional_profile!B9</f>
         <v>16202</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C50" t="s">
         <v>291</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="D50" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B51" s="4">
         <f>regional_profile!B10</f>
         <v>7593</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C51" t="s">
         <v>292</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="D51" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="4">
-        <f>B46+B45</f>
+      <c r="B52" s="4">
+        <f>B51+B50</f>
         <v>23795</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C52" t="s">
         <v>290</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="4"/>
-      <c r="D48" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="D53" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="D64" s="4"/>
     </row>
@@ -7141,53 +7639,58 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D80" s="4"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D82" s="4"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D83" s="4"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D84" s="4"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
@@ -7282,6 +7785,21 @@
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="4"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="4"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="4"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="4"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7289,7 +7807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7414,7 +7932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7681,7 +8199,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7899,11 +8417,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:H27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8374,71 +8892,178 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B25" t="s">
+        <v>392</v>
+      </c>
+      <c r="C25" t="s">
+        <v>393</v>
+      </c>
+      <c r="D25" t="s">
+        <v>394</v>
+      </c>
+      <c r="E25" t="s">
+        <v>395</v>
+      </c>
+      <c r="F25" t="s">
+        <v>379</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" t="s">
+        <v>396</v>
+      </c>
+      <c r="C26" t="s">
+        <v>397</v>
+      </c>
+      <c r="D26" t="s">
+        <v>398</v>
+      </c>
+      <c r="E26" t="s">
+        <v>399</v>
+      </c>
+      <c r="F26" t="s">
+        <v>383</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B27" t="s">
+        <v>400</v>
+      </c>
+      <c r="C27" t="s">
+        <v>401</v>
+      </c>
+      <c r="D27" t="s">
+        <v>402</v>
+      </c>
+      <c r="E27" t="s">
+        <v>403</v>
+      </c>
+      <c r="F27" t="s">
+        <v>387</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>390</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>83</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B30" t="s">
         <v>99</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C30" t="s">
         <v>100</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D30" t="s">
         <v>101</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E30" t="s">
         <v>102</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F30" t="s">
         <v>103</v>
       </c>
-      <c r="G25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="G30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>84</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B31" t="s">
         <v>94</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C31" t="s">
         <v>95</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D31" t="s">
         <v>96</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E31" t="s">
         <v>97</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F31" t="s">
         <v>98</v>
       </c>
-      <c r="G26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>85</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B32" t="s">
         <v>89</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C32" t="s">
         <v>90</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D32" t="s">
         <v>91</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E32" t="s">
         <v>92</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F32" t="s">
         <v>93</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G32" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor ins cap change in section 1
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wrldc_remc_reports_generator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.60\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB145CE-F6A9-4DD0-B274-918BEB311C22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="16" activeTab="15"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -36,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">remc_graph_data!$A$1:$C$56</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1272,7 +1273,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1325,7 +1326,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1636,7 +1637,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1683,7 +1684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2142,7 +2143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2588,7 +2589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2848,7 +2849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -3302,7 +3303,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -3554,7 +3555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
@@ -3650,10 +3651,10 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -4030,7 +4031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -4308,7 +4309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -4950,7 +4951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -5058,11 +5059,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5176,7 +5177,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="4">
-        <v>7593</v>
+        <v>8013</v>
       </c>
       <c r="C10" t="s">
         <v>154</v>
@@ -5197,7 +5198,7 @@
       </c>
       <c r="B11" s="4">
         <f>B10+B9</f>
-        <v>23795</v>
+        <v>24215</v>
       </c>
       <c r="C11" t="s">
         <v>149</v>
@@ -5234,11 +5235,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5928,11 +5929,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6563,7 +6564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G132"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -7500,7 +7501,7 @@
       </c>
       <c r="B51" s="4">
         <f>regional_profile!B10</f>
-        <v>7593</v>
+        <v>8013</v>
       </c>
       <c r="C51" t="s">
         <v>292</v>
@@ -7515,7 +7516,7 @@
       </c>
       <c r="B52" s="4">
         <f>B51+B50</f>
-        <v>23795</v>
+        <v>24215</v>
       </c>
       <c r="C52" t="s">
         <v>290</v>
@@ -7807,7 +7808,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7932,7 +7933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8199,7 +8200,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8417,7 +8418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
mh solar ic change
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.60\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4D3444-42B3-479E-9F5B-8DC19A50B648}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0471EE27-7632-40C3-9D45-6415F92409E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -5062,7 +5062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -5932,8 +5932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6100,7 +6100,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="4">
-        <v>1580</v>
+        <v>1752</v>
       </c>
       <c r="C10" t="s">
         <v>174</v>
@@ -6159,7 +6159,7 @@
       </c>
       <c r="B12" s="4">
         <f>B10+B11</f>
-        <v>6590</v>
+        <v>6762</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>26</v>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="B19" s="4">
         <f>B6+B10+B14</f>
-        <v>6290</v>
+        <v>6462</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -6293,7 +6293,7 @@
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
-        <v>20218</v>
+        <v>20390</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>74</v>
@@ -6568,7 +6568,7 @@
   <dimension ref="A1:G132"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7271,7 +7271,7 @@
         <v>46</v>
       </c>
       <c r="B38" s="4">
-        <v>1580</v>
+        <v>1752</v>
       </c>
       <c r="C38" t="s">
         <v>293</v>
@@ -7318,7 +7318,7 @@
       </c>
       <c r="B40" s="4">
         <f>B38+B39</f>
-        <v>6590</v>
+        <v>6762</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
@@ -7441,7 +7441,7 @@
       </c>
       <c r="B47" s="4">
         <f>B34+B38+B42</f>
-        <v>6290</v>
+        <v>6462</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>13</v>
@@ -7458,7 +7458,7 @@
       </c>
       <c r="B48" s="4">
         <f>SUM(B46:B47)</f>
-        <v>20218</v>
+        <v>20390</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
added 3 new gens
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\Python Projects\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55109005-6433-485D-8629-8FACB18C6429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5451140-BB6B-4DDF-9288-0EB89DCB9A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8970" yWindow="4665" windowWidth="21600" windowHeight="11325" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="446">
   <si>
     <t>name</t>
   </si>
@@ -1299,6 +1299,99 @@
   </si>
   <si>
     <t>Radhaneshda Pooling Actual for previous day</t>
+  </si>
+  <si>
+    <t>OEPL_Bachau</t>
+  </si>
+  <si>
+    <t>OKWPL Ostro Kutch_Bachau</t>
+  </si>
+  <si>
+    <t>AWEKFL (Ratadiya)_Bhuj</t>
+  </si>
+  <si>
+    <t>CPTTNPL (Dayapar)_Bhuj</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.000528267</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00058270</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00057721</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00058273</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00057713</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00058266</t>
+  </si>
+  <si>
+    <t>OEPL-WIND_WIND_AVC</t>
+  </si>
+  <si>
+    <t>AWEKFL-WIND_WIND_AVC</t>
+  </si>
+  <si>
+    <t>CPTTNPL-WIND_WIND_AVC</t>
+  </si>
+  <si>
+    <t>OEPL-Wind</t>
+  </si>
+  <si>
+    <t>AWEKFL-Wind</t>
+  </si>
+  <si>
+    <t>CPTTNPL-Wind</t>
+  </si>
+  <si>
+    <t>OEPL-WIND_WIND_R0</t>
+  </si>
+  <si>
+    <t>OEPL-WIND_WIND_16</t>
+  </si>
+  <si>
+    <t>OEPL-WIND_WIND_Act</t>
+  </si>
+  <si>
+    <t>OEPL-WIND_WIND_CUF</t>
+  </si>
+  <si>
+    <t>AWEKFL-WIND_WIND_R0</t>
+  </si>
+  <si>
+    <t>AWEKFL-WIND_WIND_16</t>
+  </si>
+  <si>
+    <t>AWEKFL-WIND_WIND_Act</t>
+  </si>
+  <si>
+    <t>AWEKFL-WIND_WIND_CUF</t>
+  </si>
+  <si>
+    <t>CPTTNPL-WIND_WIND_R0</t>
+  </si>
+  <si>
+    <t>CPTTNPL-WIND_WIND_16</t>
+  </si>
+  <si>
+    <t>CPTTNPL-WIND_WIND_Act</t>
+  </si>
+  <si>
+    <t>CPTTNPL-WIND_WIND_CUF</t>
+  </si>
+  <si>
+    <t>OEPL-WIND_WIND</t>
+  </si>
+  <si>
+    <t>AWEKFL-WIND_WIND</t>
+  </si>
+  <si>
+    <t>CPTTNPL-WIND_WIND</t>
   </si>
 </sst>
 </file>
@@ -2095,10 +2188,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,12 +2314,23 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="4"/>
+        <v>428</v>
+      </c>
+      <c r="B10" t="s">
+        <v>432</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="D10" t="s">
+        <v>433</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -2286,7 +2390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>355</v>
       </c>
@@ -2306,7 +2410,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>358</v>
       </c>
@@ -2326,7 +2430,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>359</v>
       </c>
@@ -2346,7 +2450,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>376</v>
       </c>
@@ -2366,7 +2470,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>356</v>
       </c>
@@ -2386,7 +2490,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>357</v>
       </c>
@@ -2406,25 +2510,51 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+      <c r="B23" t="s">
+        <v>436</v>
+      </c>
+      <c r="C23" t="s">
+        <v>426</v>
+      </c>
+      <c r="D23" t="s">
+        <v>437</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+      <c r="B24" t="s">
+        <v>440</v>
+      </c>
+      <c r="C24" t="s">
+        <v>427</v>
+      </c>
+      <c r="D24" t="s">
+        <v>441</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>70</v>
       </c>
@@ -2433,7 +2563,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>70</v>
       </c>
@@ -2442,7 +2572,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>70</v>
       </c>
@@ -2451,7 +2581,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -2462,7 +2592,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>70</v>
       </c>
@@ -2473,7 +2603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>352</v>
       </c>
@@ -2493,7 +2623,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>350</v>
       </c>
@@ -2513,7 +2643,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>351</v>
       </c>
@@ -2976,10 +3106,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2992,7 +3122,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3012,7 +3142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
@@ -3020,7 +3150,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>70</v>
       </c>
@@ -3029,7 +3159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
@@ -3038,7 +3168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>70</v>
       </c>
@@ -3047,7 +3177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>70</v>
       </c>
@@ -3056,7 +3186,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>70</v>
       </c>
@@ -3065,7 +3195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>354</v>
       </c>
@@ -3085,7 +3215,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>353</v>
       </c>
@@ -3105,16 +3235,29 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="B10" t="s">
+        <v>432</v>
+      </c>
+      <c r="C10" t="s">
+        <v>425</v>
+      </c>
+      <c r="D10" t="s">
+        <v>433</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
@@ -3123,7 +3266,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>70</v>
       </c>
@@ -3132,7 +3275,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>70</v>
       </c>
@@ -3141,7 +3284,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>70</v>
       </c>
@@ -3150,7 +3293,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -3161,7 +3304,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>70</v>
       </c>
@@ -3172,7 +3315,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>355</v>
       </c>
@@ -3192,7 +3335,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>358</v>
       </c>
@@ -3212,7 +3355,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>359</v>
       </c>
@@ -3232,7 +3375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>376</v>
       </c>
@@ -3252,7 +3395,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>356</v>
       </c>
@@ -3272,7 +3415,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>357</v>
       </c>
@@ -3292,25 +3435,51 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+      <c r="B23" t="s">
+        <v>436</v>
+      </c>
+      <c r="C23" t="s">
+        <v>426</v>
+      </c>
+      <c r="D23" t="s">
+        <v>437</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+      <c r="B24" t="s">
+        <v>440</v>
+      </c>
+      <c r="C24" t="s">
+        <v>427</v>
+      </c>
+      <c r="D24" t="s">
+        <v>441</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>70</v>
       </c>
@@ -3319,7 +3488,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>70</v>
       </c>
@@ -3328,7 +3497,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>70</v>
       </c>
@@ -3337,7 +3506,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -3348,7 +3517,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>70</v>
       </c>
@@ -3359,7 +3528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>352</v>
       </c>
@@ -3379,7 +3548,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>350</v>
       </c>
@@ -3399,7 +3568,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>360</v>
       </c>
@@ -3613,7 +3782,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3960,8 +4129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4056,12 +4225,17 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>428</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>443</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4203,22 +4377,32 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>70</v>
+      <c r="A22" s="4" t="s">
+        <v>429</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>444</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>70</v>
+      <c r="A23" s="4" t="s">
+        <v>430</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>445</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -4798,7 +4982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
@@ -5474,7 +5658,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5592,7 +5776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -5768,8 +5952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5859,7 +6043,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>343</v>
+        <v>416</v>
       </c>
       <c r="B7" s="1">
         <v>250</v>
@@ -5917,14 +6101,32 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9"/>
-      <c r="D9"/>
+        <v>415</v>
+      </c>
+      <c r="B9" s="4">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>425</v>
+      </c>
+      <c r="D9" t="s">
+        <v>419</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>420</v>
+      </c>
       <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -5975,8 +6177,8 @@
         <v>39</v>
       </c>
       <c r="B14" s="1">
-        <f>SUM(B7:B8)</f>
-        <v>480</v>
+        <f>SUM(B7:B9)</f>
+        <v>502</v>
       </c>
       <c r="D14"/>
       <c r="F14" s="1" t="s">
@@ -6057,7 +6259,7 @@
         <v>345</v>
       </c>
       <c r="B18" s="4">
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
         <v>138</v>
@@ -6170,27 +6372,61 @@
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22"/>
-      <c r="D22"/>
+        <v>417</v>
+      </c>
+      <c r="B22" s="2">
+        <v>68.3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>426</v>
+      </c>
+      <c r="D22" t="s">
+        <v>421</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>422</v>
+      </c>
       <c r="F22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23"/>
-      <c r="D23"/>
+        <v>418</v>
+      </c>
+      <c r="B23" s="2">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>427</v>
+      </c>
+      <c r="D23" t="s">
+        <v>423</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>424</v>
+      </c>
       <c r="F23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -6233,8 +6469,8 @@
         <v>40</v>
       </c>
       <c r="B27" s="4">
-        <f>SUM(B16:B21)</f>
-        <v>1825</v>
+        <f>SUM(B16:B23)</f>
+        <v>1923.3</v>
       </c>
       <c r="D27"/>
       <c r="F27" s="4" t="s">
@@ -6821,7 +7057,7 @@
       </c>
       <c r="B71" s="4">
         <f>B27+B14</f>
-        <v>2305</v>
+        <v>2425.3000000000002</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71"/>
@@ -6840,7 +7076,7 @@
       </c>
       <c r="B72" s="4">
         <f>B71+B70</f>
-        <v>3455</v>
+        <v>3575.3</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -7604,7 +7840,7 @@
   <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7754,15 +7990,26 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="4"/>
+        <v>415</v>
+      </c>
+      <c r="B9" s="4">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>419</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -7817,8 +8064,8 @@
         <v>39</v>
       </c>
       <c r="B14" s="4">
-        <f>SUM(B7:B8)</f>
-        <v>480</v>
+        <f>SUM(B7:B9)</f>
+        <v>502</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>76</v>
@@ -7893,7 +8140,7 @@
         <v>345</v>
       </c>
       <c r="B18" s="4">
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
         <v>285</v>
@@ -7982,27 +8229,49 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="2"/>
+        <v>417</v>
+      </c>
+      <c r="B22" s="2">
+        <v>68.3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>421</v>
+      </c>
       <c r="D22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>418</v>
+      </c>
+      <c r="B23" s="2">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>423</v>
+      </c>
       <c r="D23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -8045,8 +8314,8 @@
         <v>40</v>
       </c>
       <c r="B27" s="4">
-        <f>SUM(B16:B21)</f>
-        <v>1825</v>
+        <f>SUM(B16:B23)</f>
+        <v>1923.3</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>76</v>
@@ -8423,7 +8692,7 @@
       </c>
       <c r="B51" s="4">
         <f>B27+B14</f>
-        <v>2305</v>
+        <v>2425.3000000000002</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>13</v>
@@ -8440,7 +8709,7 @@
       </c>
       <c r="B52" s="4">
         <f>B51+B50</f>
-        <v>3055</v>
+        <v>3175.3</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
@@ -9719,8 +9988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9886,12 +10155,29 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>70</v>
+        <v>428</v>
+      </c>
+      <c r="B10" t="s">
+        <v>431</v>
+      </c>
+      <c r="C10" t="s">
+        <v>432</v>
+      </c>
+      <c r="D10" t="s">
+        <v>433</v>
+      </c>
+      <c r="E10" t="s">
+        <v>434</v>
+      </c>
+      <c r="F10" t="s">
+        <v>425</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -10111,21 +10397,55 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>70</v>
+        <v>429</v>
+      </c>
+      <c r="B23" t="s">
+        <v>435</v>
+      </c>
+      <c r="C23" t="s">
+        <v>436</v>
+      </c>
+      <c r="D23" t="s">
+        <v>437</v>
+      </c>
+      <c r="E23" t="s">
+        <v>438</v>
+      </c>
+      <c r="F23" t="s">
+        <v>426</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>70</v>
+        <v>430</v>
+      </c>
+      <c r="B24" t="s">
+        <v>439</v>
+      </c>
+      <c r="C24" t="s">
+        <v>440</v>
+      </c>
+      <c r="D24" t="s">
+        <v>441</v>
+      </c>
+      <c r="E24" t="s">
+        <v>442</v>
+      </c>
+      <c r="F24" t="s">
+        <v>427</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">

</xml_diff>

<commit_message>
mh solar ic changed
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\Python Projects\wrldc_remc_reports_generator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.58\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5901685-00D0-4C23-BCDE-80AC831ECE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0676FEE-9B40-429C-A3AD-335F8DD40EB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -41,13 +41,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -5776,7 +5769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -7118,7 +7111,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7284,7 +7279,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="4">
-        <v>1752</v>
+        <v>1826</v>
       </c>
       <c r="C10" t="s">
         <v>174</v>
@@ -7343,7 +7338,7 @@
       </c>
       <c r="B12" s="4">
         <f>B10+B11</f>
-        <v>6762</v>
+        <v>6836</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>26</v>
@@ -7462,7 +7457,7 @@
       </c>
       <c r="B19" s="4">
         <f>B6+B10+B14</f>
-        <v>6462</v>
+        <v>6536</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -7477,7 +7472,7 @@
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
-        <v>20390</v>
+        <v>20464</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>74</v>
@@ -7839,8 +7834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8816,7 +8811,7 @@
         <v>46</v>
       </c>
       <c r="B58" s="4">
-        <v>1752</v>
+        <v>1826</v>
       </c>
       <c r="C58" t="s">
         <v>293</v>
@@ -8863,7 +8858,7 @@
       </c>
       <c r="B60" s="4">
         <f>B58+B59</f>
-        <v>6762</v>
+        <v>6836</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
@@ -8986,7 +8981,7 @@
       </c>
       <c r="B67" s="4">
         <f>B54+B58+B62</f>
-        <v>6462</v>
+        <v>6536</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>13</v>
@@ -9003,7 +8998,7 @@
       </c>
       <c r="B68" s="4">
         <f>SUM(B66:B67)</f>
-        <v>20390</v>
+        <v>20464</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
solar ic changed for wr, mp
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.58\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0676FEE-9B40-429C-A3AD-335F8DD40EB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFCE5D7-AC17-4745-85D2-7F413E6146FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -5769,8 +5769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5884,7 +5884,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="4">
-        <v>7612</v>
+        <v>7706</v>
       </c>
       <c r="C10" t="s">
         <v>154</v>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="B11" s="4">
         <f>B10+B9</f>
-        <v>23845</v>
+        <v>23939</v>
       </c>
       <c r="C11" t="s">
         <v>149</v>
@@ -5945,7 +5945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -7111,8 +7111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7360,7 +7360,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="4">
-        <v>1560</v>
+        <v>1580</v>
       </c>
       <c r="C14" t="s">
         <v>164</v>
@@ -7419,7 +7419,7 @@
       </c>
       <c r="B16" s="4">
         <f>B15+B14</f>
-        <v>3984</v>
+        <v>4004</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>26</v>
@@ -7457,7 +7457,7 @@
       </c>
       <c r="B19" s="4">
         <f>B6+B10+B14</f>
-        <v>6536</v>
+        <v>6556</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -7472,7 +7472,7 @@
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
-        <v>20464</v>
+        <v>20484</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>74</v>
@@ -7834,8 +7834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8669,8 +8669,8 @@
         <v>362</v>
       </c>
       <c r="B50" s="4">
-        <f>B38</f>
-        <v>750</v>
+        <f>B38+B48</f>
+        <v>1150</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>13</v>
@@ -8704,7 +8704,7 @@
       </c>
       <c r="B52" s="4">
         <f>B51+B50</f>
-        <v>3175.3</v>
+        <v>3575.3</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
@@ -8888,7 +8888,7 @@
         <v>51</v>
       </c>
       <c r="B62" s="4">
-        <v>1560</v>
+        <v>1580</v>
       </c>
       <c r="C62" t="s">
         <v>296</v>
@@ -8935,7 +8935,7 @@
       </c>
       <c r="B64" s="4">
         <f>B63+B62</f>
-        <v>3984</v>
+        <v>4004</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>76</v>
@@ -8981,7 +8981,7 @@
       </c>
       <c r="B67" s="4">
         <f>B54+B58+B62</f>
-        <v>6536</v>
+        <v>6556</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>13</v>
@@ -8998,7 +8998,7 @@
       </c>
       <c r="B68" s="4">
         <f>SUM(B66:B67)</f>
-        <v>20464</v>
+        <v>20484</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>74</v>
@@ -9041,7 +9041,7 @@
       </c>
       <c r="B71" s="4">
         <f>regional_profile!B10</f>
-        <v>7612</v>
+        <v>7706</v>
       </c>
       <c r="C71" t="s">
         <v>292</v>
@@ -9056,7 +9056,7 @@
       </c>
       <c r="B72" s="4">
         <f>B71+B70</f>
-        <v>23845</v>
+        <v>23939</v>
       </c>
       <c r="C72" t="s">
         <v>290</v>

</xml_diff>

<commit_message>
mh solar updated in config excel
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.58\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFCE5D7-AC17-4745-85D2-7F413E6146FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27970D05-44D9-4E94-8D56-A253C9EFAAD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4976,7 +4976,7 @@
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5884,7 +5884,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="4">
-        <v>7706</v>
+        <v>7718</v>
       </c>
       <c r="C10" t="s">
         <v>154</v>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="B11" s="4">
         <f>B10+B9</f>
-        <v>23939</v>
+        <v>23951</v>
       </c>
       <c r="C11" t="s">
         <v>149</v>
@@ -5945,7 +5945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -7112,7 +7112,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7279,7 +7279,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="4">
-        <v>1826</v>
+        <v>1848</v>
       </c>
       <c r="C10" t="s">
         <v>174</v>
@@ -7338,7 +7338,7 @@
       </c>
       <c r="B12" s="4">
         <f>B10+B11</f>
-        <v>6836</v>
+        <v>6858</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>26</v>
@@ -7457,7 +7457,7 @@
       </c>
       <c r="B19" s="4">
         <f>B6+B10+B14</f>
-        <v>6556</v>
+        <v>6578</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -7472,7 +7472,7 @@
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
-        <v>20484</v>
+        <v>20506</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>74</v>
@@ -7834,7 +7834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
@@ -8811,7 +8811,7 @@
         <v>46</v>
       </c>
       <c r="B58" s="4">
-        <v>1826</v>
+        <v>1848</v>
       </c>
       <c r="C58" t="s">
         <v>293</v>
@@ -8858,7 +8858,7 @@
       </c>
       <c r="B60" s="4">
         <f>B58+B59</f>
-        <v>6836</v>
+        <v>6858</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
@@ -8981,7 +8981,7 @@
       </c>
       <c r="B67" s="4">
         <f>B54+B58+B62</f>
-        <v>6556</v>
+        <v>6578</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>13</v>
@@ -8998,7 +8998,7 @@
       </c>
       <c r="B68" s="4">
         <f>SUM(B66:B67)</f>
-        <v>20484</v>
+        <v>20506</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>74</v>
@@ -9041,7 +9041,7 @@
       </c>
       <c r="B71" s="4">
         <f>regional_profile!B10</f>
-        <v>7706</v>
+        <v>7718</v>
       </c>
       <c r="C71" t="s">
         <v>292</v>
@@ -9056,7 +9056,7 @@
       </c>
       <c r="B72" s="4">
         <f>B71+B70</f>
-        <v>23939</v>
+        <v>23951</v>
       </c>
       <c r="C72" t="s">
         <v>290</v>

</xml_diff>

<commit_message>
mp wind solar ic changes in config
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.58\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27970D05-44D9-4E94-8D56-A253C9EFAAD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225C4331-4CE3-43AA-8576-035813B0686D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1758,7 +1758,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5864,7 +5864,7 @@
         <v>79</v>
       </c>
       <c r="B9" s="4">
-        <v>16233</v>
+        <v>16279</v>
       </c>
       <c r="C9" t="s">
         <v>159</v>
@@ -5884,7 +5884,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="4">
-        <v>7718</v>
+        <v>7727</v>
       </c>
       <c r="C10" t="s">
         <v>154</v>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="B11" s="4">
         <f>B10+B9</f>
-        <v>23951</v>
+        <v>24006</v>
       </c>
       <c r="C11" t="s">
         <v>149</v>
@@ -5945,8 +5945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7112,7 +7112,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7360,7 +7360,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="4">
-        <v>1580</v>
+        <v>1589</v>
       </c>
       <c r="C14" t="s">
         <v>164</v>
@@ -7389,7 +7389,7 @@
         <v>52</v>
       </c>
       <c r="B15" s="4">
-        <v>2424</v>
+        <v>2470</v>
       </c>
       <c r="C15" t="s">
         <v>169</v>
@@ -7419,7 +7419,7 @@
       </c>
       <c r="B16" s="4">
         <f>B15+B14</f>
-        <v>4004</v>
+        <v>4059</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>26</v>
@@ -7442,7 +7442,7 @@
       </c>
       <c r="B18" s="4">
         <f>B7+B11+B15</f>
-        <v>13928</v>
+        <v>13974</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
@@ -7457,7 +7457,7 @@
       </c>
       <c r="B19" s="4">
         <f>B6+B10+B14</f>
-        <v>6578</v>
+        <v>6587</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -7472,7 +7472,7 @@
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
-        <v>20506</v>
+        <v>20561</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>74</v>
@@ -7834,8 +7834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8888,7 +8888,7 @@
         <v>51</v>
       </c>
       <c r="B62" s="4">
-        <v>1580</v>
+        <v>1589</v>
       </c>
       <c r="C62" t="s">
         <v>296</v>
@@ -8911,7 +8911,7 @@
         <v>52</v>
       </c>
       <c r="B63" s="4">
-        <v>2424</v>
+        <v>2470</v>
       </c>
       <c r="C63" t="s">
         <v>295</v>
@@ -8935,7 +8935,7 @@
       </c>
       <c r="B64" s="4">
         <f>B63+B62</f>
-        <v>4004</v>
+        <v>4059</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>76</v>
@@ -8964,7 +8964,7 @@
       </c>
       <c r="B66" s="4">
         <f>B55+B59+B63</f>
-        <v>13928</v>
+        <v>13974</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>13</v>
@@ -8981,7 +8981,7 @@
       </c>
       <c r="B67" s="4">
         <f>B54+B58+B62</f>
-        <v>6578</v>
+        <v>6587</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>13</v>
@@ -8998,7 +8998,7 @@
       </c>
       <c r="B68" s="4">
         <f>SUM(B66:B67)</f>
-        <v>20506</v>
+        <v>20561</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>74</v>
@@ -9026,7 +9026,7 @@
       </c>
       <c r="B70" s="4">
         <f>regional_profile!B9</f>
-        <v>16233</v>
+        <v>16279</v>
       </c>
       <c r="C70" t="s">
         <v>291</v>
@@ -9041,7 +9041,7 @@
       </c>
       <c r="B71" s="4">
         <f>regional_profile!B10</f>
-        <v>7718</v>
+        <v>7727</v>
       </c>
       <c r="C71" t="s">
         <v>292</v>
@@ -9056,7 +9056,7 @@
       </c>
       <c r="B72" s="4">
         <f>B71+B70</f>
-        <v>23951</v>
+        <v>24006</v>
       </c>
       <c r="C72" t="s">
         <v>290</v>

</xml_diff>

<commit_message>
sch point corrected for ENGIE and TRPL in config
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.58\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225C4331-4CE3-43AA-8576-035813B0686D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88083A11-2BBB-41FE-86D4-BF9D0C0294F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1804,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2842,7 +2842,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3775,7 +3775,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4975,7 +4975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -5770,7 +5770,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5945,8 +5945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6765,7 +6765,7 @@
         <v>379</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>5</v>
@@ -6823,7 +6823,7 @@
         <v>387</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>5</v>
@@ -7112,7 +7112,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7834,8 +7834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
athena added to config
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.58\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB57B351-61AD-4DBF-BA56-6FE3B101F6E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D68A0D5-FA00-43F7-B4F1-82BD15ECD3C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -376,21 +376,6 @@
     <t>OKWPL_RE-WIND_WIND_AVC</t>
   </si>
   <si>
-    <t>Acme_RUMS-SOLAR_SOLAR_R0</t>
-  </si>
-  <si>
-    <t>Acme_RUMS-SOLAR_SOLAR_16</t>
-  </si>
-  <si>
-    <t>Acme_RUMS-SOLAR_SOLAR_Act</t>
-  </si>
-  <si>
-    <t>Acme_RUMS-SOLAR_SOLAR_CUF</t>
-  </si>
-  <si>
-    <t>Acme_RUMS-SOLAR_SOLAR_AVC</t>
-  </si>
-  <si>
     <t>Arinsun_RUMS-SOLAR_SOLAR_R0</t>
   </si>
   <si>
@@ -649,9 +634,6 @@
     <t>OKWPL_RE-WIND_WIND</t>
   </si>
   <si>
-    <t>Acme_RUMS-SOLAR_SOLAR</t>
-  </si>
-  <si>
     <t>Arinsun_RUMS-SOLAR_SOLAR</t>
   </si>
   <si>
@@ -739,12 +721,6 @@
     <t>Bhuj Pooling Actual</t>
   </si>
   <si>
-    <t>Arinsun_RUMS-SOLAR_SOLAR_16,Acme_RUMS-SOLAR_SOLAR_16,Mahindra_RUMS-SOLAR_SOLAR_16</t>
-  </si>
-  <si>
-    <t>Arinsun_RUMS-SOLAR_SOLAR_Act,Acme_RUMS-SOLAR_SOLAR_Act,Mahindra_RUMS-SOLAR_SOLAR_Act</t>
-  </si>
-  <si>
     <t>Rewa Pooling Actual</t>
   </si>
   <si>
@@ -1069,9 +1045,6 @@
     <t>WREMCPRI.SCADA01.00046369</t>
   </si>
   <si>
-    <t>Acme (Ramnagar)_Rewa</t>
-  </si>
-  <si>
     <t>Mahindra (Badwar)_Rewa</t>
   </si>
   <si>
@@ -1099,9 +1072,6 @@
     <t>Renew(AP2)_Bhuj</t>
   </si>
   <si>
-    <t>Ram nagar (ACME RUMS)-Solar</t>
-  </si>
-  <si>
     <t>Badwar( Mahindra Rums)-Solar</t>
   </si>
   <si>
@@ -1385,6 +1355,36 @@
   </si>
   <si>
     <t>WREMCPRI.SCADA02.00058267</t>
+  </si>
+  <si>
+    <t>Athena (Ramnagar)_Rewa</t>
+  </si>
+  <si>
+    <t>Athena_RUMS-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>Athena_RUMS-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>Athena_RUMS-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>Athena_RUMS-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>Athena_RUMS-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>Ram nagar (ATHENA RUMS)-Solar</t>
+  </si>
+  <si>
+    <t>Athena_RUMS-SOLAR_SOLAR</t>
+  </si>
+  <si>
+    <t>Arinsun_RUMS-SOLAR_SOLAR_16,Athena_RUMS-SOLAR_SOLAR_16,Mahindra_RUMS-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>Arinsun_RUMS-SOLAR_SOLAR_Act,Athena_RUMS-SOLAR_SOLAR_Act,Mahindra_RUMS-SOLAR_SOLAR_Act</t>
   </si>
 </sst>
 </file>
@@ -1765,34 +1765,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B1" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B3" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B4" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -1851,7 +1851,7 @@
         <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1891,19 +1891,19 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -1923,19 +1923,19 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -1974,19 +1974,19 @@
         <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E10" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F10" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -2006,19 +2006,19 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D11" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E11" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F11" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
@@ -2057,19 +2057,19 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E14" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F14" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
@@ -2089,19 +2089,19 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E15" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
@@ -2168,7 +2168,7 @@
         <v>75</v>
       </c>
       <c r="G20" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="J20" t="s">
         <v>71</v>
@@ -2184,7 +2184,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B8" t="s">
         <v>105</v>
@@ -2287,16 +2287,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>5</v>
@@ -2307,16 +2307,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B10" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="D10" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>5</v>
@@ -2385,16 +2385,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>5</v>
@@ -2405,16 +2405,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>5</v>
@@ -2425,16 +2425,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>5</v>
@@ -2445,16 +2445,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B20" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="C20" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D20" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>5</v>
@@ -2465,16 +2465,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B21" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C21" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D21" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>5</v>
@@ -2485,16 +2485,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B22" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C22" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D22" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>5</v>
@@ -2505,16 +2505,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="B23" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="C23" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="D23" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>5</v>
@@ -2527,16 +2527,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B24" t="s">
         <v>429</v>
       </c>
-      <c r="B24" t="s">
-        <v>439</v>
-      </c>
       <c r="C24" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="D24" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>5</v>
@@ -2598,16 +2598,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
@@ -2618,16 +2618,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>350</v>
+        <v>442</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>439</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>437</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>440</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
@@ -2638,16 +2638,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -2717,62 +2717,62 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B40" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="C40" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="D40" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="E40" t="s">
         <v>5</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B41" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="C41" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="D41" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="E41" t="s">
         <v>5</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B42" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C42" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D42" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="E42" t="s">
         <v>5</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2822,14 +2822,14 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="B48" s="2"/>
       <c r="E48" t="s">
         <v>76</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -2928,13 +2928,13 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -2948,13 +2948,13 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -2987,13 +2987,13 @@
         <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -3007,13 +3007,13 @@
         <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -3046,13 +3046,13 @@
         <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -3066,13 +3066,13 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -3102,7 +3102,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B8" t="s">
         <v>105</v>
@@ -3210,16 +3210,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>5</v>
@@ -3230,16 +3230,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B10" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="C10" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="D10" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>5</v>
@@ -3310,16 +3310,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>5</v>
@@ -3330,16 +3330,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>5</v>
@@ -3350,16 +3350,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>5</v>
@@ -3370,16 +3370,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B20" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="C20" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D20" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>5</v>
@@ -3390,16 +3390,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B21" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C21" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D21" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>5</v>
@@ -3410,16 +3410,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B22" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C22" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D22" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>5</v>
@@ -3430,16 +3430,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="B23" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="C23" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="D23" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>5</v>
@@ -3452,16 +3452,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B24" t="s">
         <v>429</v>
       </c>
-      <c r="B24" t="s">
-        <v>439</v>
-      </c>
       <c r="C24" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="D24" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>5</v>
@@ -3523,16 +3523,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
@@ -3543,16 +3543,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>350</v>
+        <v>442</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>439</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>437</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>440</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
@@ -3563,16 +3563,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -3650,62 +3650,62 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B40" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="C40" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="D40" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="E40" t="s">
         <v>5</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B41" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="C41" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="D41" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="E41" t="s">
         <v>5</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B42" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C42" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D42" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="E42" t="s">
         <v>5</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3755,13 +3755,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="E48" t="s">
         <v>76</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -3853,13 +3853,13 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -3873,13 +3873,13 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -3912,13 +3912,13 @@
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -3932,13 +3932,13 @@
         <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D12" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -3971,13 +3971,13 @@
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -3991,13 +3991,13 @@
         <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -4045,7 +4045,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4082,35 +4082,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4123,7 +4123,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4142,7 +4142,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -4190,13 +4190,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>41</v>
@@ -4204,13 +4204,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>41</v>
@@ -4218,13 +4218,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>41</v>
@@ -4287,13 +4287,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>42</v>
@@ -4301,13 +4301,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>42</v>
@@ -4315,13 +4315,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>42</v>
@@ -4329,13 +4329,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>42</v>
@@ -4343,13 +4343,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>42</v>
@@ -4357,13 +4357,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>42</v>
@@ -4371,13 +4371,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>42</v>
@@ -4385,13 +4385,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>42</v>
@@ -4445,13 +4445,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D29" t="s">
         <v>43</v>
@@ -4459,13 +4459,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>350</v>
+        <v>442</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>200</v>
+        <v>443</v>
       </c>
       <c r="D30" t="s">
         <v>43</v>
@@ -4473,13 +4473,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D31" t="s">
         <v>43</v>
@@ -4551,44 +4551,44 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4638,13 +4638,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="B47" t="s">
         <v>76</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4663,7 +4663,7 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -4674,7 +4674,7 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4685,7 +4685,7 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4719,7 +4719,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
@@ -4763,7 +4763,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>22</v>
@@ -4783,7 +4783,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>22</v>
@@ -4822,7 +4822,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>49</v>
@@ -4842,7 +4842,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>49</v>
@@ -4882,7 +4882,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>50</v>
@@ -4902,7 +4902,7 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>50</v>
@@ -4975,9 +4975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4999,645 +4997,645 @@
         <v>38</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C16" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C17" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C21" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C22" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C23" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="C24" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C25" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C26" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>230</v>
+        <v>444</v>
       </c>
       <c r="C27" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>231</v>
+        <v>445</v>
       </c>
       <c r="C28" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>231</v>
+        <v>445</v>
       </c>
       <c r="C29" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C30" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C31" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C32" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C33" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C34" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C35" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C36" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C37" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C38" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C39" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C40" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C41" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C42" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C44" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C45" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" t="s">
         <v>240</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C46" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C48" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C49" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C50" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C51" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C52" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C53" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C54" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C55" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C56" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="C57" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C58" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C59" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -5674,10 +5672,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -5685,7 +5683,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -5696,10 +5694,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B4" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -5707,7 +5705,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
@@ -5718,10 +5716,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -5729,7 +5727,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -5740,10 +5738,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B8" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -5751,10 +5749,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="B9" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -5867,10 +5865,10 @@
         <v>16279</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D9" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>55</v>
@@ -5887,10 +5885,10 @@
         <v>7727</v>
       </c>
       <c r="C10" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>56</v>
@@ -5908,10 +5906,10 @@
         <v>24006</v>
       </c>
       <c r="C11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D11" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>57</v>
@@ -5945,8 +5943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6036,7 +6034,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="B7" s="1">
         <v>250</v>
@@ -6045,7 +6043,7 @@
         <v>108</v>
       </c>
       <c r="D7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>63</v>
@@ -6065,16 +6063,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B8" s="1">
         <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>62</v>
@@ -6094,19 +6092,19 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="B9" s="4">
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="D9" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>5</v>
@@ -6191,16 +6189,16 @@
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B16" s="4">
         <v>250</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D16" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>61</v>
@@ -6220,16 +6218,16 @@
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B17" s="4">
         <v>300</v>
       </c>
       <c r="C17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>60</v>
@@ -6249,16 +6247,16 @@
     </row>
     <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="B18" s="4">
         <v>210</v>
       </c>
       <c r="C18" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>59</v>
@@ -6278,16 +6276,16 @@
     </row>
     <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B19" s="4">
         <v>425</v>
       </c>
       <c r="C19" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D19" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>58</v>
@@ -6307,19 +6305,19 @@
     </row>
     <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B20" s="2">
         <v>300</v>
       </c>
       <c r="C20" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D20" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>5</v>
@@ -6336,19 +6334,19 @@
     </row>
     <row r="21" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B21" s="2">
         <v>300</v>
       </c>
       <c r="C21" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D21" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>5</v>
@@ -6365,19 +6363,19 @@
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="B22" s="2">
         <v>68.3</v>
       </c>
       <c r="C22" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="D22" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>5</v>
@@ -6394,19 +6392,19 @@
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="B23" s="2">
         <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="D23" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>5</v>
@@ -6582,16 +6580,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B40" s="4">
         <v>250</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D40" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>18</v>
@@ -6611,16 +6609,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>340</v>
+        <v>436</v>
       </c>
       <c r="B41" s="4">
         <v>250</v>
       </c>
       <c r="C41" t="s">
-        <v>113</v>
+        <v>437</v>
       </c>
       <c r="D41" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>19</v>
@@ -6640,16 +6638,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B42" s="4">
         <v>250</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D42" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>20</v>
@@ -6753,25 +6751,25 @@
     </row>
     <row r="50" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B50" s="4">
         <v>100</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D50" t="s">
+        <v>369</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="D50" t="s">
-        <v>379</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>388</v>
-      </c>
       <c r="F50" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>3</v>
@@ -6782,25 +6780,25 @@
     </row>
     <row r="51" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B51" s="4">
         <v>100</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="D51" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>3</v>
@@ -6811,25 +6809,25 @@
     </row>
     <row r="52" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B52" s="4">
         <v>200</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D52" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="E52" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" s="4" t="s">
         <v>380</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>390</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>3</v>
@@ -6890,7 +6888,7 @@
     </row>
     <row r="58" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="B58" s="2">
         <f>SUM(B50:B52)</f>
@@ -6901,7 +6899,7 @@
         <v>76</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="H58" s="2"/>
     </row>
@@ -7199,10 +7197,10 @@
         <v>3150</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>28</v>
@@ -7228,10 +7226,10 @@
         <v>6494</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>27</v>
@@ -7282,10 +7280,10 @@
         <v>1848</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>64</v>
@@ -7311,10 +7309,10 @@
         <v>5010</v>
       </c>
       <c r="C11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D11" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>65</v>
@@ -7363,10 +7361,10 @@
         <v>1589</v>
       </c>
       <c r="C14" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D14" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>66</v>
@@ -7392,10 +7390,10 @@
         <v>2470</v>
       </c>
       <c r="C15" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D15" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>67</v>
@@ -7835,7 +7833,7 @@
   <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7939,13 +7937,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B7" s="4">
         <v>250</v>
       </c>
       <c r="C7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
@@ -7954,21 +7952,21 @@
         <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B8" s="4">
         <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>5</v>
@@ -7977,21 +7975,21 @@
         <v>41</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="B9" s="4">
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>5</v>
@@ -8000,10 +7998,10 @@
         <v>41</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -8086,13 +8084,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B16" s="4">
         <v>250</v>
       </c>
       <c r="C16" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>5</v>
@@ -8101,21 +8099,21 @@
         <v>42</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B17" s="4">
         <v>300</v>
       </c>
       <c r="C17" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>5</v>
@@ -8124,21 +8122,21 @@
         <v>42</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="B18" s="4">
         <v>210</v>
       </c>
       <c r="C18" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>5</v>
@@ -8147,21 +8145,21 @@
         <v>42</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B19" s="4">
         <v>425</v>
       </c>
       <c r="C19" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>5</v>
@@ -8170,21 +8168,21 @@
         <v>42</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B20" s="2">
         <v>300</v>
       </c>
       <c r="C20" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>5</v>
@@ -8193,21 +8191,21 @@
         <v>42</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B21" s="2">
         <v>300</v>
       </c>
       <c r="C21" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>5</v>
@@ -8216,21 +8214,21 @@
         <v>42</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="B22" s="2">
         <v>68.3</v>
       </c>
       <c r="C22" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>5</v>
@@ -8239,21 +8237,21 @@
         <v>42</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="B23" s="2">
         <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>5</v>
@@ -8262,10 +8260,10 @@
         <v>42</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -8349,13 +8347,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B30" s="4">
         <v>250</v>
       </c>
       <c r="C30" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>5</v>
@@ -8364,21 +8362,21 @@
         <v>43</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>340</v>
+        <v>436</v>
       </c>
       <c r="B31" s="4">
         <v>250</v>
       </c>
       <c r="C31" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>5</v>
@@ -8387,21 +8385,21 @@
         <v>43</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B32" s="4">
         <v>250</v>
       </c>
       <c r="C32" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>5</v>
@@ -8410,10 +8408,10 @@
         <v>43</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -8508,71 +8506,71 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B40" s="4">
         <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B41" s="4">
         <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B42" s="4">
         <v>200</v>
       </c>
       <c r="C42" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -8637,7 +8635,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="B48" s="2">
         <f>SUM(B40:B42)</f>
@@ -8647,7 +8645,7 @@
         <v>76</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="4"/>
@@ -8666,7 +8664,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B50" s="4">
         <f>B38+B48</f>
@@ -8677,13 +8675,13 @@
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B51" s="4">
         <f>B27+B14</f>
@@ -8694,7 +8692,7 @@
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G51" s="4"/>
     </row>
@@ -8713,7 +8711,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -8737,7 +8735,7 @@
         <v>3150</v>
       </c>
       <c r="C54" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>5</v>
@@ -8746,10 +8744,10 @@
         <v>22</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -8760,7 +8758,7 @@
         <v>6494</v>
       </c>
       <c r="C55" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>5</v>
@@ -8769,10 +8767,10 @@
         <v>22</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -8814,7 +8812,7 @@
         <v>1848</v>
       </c>
       <c r="C58" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>5</v>
@@ -8823,10 +8821,10 @@
         <v>49</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -8837,7 +8835,7 @@
         <v>5010</v>
       </c>
       <c r="C59" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>5</v>
@@ -8846,10 +8844,10 @@
         <v>49</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -8891,7 +8889,7 @@
         <v>1589</v>
       </c>
       <c r="C62" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>5</v>
@@ -8900,10 +8898,10 @@
         <v>50</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -8914,7 +8912,7 @@
         <v>2470</v>
       </c>
       <c r="C63" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>5</v>
@@ -8923,10 +8921,10 @@
         <v>50</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -8971,7 +8969,7 @@
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="G66" s="4"/>
     </row>
@@ -8988,7 +8986,7 @@
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="2" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="G67" s="4"/>
     </row>
@@ -9006,7 +9004,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -9029,7 +9027,7 @@
         <v>16279</v>
       </c>
       <c r="C70" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>5</v>
@@ -9044,7 +9042,7 @@
         <v>7727</v>
       </c>
       <c r="C71" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>5</v>
@@ -9059,7 +9057,7 @@
         <v>24006</v>
       </c>
       <c r="C72" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>5</v>
@@ -9453,10 +9451,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>5</v>
@@ -9641,16 +9639,16 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D11" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>5</v>
@@ -9661,16 +9659,16 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D12" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>5</v>
@@ -9678,19 +9676,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" t="s">
         <v>144</v>
-      </c>
-      <c r="B13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" t="s">
-        <v>147</v>
-      </c>
-      <c r="D13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E13" t="s">
-        <v>149</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>5</v>
@@ -9698,7 +9696,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B14" t="s">
         <v>94</v>
@@ -9718,7 +9716,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B15" t="s">
         <v>99</v>
@@ -9738,7 +9736,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B16" t="s">
         <v>89</v>
@@ -9859,16 +9857,16 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E7" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>5</v>
@@ -9879,16 +9877,16 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>5</v>
@@ -9896,19 +9894,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" t="s">
         <v>144</v>
-      </c>
-      <c r="B9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E9" t="s">
-        <v>149</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>5</v>
@@ -9916,7 +9914,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B10" t="s">
         <v>95</v>
@@ -9936,7 +9934,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
         <v>100</v>
@@ -9956,7 +9954,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s">
         <v>90</v>
@@ -9984,7 +9982,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10098,7 +10096,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B8" t="s">
         <v>104</v>
@@ -10124,22 +10122,22 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>5</v>
@@ -10150,22 +10148,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B10" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="C10" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="D10" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="E10" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="F10" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>5</v>
@@ -10236,22 +10234,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>5</v>
@@ -10262,22 +10260,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F18" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>5</v>
@@ -10288,22 +10286,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E19" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F19" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>5</v>
@@ -10314,22 +10312,22 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B20" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="C20" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="D20" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="E20" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="F20" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>5</v>
@@ -10340,22 +10338,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B21" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C21" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="D21" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="E21" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="F21" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>5</v>
@@ -10366,22 +10364,22 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B22" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C22" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="D22" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E22" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="F22" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>5</v>
@@ -10392,22 +10390,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="B23" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="C23" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="D23" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="E23" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="F23" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>5</v>
@@ -10418,22 +10416,22 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B24" t="s">
+        <v>428</v>
+      </c>
+      <c r="C24" t="s">
         <v>429</v>
       </c>
-      <c r="B24" t="s">
-        <v>438</v>
-      </c>
-      <c r="C24" t="s">
-        <v>439</v>
-      </c>
       <c r="D24" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="E24" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="F24" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>5</v>
@@ -10495,22 +10493,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D30" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E30" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F30" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
@@ -10521,22 +10519,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>350</v>
+        <v>442</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>438</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>439</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>440</v>
       </c>
       <c r="E31" t="s">
-        <v>112</v>
+        <v>441</v>
       </c>
       <c r="F31" t="s">
-        <v>113</v>
+        <v>437</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
@@ -10547,22 +10545,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E32" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F32" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
@@ -10637,80 +10635,80 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B40" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="C40" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="D40" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="E40" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="F40" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B41" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="C41" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D41" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="E41" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="F41" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B42" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="C42" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="D42" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="E42" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="F42" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -10760,7 +10758,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="4"/>
@@ -10771,7 +10769,7 @@
         <v>76</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mp installed capacity changes
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.58\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAB4B3C-E140-48A4-8175-A7C4F91D1BF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586FA3D5-847C-4A5C-966B-CFAA39FE1C75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -1757,7 +1757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -5767,7 +5767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -5862,7 +5862,7 @@
         <v>79</v>
       </c>
       <c r="B9" s="4">
-        <v>16279</v>
+        <v>16333</v>
       </c>
       <c r="C9" t="s">
         <v>154</v>
@@ -5903,7 +5903,7 @@
       </c>
       <c r="B11" s="4">
         <f>B10+B9</f>
-        <v>24282</v>
+        <v>24336</v>
       </c>
       <c r="C11" t="s">
         <v>144</v>
@@ -7110,7 +7110,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7387,7 +7387,7 @@
         <v>52</v>
       </c>
       <c r="B15" s="4">
-        <v>2470</v>
+        <v>2524</v>
       </c>
       <c r="C15" t="s">
         <v>164</v>
@@ -7417,7 +7417,7 @@
       </c>
       <c r="B16" s="4">
         <f>B15+B14</f>
-        <v>4059</v>
+        <v>4113</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>26</v>
@@ -7440,7 +7440,7 @@
       </c>
       <c r="B18" s="4">
         <f>B7+B11+B15</f>
-        <v>13974</v>
+        <v>14028</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
@@ -7470,7 +7470,7 @@
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
-        <v>20837</v>
+        <v>20891</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>74</v>
@@ -7833,7 +7833,7 @@
   <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8909,7 +8909,7 @@
         <v>52</v>
       </c>
       <c r="B63" s="4">
-        <v>2470</v>
+        <v>2524</v>
       </c>
       <c r="C63" t="s">
         <v>287</v>
@@ -8933,7 +8933,7 @@
       </c>
       <c r="B64" s="4">
         <f>B63+B62</f>
-        <v>4059</v>
+        <v>4113</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>76</v>
@@ -8962,7 +8962,7 @@
       </c>
       <c r="B66" s="4">
         <f>B55+B59+B63</f>
-        <v>13974</v>
+        <v>14028</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>13</v>
@@ -8996,7 +8996,7 @@
       </c>
       <c r="B68" s="4">
         <f>SUM(B66:B67)</f>
-        <v>20837</v>
+        <v>20891</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>74</v>
@@ -9024,7 +9024,7 @@
       </c>
       <c r="B70" s="4">
         <f>regional_profile!B9</f>
-        <v>16279</v>
+        <v>16333</v>
       </c>
       <c r="C70" t="s">
         <v>283</v>
@@ -9054,7 +9054,7 @@
       </c>
       <c r="B72" s="4">
         <f>B71+B70</f>
-        <v>24282</v>
+        <v>24336</v>
       </c>
       <c r="C72" t="s">
         <v>282</v>

</xml_diff>

<commit_message>
GSECL and ASIPL added to reports
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.58\d$\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586FA3D5-847C-4A5C-966B-CFAA39FE1C75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F28724-3CEF-4984-89F4-06EFB5DD280C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="465">
   <si>
     <t>name</t>
   </si>
@@ -1385,6 +1385,63 @@
   </si>
   <si>
     <t>Arinsun_RUMS-SOLAR_SOLAR_Act,Athena_RUMS-SOLAR_SOLAR_Act,Mahindra_RUMS-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>ASIPL (Baranda)_Bhuj</t>
+  </si>
+  <si>
+    <t>ASIPL_BARANDA-WIND_WIND_AVC</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00058915</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00058926</t>
+  </si>
+  <si>
+    <t>GSECL_RSP</t>
+  </si>
+  <si>
+    <t>GSECL_RSP-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00058920</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00058923</t>
+  </si>
+  <si>
+    <t>ASIPL (Baranda)-WIND</t>
+  </si>
+  <si>
+    <t>ASIPL_BARANDA-WIND_WIND_R0</t>
+  </si>
+  <si>
+    <t>ASIPL_BARANDA-WIND_WIND_16</t>
+  </si>
+  <si>
+    <t>ASIPL_BARANDA-WIND_WIND_Act</t>
+  </si>
+  <si>
+    <t>ASIPL_BARANDA-WIND_WIND_CUF</t>
+  </si>
+  <si>
+    <t>GSECL_RSP-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>GSECL_RSP-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>GSECL_RSP-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>GSECL_RSP-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>ASIPL_BARANDA-WIND_WIND</t>
+  </si>
+  <si>
+    <t>GSECL_RSP-SOLAR_SOLAR</t>
   </si>
 </sst>
 </file>
@@ -1757,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2549,12 +2606,23 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="4"/>
+        <v>454</v>
+      </c>
+      <c r="B25" t="s">
+        <v>456</v>
+      </c>
+      <c r="C25" t="s">
+        <v>447</v>
+      </c>
+      <c r="D25" t="s">
+        <v>457</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -2777,12 +2845,23 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" s="4"/>
+        <v>450</v>
+      </c>
+      <c r="B43" t="s">
+        <v>460</v>
+      </c>
+      <c r="C43" t="s">
+        <v>451</v>
+      </c>
+      <c r="D43" t="s">
+        <v>461</v>
+      </c>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
@@ -3101,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3474,12 +3553,23 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="4"/>
+        <v>454</v>
+      </c>
+      <c r="B25" t="s">
+        <v>456</v>
+      </c>
+      <c r="C25" t="s">
+        <v>447</v>
+      </c>
+      <c r="D25" t="s">
+        <v>457</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -3710,12 +3800,23 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>70</v>
+        <v>450</v>
+      </c>
+      <c r="B43" t="s">
+        <v>460</v>
+      </c>
+      <c r="C43" t="s">
+        <v>451</v>
+      </c>
+      <c r="D43" t="s">
+        <v>461</v>
       </c>
       <c r="E43" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
@@ -4123,7 +4224,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4399,12 +4500,17 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>454</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>463</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -4593,12 +4699,17 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>450</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>464</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -5943,8 +6054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6421,15 +6532,32 @@
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24"/>
-      <c r="D24"/>
+        <v>446</v>
+      </c>
+      <c r="B24" s="2">
+        <v>113.4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>447</v>
+      </c>
+      <c r="D24" t="s">
+        <v>448</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>449</v>
+      </c>
       <c r="F24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -6460,8 +6588,8 @@
         <v>40</v>
       </c>
       <c r="B27" s="4">
-        <f>SUM(B16:B23)</f>
-        <v>1923.3</v>
+        <f>SUM(B16:B24)</f>
+        <v>2036.7</v>
       </c>
       <c r="D27"/>
       <c r="F27" s="4" t="s">
@@ -6838,13 +6966,32 @@
     </row>
     <row r="53" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D53"/>
+        <v>450</v>
+      </c>
+      <c r="B53" s="2">
+        <v>62.5</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D53" t="s">
+        <v>452</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>453</v>
+      </c>
       <c r="F53" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I53" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="54" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -6891,8 +7038,8 @@
         <v>379</v>
       </c>
       <c r="B58" s="2">
-        <f>SUM(B50:B52)</f>
-        <v>400</v>
+        <f>SUM(B50:B53)</f>
+        <v>462.5</v>
       </c>
       <c r="D58"/>
       <c r="F58" s="4" t="s">
@@ -7029,7 +7176,7 @@
       </c>
       <c r="B70" s="4">
         <f>B48+B58</f>
-        <v>1150</v>
+        <v>1212.5</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70"/>
@@ -7048,7 +7195,7 @@
       </c>
       <c r="B71" s="4">
         <f>B27+B14</f>
-        <v>2425.3000000000002</v>
+        <v>2538.6999999999998</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71"/>
@@ -7067,7 +7214,7 @@
       </c>
       <c r="B72" s="4">
         <f>B71+B70</f>
-        <v>3575.3</v>
+        <v>3751.2</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -7110,7 +7257,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7194,7 +7341,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="4">
-        <v>3150</v>
+        <v>4748</v>
       </c>
       <c r="C6" t="s">
         <v>179</v>
@@ -7253,7 +7400,7 @@
       </c>
       <c r="B8" s="4">
         <f>SUM(B6:B7)</f>
-        <v>9644</v>
+        <v>11242</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>26</v>
@@ -7455,7 +7602,7 @@
       </c>
       <c r="B19" s="4">
         <f>B6+B10+B14</f>
-        <v>6863</v>
+        <v>8461</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -7470,7 +7617,7 @@
       </c>
       <c r="B20" s="4">
         <f>SUM(B18:B19)</f>
-        <v>20891</v>
+        <v>22489</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>74</v>
@@ -7832,8 +7979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8268,15 +8415,26 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="2"/>
+        <v>446</v>
+      </c>
+      <c r="B24" s="2">
+        <v>113.4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>448</v>
+      </c>
       <c r="D24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -8307,8 +8465,8 @@
         <v>40</v>
       </c>
       <c r="B27" s="4">
-        <f>SUM(B16:B23)</f>
-        <v>1923.3</v>
+        <f>SUM(B16:B26)</f>
+        <v>2036.7</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>76</v>
@@ -8575,15 +8733,26 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" s="4"/>
+        <v>450</v>
+      </c>
+      <c r="B43" s="4">
+        <v>62.5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>452</v>
+      </c>
       <c r="D43" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
@@ -8638,8 +8807,8 @@
         <v>379</v>
       </c>
       <c r="B48" s="2">
-        <f>SUM(B40:B42)</f>
-        <v>400</v>
+        <f>SUM(B40:B47)</f>
+        <v>462.5</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>76</v>
@@ -8668,7 +8837,7 @@
       </c>
       <c r="B50" s="4">
         <f>B38+B48</f>
-        <v>1150</v>
+        <v>1212.5</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>13</v>
@@ -8685,7 +8854,7 @@
       </c>
       <c r="B51" s="4">
         <f>B27+B14</f>
-        <v>2425.3000000000002</v>
+        <v>2538.6999999999998</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>13</v>
@@ -8702,7 +8871,7 @@
       </c>
       <c r="B52" s="4">
         <f>B51+B50</f>
-        <v>3575.3</v>
+        <v>3751.2</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
@@ -8732,7 +8901,7 @@
         <v>23</v>
       </c>
       <c r="B54" s="4">
-        <v>3150</v>
+        <v>4748</v>
       </c>
       <c r="C54" t="s">
         <v>291</v>
@@ -8779,7 +8948,7 @@
       </c>
       <c r="B56" s="4">
         <f>SUM(B54:B55)</f>
-        <v>9644</v>
+        <v>11242</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
@@ -8979,7 +9148,7 @@
       </c>
       <c r="B67" s="4">
         <f>B54+B58+B62</f>
-        <v>6863</v>
+        <v>8461</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>13</v>
@@ -8996,7 +9165,7 @@
       </c>
       <c r="B68" s="4">
         <f>SUM(B66:B67)</f>
-        <v>20891</v>
+        <v>22489</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>74</v>
@@ -9981,8 +10150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10442,12 +10611,29 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>70</v>
+        <v>454</v>
+      </c>
+      <c r="B25" t="s">
+        <v>455</v>
+      </c>
+      <c r="C25" t="s">
+        <v>456</v>
+      </c>
+      <c r="D25" t="s">
+        <v>457</v>
+      </c>
+      <c r="E25" t="s">
+        <v>458</v>
+      </c>
+      <c r="F25" t="s">
+        <v>447</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -10713,12 +10899,29 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="4"/>
+        <v>450</v>
+      </c>
+      <c r="B43" t="s">
+        <v>459</v>
+      </c>
+      <c r="C43" t="s">
+        <v>460</v>
+      </c>
+      <c r="D43" t="s">
+        <v>461</v>
+      </c>
+      <c r="E43" t="s">
+        <v>462</v>
+      </c>
+      <c r="F43" t="s">
+        <v>451</v>
+      </c>
+      <c r="G43" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">

</xml_diff>

<commit_message>
max avc compute with scada and fca combination
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\D Drive\POSOCO\IT\Python Projects\wrldc_remc_reports_generator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28410" windowHeight="11250" firstSheet="12" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3243" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3269" uniqueCount="653">
   <si>
     <t>name</t>
   </si>
@@ -1824,9 +1824,6 @@
     <t>Sitac Kabini Renewable Private Ltd.(Chugger)_Bhuj_2</t>
   </si>
   <si>
-    <t>Alfanar Netra Vayu (Netra_Vayu)_Bhuj_2</t>
-  </si>
-  <si>
     <t>Apraava Energy Private Limited (AEPL) (Khakharda)_Jamkhambaliya</t>
   </si>
   <si>
@@ -1972,6 +1969,42 @@
   </si>
   <si>
     <t>Khavda PSS3 Pooling</t>
+  </si>
+  <si>
+    <t>SJVN Green Energy Limited</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00081454</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00081290</t>
+  </si>
+  <si>
+    <t>SGEL_RSP_S-SOLAR_SOLAR_CUF_AVC</t>
+  </si>
+  <si>
+    <t>Alfanar Netra Vayu</t>
+  </si>
+  <si>
+    <t>SGEL_RSP_S-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>SGEL_RSP_S-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>SGEL_RSP_S-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>SGEL_RSP_S-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>SGEL_RSP_S-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>SGEL_RSP_S-SOLAR_SOLAR</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00081296</t>
   </si>
 </sst>
 </file>
@@ -2821,8 +2854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:D60"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3207,12 +3240,23 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="4"/>
+        <v>645</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -3285,16 +3329,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>5</v>
@@ -3304,23 +3348,11 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>527</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>479</v>
+      <c r="A33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3385,16 +3417,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>600</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>598</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>601</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>5</v>
@@ -3696,16 +3728,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B60" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>607</v>
+      </c>
+      <c r="D60" s="10" t="s">
         <v>610</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>608</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>611</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>5</v>
@@ -3715,13 +3747,24 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>70</v>
+      <c r="A61" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>647</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>648</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F61" s="4"/>
+      <c r="F61" s="4" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
@@ -4223,8 +4266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4616,12 +4659,23 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="4"/>
+        <v>645</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -4696,16 +4750,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>5</v>
@@ -4715,23 +4769,11 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>479</v>
+      <c r="A33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4795,16 +4837,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>600</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>598</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>601</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>5</v>
@@ -5117,16 +5159,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B60" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>607</v>
+      </c>
+      <c r="D60" s="10" t="s">
         <v>610</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>608</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>611</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>5</v>
@@ -5136,13 +5178,24 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E61" t="s">
-        <v>17</v>
-      </c>
-      <c r="F61" s="4"/>
+      <c r="A61" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>647</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>648</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
@@ -5641,7 +5694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -5737,8 +5790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6027,13 +6080,18 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>70</v>
+      <c r="A25" s="2" t="s">
+        <v>526</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -6093,31 +6151,27 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>566</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>479</v>
-      </c>
+      <c r="A32" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -6168,13 +6222,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>483</v>
@@ -6414,7 +6468,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>5</v>
@@ -6427,13 +6481,18 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="4"/>
+      <c r="A60" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>651</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -6957,7 +7016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7632,7 +7691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -7847,7 +7906,7 @@
       </c>
       <c r="B9" s="8">
         <f>ists_gen!B104+state_gen!B18</f>
-        <v>19758.580000000002</v>
+        <v>19708.580000000002</v>
       </c>
       <c r="C9" t="s">
         <v>154</v>
@@ -7868,7 +7927,7 @@
       </c>
       <c r="B10" s="8">
         <f>ists_gen!B103+state_gen!B19</f>
-        <v>15034.86</v>
+        <v>15109.86</v>
       </c>
       <c r="C10" t="s">
         <v>149</v>
@@ -7889,7 +7948,7 @@
       </c>
       <c r="B11" s="8">
         <f>B10+B9</f>
-        <v>34793.440000000002</v>
+        <v>34818.44</v>
       </c>
       <c r="C11" t="s">
         <v>144</v>
@@ -7929,8 +7988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8435,25 +8494,42 @@
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>604</v>
-      </c>
-      <c r="B25" s="2">
+      <c r="A25" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="B25" s="4">
+        <v>161.80000000000001</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>603</v>
+      </c>
+      <c r="B26" s="2">
         <v>50</v>
       </c>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="F25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26"/>
+      <c r="C26" s="11"/>
       <c r="D26"/>
       <c r="F26" s="4" t="s">
         <v>17</v>
@@ -8466,7 +8542,7 @@
       </c>
       <c r="B27" s="4">
         <f>SUM(B16:B25)</f>
-        <v>2298.5</v>
+        <v>2410.3000000000002</v>
       </c>
       <c r="D27"/>
       <c r="F27" s="4" t="s">
@@ -8545,19 +8621,19 @@
     </row>
     <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>592</v>
+        <v>527</v>
       </c>
       <c r="B31" s="4">
-        <v>161.80000000000001</v>
+        <v>203.7</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>5</v>
@@ -8574,31 +8650,10 @@
     </row>
     <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="B32" s="4">
-        <v>203.7</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>573</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>574</v>
+        <v>70</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -8606,8 +8661,8 @@
         <v>478</v>
       </c>
       <c r="B33" s="4">
-        <f>SUM(B29:B32)</f>
-        <v>816.40000000000009</v>
+        <f>SUM(B29:B31)</f>
+        <v>654.59999999999991</v>
       </c>
       <c r="D33"/>
       <c r="F33" s="4" t="s">
@@ -8657,7 +8712,7 @@
     </row>
     <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B36" s="2">
         <v>210</v>
@@ -8686,19 +8741,19 @@
     </row>
     <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B37" s="2">
         <v>115</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>595</v>
+      </c>
+      <c r="E37" s="12" t="s">
         <v>596</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>597</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>5</v>
@@ -8740,7 +8795,7 @@
     </row>
     <row r="40" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B40" s="4">
         <v>324.39999999999998</v>
@@ -9107,19 +9162,19 @@
     </row>
     <row r="60" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B60" s="2">
         <v>100</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D60" s="12" t="s">
+        <v>605</v>
+      </c>
+      <c r="E60" s="12" t="s">
         <v>606</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>607</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>5</v>
@@ -9135,14 +9190,33 @@
       </c>
     </row>
     <row r="61" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D61"/>
+      <c r="A61" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="B61" s="2">
+        <v>75</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>643</v>
+      </c>
       <c r="F61" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I61" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="62" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
@@ -9169,8 +9243,8 @@
         <v>379</v>
       </c>
       <c r="B64" s="2">
-        <f>SUM(B56:B60)</f>
-        <v>600</v>
+        <f>SUM(B56:B61)</f>
+        <v>675</v>
       </c>
       <c r="D64"/>
       <c r="F64" s="4" t="s">
@@ -9468,25 +9542,25 @@
     </row>
     <row r="82" spans="1:9" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B82" s="2">
         <v>300</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D82" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="E82" s="10" t="s">
         <v>618</v>
       </c>
-      <c r="E82" s="10" t="s">
-        <v>619</v>
-      </c>
       <c r="F82" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>3</v>
@@ -9508,7 +9582,7 @@
     </row>
     <row r="84" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B84" s="2">
         <f>SUM(B82:B83)</f>
@@ -9519,7 +9593,7 @@
         <v>76</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="H84" s="2"/>
     </row>
@@ -9536,25 +9610,25 @@
     </row>
     <row r="86" spans="1:9" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B86" s="2">
         <v>1000</v>
       </c>
       <c r="C86" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="D86" s="10" t="s">
         <v>621</v>
       </c>
-      <c r="D86" s="10" t="s">
+      <c r="E86" s="10" t="s">
         <v>622</v>
       </c>
-      <c r="E86" s="10" t="s">
-        <v>623</v>
-      </c>
       <c r="F86" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G86" s="13" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>3</v>
@@ -9576,7 +9650,7 @@
     </row>
     <row r="88" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B88" s="2">
         <f>SUM(B86:B87)</f>
@@ -9587,7 +9661,7 @@
         <v>76</v>
       </c>
       <c r="G88" s="13" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="H88" s="2"/>
     </row>
@@ -9610,7 +9684,7 @@
         <v>500</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D90" s="18"/>
       <c r="E90" s="17"/>
@@ -9618,7 +9692,7 @@
         <v>17</v>
       </c>
       <c r="G90" s="13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>3</v>
@@ -9635,7 +9709,7 @@
         <v>100</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D91" s="18"/>
       <c r="E91" s="17"/>
@@ -9643,7 +9717,7 @@
         <v>17</v>
       </c>
       <c r="G91" s="13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>3</v>
@@ -9660,7 +9734,7 @@
         <v>250</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D92" s="18"/>
       <c r="E92" s="17"/>
@@ -9668,7 +9742,7 @@
         <v>17</v>
       </c>
       <c r="G92" s="13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>3</v>
@@ -9686,14 +9760,14 @@
         <v>850</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D93" s="11"/>
       <c r="F93" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G93" s="13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H93" s="2"/>
     </row>
@@ -9716,7 +9790,7 @@
         <v>12.5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D95" s="18"/>
       <c r="E95" s="17"/>
@@ -9724,7 +9798,7 @@
         <v>17</v>
       </c>
       <c r="G95" s="13" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>3</v>
@@ -9741,7 +9815,7 @@
         <v>162.5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D96" s="18"/>
       <c r="E96" s="17"/>
@@ -9749,7 +9823,7 @@
         <v>17</v>
       </c>
       <c r="G96" s="13" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>3</v>
@@ -9800,14 +9874,14 @@
         <v>175</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D100" s="11"/>
       <c r="F100" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G100" s="13" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H100" s="2"/>
     </row>
@@ -9838,7 +9912,7 @@
       </c>
       <c r="B103" s="4">
         <f>B54+B64+B68+B72+B76+B80+B84+B88</f>
-        <v>2786</v>
+        <v>2861</v>
       </c>
       <c r="C103" s="4"/>
       <c r="D103"/>
@@ -9857,7 +9931,7 @@
       </c>
       <c r="B104" s="4">
         <f>B27+B14+B33+B38+B43</f>
-        <v>4344.8999999999996</v>
+        <v>4294.8999999999996</v>
       </c>
       <c r="C104" s="4"/>
       <c r="D104"/>
@@ -9876,7 +9950,7 @@
       </c>
       <c r="B105" s="4">
         <f>B104+B103</f>
-        <v>7130.9</v>
+        <v>7155.9</v>
       </c>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
@@ -11137,8 +11211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11608,15 +11682,27 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="2"/>
+        <v>645</v>
+      </c>
+      <c r="B25" s="2">
+        <f>ists_gen!B25</f>
+        <v>161.80000000000001</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>571</v>
+      </c>
       <c r="D25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -11636,7 +11722,7 @@
       </c>
       <c r="B27" s="4">
         <f>ists_gen!B27</f>
-        <v>2298.5</v>
+        <v>2410.3000000000002</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>76</v>
@@ -11710,14 +11796,14 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B31" s="4">
         <f>ists_gen!B31</f>
-        <v>161.80000000000001</v>
+        <v>203.7</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>5</v>
@@ -11733,27 +11819,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="B32" s="4">
-        <f>ists_gen!B32</f>
-        <v>203.7</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>573</v>
+      <c r="A32" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>351</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -11762,7 +11832,7 @@
       </c>
       <c r="B33" s="4">
         <f>ists_gen!B33</f>
-        <v>816.40000000000009</v>
+        <v>654.59999999999991</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>76</v>
@@ -11835,13 +11905,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B37" s="4">
         <v>115</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>5</v>
@@ -12228,13 +12298,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B59" s="4">
         <v>100</v>
       </c>
-      <c r="C59" s="10" t="s">
-        <v>596</v>
+      <c r="C59" s="12" t="s">
+        <v>605</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>5</v>
@@ -12250,16 +12320,27 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" s="4"/>
+      <c r="A60" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="B60" s="4">
+        <v>75</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>642</v>
+      </c>
       <c r="D60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
@@ -12291,7 +12372,7 @@
       </c>
       <c r="B63" s="2">
         <f>ists_gen!B64</f>
-        <v>600</v>
+        <v>675</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>76</v>
@@ -12576,19 +12657,19 @@
     </row>
     <row r="81" spans="1:7" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B81" s="4">
         <v>300</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E81" s="16" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F81" s="4" t="s">
         <v>210</v>
@@ -12611,7 +12692,7 @@
     </row>
     <row r="83" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B83" s="2">
         <f>SUM(B81:B82)</f>
@@ -12621,7 +12702,7 @@
         <v>76</v>
       </c>
       <c r="E83" s="16" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="4"/>
@@ -12640,19 +12721,19 @@
     </row>
     <row r="85" spans="1:7" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B85" s="4">
         <v>1000</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E85" s="16" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>210</v>
@@ -12675,7 +12756,7 @@
     </row>
     <row r="87" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B87" s="2">
         <f>SUM(B85:B86)</f>
@@ -12685,7 +12766,7 @@
         <v>76</v>
       </c>
       <c r="E87" s="16" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="4"/>
@@ -12710,13 +12791,13 @@
         <v>500</v>
       </c>
       <c r="C89" s="19" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F89" s="4" t="s">
         <v>210</v>
@@ -12733,13 +12814,13 @@
         <v>100</v>
       </c>
       <c r="C90" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F90" s="4" t="s">
         <v>210</v>
@@ -12756,13 +12837,13 @@
         <v>250</v>
       </c>
       <c r="C91" s="19" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F91" s="4" t="s">
         <v>210</v>
@@ -12780,13 +12861,13 @@
         <v>850</v>
       </c>
       <c r="C92" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>636</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E92" s="13" t="s">
-        <v>637</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="4"/>
@@ -12811,13 +12892,13 @@
         <v>12.5</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F94" s="4" t="s">
         <v>210</v>
@@ -12834,13 +12915,13 @@
         <v>162.5</v>
       </c>
       <c r="C95" s="19" t="s">
+        <v>638</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E95" s="13" t="s">
         <v>639</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E95" s="13" t="s">
-        <v>640</v>
       </c>
       <c r="F95" s="4" t="s">
         <v>210</v>
@@ -12894,13 +12975,13 @@
         <v>175</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="4"/>
@@ -12947,7 +13028,7 @@
       </c>
       <c r="B103" s="4">
         <f>B71+B67+B63+B53+B75+B79+B83+B87</f>
-        <v>2786</v>
+        <v>2861</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>13</v>
@@ -12964,7 +13045,7 @@
       </c>
       <c r="B104" s="4">
         <f>B38+B33+B27+B14+B42</f>
-        <v>4344.8999999999996</v>
+        <v>4294.8999999999996</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>13</v>
@@ -12981,7 +13062,7 @@
       </c>
       <c r="B105" s="4">
         <f>B104+B103</f>
-        <v>7130.9</v>
+        <v>7155.9</v>
       </c>
       <c r="C105" s="4"/>
       <c r="D105" s="4" t="s">
@@ -13303,7 +13384,7 @@
       </c>
       <c r="B123" s="4">
         <f>regional_profile!B9</f>
-        <v>19758.580000000002</v>
+        <v>19708.580000000002</v>
       </c>
       <c r="C123" t="s">
         <v>283</v>
@@ -13318,7 +13399,7 @@
       </c>
       <c r="B124" s="4">
         <f>regional_profile!B10</f>
-        <v>15034.86</v>
+        <v>15109.86</v>
       </c>
       <c r="C124" t="s">
         <v>284</v>
@@ -13333,7 +13414,7 @@
       </c>
       <c r="B125" s="4">
         <f>B124+B123</f>
-        <v>34793.440000000002</v>
+        <v>34818.44</v>
       </c>
       <c r="C125" t="s">
         <v>282</v>
@@ -14261,8 +14342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63:F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14748,12 +14829,29 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>70</v>
+        <v>645</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>536</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -14842,22 +14940,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>5</v>
@@ -14868,28 +14966,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>537</v>
+        <v>70</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>479</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -14966,22 +15046,22 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="D38" s="9" t="s">
         <v>600</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="E38" s="9" t="s">
         <v>601</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>602</v>
-      </c>
       <c r="F38" s="9" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>5</v>
@@ -15340,22 +15420,22 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B62" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="C62" s="10" t="s">
         <v>609</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="D62" s="10" t="s">
         <v>610</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="E62" s="10" t="s">
         <v>611</v>
       </c>
-      <c r="E62" s="10" t="s">
-        <v>612</v>
-      </c>
       <c r="F62" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G62" s="11" t="s">
         <v>5</v>
@@ -15365,13 +15445,30 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>70</v>
+      <c r="A63" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>646</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>647</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>648</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>650</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H63" s="4"/>
+      <c r="H63" s="4" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
@@ -15698,28 +15795,28 @@
     </row>
     <row r="84" spans="1:8" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B84" s="10" t="s">
+        <v>624</v>
+      </c>
+      <c r="C84" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="D84" s="10" t="s">
         <v>626</v>
       </c>
-      <c r="D84" s="10" t="s">
+      <c r="E84" s="10" t="s">
         <v>627</v>
       </c>
-      <c r="E84" s="10" t="s">
-        <v>628</v>
-      </c>
       <c r="F84" s="10" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G84" s="11" t="s">
         <v>5</v>
       </c>
       <c r="H84" s="16" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="85" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -15738,7 +15835,7 @@
     </row>
     <row r="86" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -15749,7 +15846,7 @@
         <v>76</v>
       </c>
       <c r="H86" s="16" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="87" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -15768,28 +15865,28 @@
     </row>
     <row r="88" spans="1:8" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
+        <v>614</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="F88" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H88" s="16" t="s">
         <v>615</v>
-      </c>
-      <c r="B88" s="10" t="s">
-        <v>629</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>630</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>631</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>632</v>
-      </c>
-      <c r="F88" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G88" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H88" s="16" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="89" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -15808,7 +15905,7 @@
     </row>
     <row r="90" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -15819,7 +15916,7 @@
         <v>76</v>
       </c>
       <c r="H90" s="16" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new gens and ic changes
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\D Drive\POSOCO\IT\Python Projects\wr_remc_report_generator_configs\2025-02-25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\D Drive\POSOCO\IT\Python Projects\wr_remc_report_generator_configs\2025-03-07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11580" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="app_config" sheetId="18" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="scada_graph_data" sheetId="17" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ists_gen!$A$1:$I$108</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">remc_graph_data!$A$1:$C$56</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3557" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="769">
   <si>
     <t>name</t>
   </si>
@@ -2200,6 +2200,159 @@
   </si>
   <si>
     <t>ARE55L_PSS3_KPS1_S</t>
+  </si>
+  <si>
+    <t>Adani Renewable Energy Holding Four Limited-Solar (AREH4L_PSS1_KPS1_SF)</t>
+  </si>
+  <si>
+    <t>AGE25BL_PSS2_KPS1_S</t>
+  </si>
+  <si>
+    <t>NTPC_REL_SJPR_RUMS_S</t>
+  </si>
+  <si>
+    <t>NTPCREL1_SJPR_RUMS_S</t>
+  </si>
+  <si>
+    <t>NTPC_REL_SJPR_RUMS_S-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>NTPCREL1_SJPR_RUMS_S-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00088849</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00093355</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00088734</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00093335</t>
+  </si>
+  <si>
+    <t>ACL_PSS3_KPS1_S</t>
+  </si>
+  <si>
+    <t>ARE55L_PSS3_KPS1_HS</t>
+  </si>
+  <si>
+    <t>ACL_PSS3_KPS1_S-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>ARE55L_PSS3_KPS1_S-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00096591</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00096598</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00096594</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00088646</t>
+  </si>
+  <si>
+    <t>NTPC_REL_SJPR_RUMS_S-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>NTPC_REL_SJPR_RUMS_S-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>NTPC_REL_SJPR_RUMS_S-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>NTPC_REL_SJPR_RUMS_S-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>NTPCREL1_SJPR_RUMS_S-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>NTPCREL1_SJPR_RUMS_S-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>NTPCREL1_SJPR_RUMS_S-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>NTPCREL1_SJPR_RUMS_S-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>ACL_PSS3_KPS1_S-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>ACL_PSS3_KPS1_S-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>ACL_PSS3_KPS1_S-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>ACL_PSS3_KPS1_S-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>ARE55L_PSS3_KPS1_S-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>ARE55L_PSS3_KPS1_S-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>ARE55L_PSS3_KPS1_S-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>ARE55L_PSS3_KPS1_S-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>Neemuch Pooling</t>
+  </si>
+  <si>
+    <t>TPSOURY_KWAI_NMCH_S</t>
+  </si>
+  <si>
+    <t>TPSOURY_BRVD_NMCH_S</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00086554</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00090241</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00086499</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA02.00090240</t>
+  </si>
+  <si>
+    <t>TPSOURY_KWAI_NMCH_S-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>TPSOURY_BRVD_NMCH_S-SOLAR_SOLAR_AVC</t>
+  </si>
+  <si>
+    <t>TPSOURY_KWAI_NMCH_S-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>TPSOURY_KWAI_NMCH_S-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>TPSOURY_KWAI_NMCH_S-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>TPSOURY_KWAI_NMCH_S-SOLAR_SOLAR_CUF</t>
+  </si>
+  <si>
+    <t>TPSOURY_BRVD_NMCH_S-SOLAR_SOLAR_R0</t>
+  </si>
+  <si>
+    <t>TPSOURY_BRVD_NMCH_S-SOLAR_SOLAR_16</t>
+  </si>
+  <si>
+    <t>TPSOURY_BRVD_NMCH_S-SOLAR_SOLAR_Act</t>
+  </si>
+  <si>
+    <t>TPSOURY_BRVD_NMCH_S-SOLAR_SOLAR_CUF</t>
   </si>
 </sst>
 </file>
@@ -2314,9 +2467,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3058,10 +3211,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4394,65 +4547,76 @@
     </row>
     <row r="92" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>70</v>
+        <v>728</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>730</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>746</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F92" s="14"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>613</v>
-      </c>
-      <c r="E93" s="10" t="s">
-        <v>76</v>
+        <v>729</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>749</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>731</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>750</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="F93" s="14" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F94" s="14"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="10" t="s">
-        <v>689</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>703</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>706</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>704</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F95" s="10" t="s">
-        <v>691</v>
-      </c>
+        <v>613</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F95" s="14"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>5</v>
@@ -4463,17 +4627,139 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>691</v>
+        <v>690</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>700</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="F97" s="10" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
+    <row r="98" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>737</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>722</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>738</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>741</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>723</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>742</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F99" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F100" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B101" s="10"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
+        <v>753</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>759</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F102" s="10" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="s">
+        <v>754</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>760</v>
+      </c>
+      <c r="D103" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="E103" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F103" s="10" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="B104" s="10"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="10"/>
+      <c r="E104" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F104" s="10" t="s">
+        <v>752</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4742,10 +5028,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6113,25 +6399,39 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F92" s="14"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>728</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>730</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>746</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>613</v>
-      </c>
-      <c r="B93" s="10"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
+        <v>729</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>749</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>731</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>750</v>
+      </c>
       <c r="E93" s="10" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="F93" s="14" t="s">
         <v>613</v>
@@ -6139,48 +6439,42 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>70</v>
+        <v>613</v>
       </c>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
-      <c r="E94" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F94" s="14"/>
+      <c r="E94" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="10" t="s">
-        <v>689</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>703</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>706</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>704</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F95" s="10" t="s">
-        <v>691</v>
-      </c>
+      <c r="A95" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F95" s="14"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>5</v>
@@ -6191,16 +6485,135 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>691</v>
-      </c>
-      <c r="B97" s="10"/>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
+        <v>690</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>700</v>
+      </c>
       <c r="E97" s="10" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="F97" s="10" t="s">
         <v>691</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>737</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F99" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F100" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>753</v>
+      </c>
+      <c r="B102" t="s">
+        <v>762</v>
+      </c>
+      <c r="C102" t="s">
+        <v>759</v>
+      </c>
+      <c r="D102" t="s">
+        <v>763</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F102" s="10" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>754</v>
+      </c>
+      <c r="B103" t="s">
+        <v>766</v>
+      </c>
+      <c r="C103" t="s">
+        <v>760</v>
+      </c>
+      <c r="D103" t="s">
+        <v>767</v>
+      </c>
+      <c r="E103" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F103" s="10" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F104" s="10" t="s">
+        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -6562,7 +6975,7 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7792,7 +8205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -8587,7 +9000,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8681,7 +9094,7 @@
         <v>79</v>
       </c>
       <c r="B9" s="8">
-        <f>ists_gen!B104+state_gen!B20</f>
+        <f>ists_gen!B107+state_gen!B20</f>
         <v>20541.38</v>
       </c>
       <c r="C9" t="s">
@@ -8702,8 +9115,8 @@
         <v>80</v>
       </c>
       <c r="B10" s="8">
-        <f>ists_gen!B103+state_gen!B21</f>
-        <v>23492.2</v>
+        <f>ists_gen!B106+state_gen!B21</f>
+        <v>24482.184999999998</v>
       </c>
       <c r="C10" t="s">
         <v>149</v>
@@ -8724,7 +9137,7 @@
       </c>
       <c r="B11" s="8">
         <f>B10+B9</f>
-        <v>44033.58</v>
+        <v>45023.565000000002</v>
       </c>
       <c r="C11" t="s">
         <v>144</v>
@@ -8762,10 +9175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10401,7 +10814,7 @@
     </row>
     <row r="86" spans="1:9" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>611</v>
+        <v>718</v>
       </c>
       <c r="B86" s="2">
         <v>1000</v>
@@ -10430,10 +10843,10 @@
     </row>
     <row r="87" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>629</v>
+        <v>719</v>
       </c>
       <c r="B87" s="2">
-        <v>499.97500000000002</v>
+        <v>582.97500000000002</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>653</v>
@@ -10462,7 +10875,7 @@
         <v>714</v>
       </c>
       <c r="B88" s="2">
-        <v>87.724999999999994</v>
+        <v>167</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>654</v>
@@ -10491,7 +10904,7 @@
         <v>715</v>
       </c>
       <c r="B89" s="2">
-        <v>387.5</v>
+        <v>500</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>657</v>
@@ -10574,41 +10987,55 @@
       </c>
     </row>
     <row r="92" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
-        <v>613</v>
+      <c r="A92" s="10" t="s">
+        <v>728</v>
       </c>
       <c r="B92" s="2">
-        <f>SUM(B86:B91)</f>
-        <v>2150.1999999999998</v>
+        <v>200</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>733</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="G92" s="11" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H92" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
-        <v>689</v>
+        <v>729</v>
       </c>
       <c r="B93" s="2">
-        <v>350</v>
-      </c>
-      <c r="C93" s="20" t="s">
-        <v>696</v>
-      </c>
-      <c r="D93" s="18" t="s">
-        <v>694</v>
-      </c>
-      <c r="E93" s="18" t="s">
-        <v>695</v>
+        <v>25</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>731</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>665</v>
       </c>
       <c r="F93" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G93" s="10" t="s">
-        <v>691</v>
+      <c r="G93" s="11" t="s">
+        <v>613</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>3</v>
@@ -10617,125 +11044,167 @@
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
+    <row r="94" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="B94" s="2">
+        <f>SUM(B86:B93)</f>
+        <v>2649.9749999999999</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G95" s="11"/>
+    </row>
+    <row r="96" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="B96" s="2">
+        <v>350</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>696</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="10" t="s">
         <v>690</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B97" s="2">
         <v>200</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C97" s="10" t="s">
         <v>697</v>
       </c>
-      <c r="D94" s="18" t="s">
+      <c r="D97" s="10" t="s">
         <v>692</v>
       </c>
-      <c r="E94" s="18" t="s">
+      <c r="E97" s="10" t="s">
         <v>693</v>
       </c>
-      <c r="F94" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G94" s="10" t="s">
+      <c r="F97" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G97" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="H94" s="2" t="s">
+      <c r="H97" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I94" s="2" t="s">
+      <c r="I97" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="10" t="s">
+    <row r="98" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="B98" s="2">
+        <v>100</v>
+      </c>
+      <c r="C98" s="19" t="s">
+        <v>722</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>724</v>
+      </c>
+      <c r="E98" s="18" t="s">
+        <v>725</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G98" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="B95" s="2">
-        <f>B93+B94</f>
-        <v>550</v>
-      </c>
-      <c r="C95" s="19"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="19"/>
-      <c r="F95" s="4" t="s">
+      <c r="H98" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="B99" s="2">
+        <v>55</v>
+      </c>
+      <c r="C99" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>726</v>
+      </c>
+      <c r="E99" s="18" t="s">
+        <v>727</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="B100" s="2">
+        <f>SUM(B96:B99)</f>
+        <v>705</v>
+      </c>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G95" s="10" t="s">
+      <c r="G100" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
-    </row>
-    <row r="96" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G96" s="11"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-    </row>
-    <row r="97" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H97" s="2"/>
-    </row>
-    <row r="98" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H98" s="2"/>
-    </row>
-    <row r="99" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H99" s="2"/>
-    </row>
-    <row r="100" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G100" s="11"/>
       <c r="H100" s="2"/>
     </row>
     <row r="101" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B101" s="2"/>
@@ -10749,89 +11218,166 @@
     </row>
     <row r="102" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D102"/>
+        <v>753</v>
+      </c>
+      <c r="B102" s="2">
+        <v>170</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>756</v>
+      </c>
       <c r="F102" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H102" s="2"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G102" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
+        <v>754</v>
+      </c>
+      <c r="B103" s="2">
+        <v>160</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G103" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="B104" s="2">
+        <f>SUM(B102:B103)</f>
+        <v>330</v>
+      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G104" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="H104" s="2"/>
+    </row>
+    <row r="105" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D105"/>
+      <c r="F105" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H105" s="2"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B103" s="4">
-        <f>B54+B64+B68+B72+B76+B80+B84+B92+B95</f>
-        <v>4586.2</v>
-      </c>
-      <c r="C103" s="4"/>
-      <c r="D103"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4" t="s">
+      <c r="B106" s="4">
+        <f>B54+B64+B68+B72+B76+B80+B84+B94+B100+B104</f>
+        <v>5570.9750000000004</v>
+      </c>
+      <c r="C106" s="4"/>
+      <c r="D106"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4" t="s">
+      <c r="G106" s="4"/>
+      <c r="H106" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B104" s="4">
+      <c r="B107" s="4">
         <f>B27+B14+B33+B38+B43</f>
         <v>4538.7</v>
       </c>
-      <c r="C104" s="4"/>
-      <c r="D104"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4" t="s">
+      <c r="C107" s="4"/>
+      <c r="D107"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4" t="s">
+      <c r="G107" s="4"/>
+      <c r="H107" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B105" s="4">
-        <f>B104+B103</f>
-        <v>9124.9</v>
-      </c>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4" t="s">
+      <c r="B108" s="4">
+        <f>B107+B106</f>
+        <v>10109.674999999999</v>
+      </c>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I105" s="1" t="s">
+      <c r="I108" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10843,8 +11389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11092,7 +11638,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="4">
-        <v>2077</v>
+        <v>2082.21</v>
       </c>
       <c r="C14" t="s">
         <v>159</v>
@@ -11151,7 +11697,7 @@
       </c>
       <c r="B16" s="4">
         <f>B15+B14</f>
-        <v>4605.68</v>
+        <v>4610.8899999999994</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>26</v>
@@ -11224,7 +11770,7 @@
       </c>
       <c r="B21" s="4">
         <f>B6+B10+B14+B18</f>
-        <v>18906</v>
+        <v>18911.21</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>13</v>
@@ -11239,7 +11785,7 @@
       </c>
       <c r="B22" s="4">
         <f>SUM(B20:B21)</f>
-        <v>34908.68</v>
+        <v>34913.89</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>74</v>
@@ -12095,10 +12641,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G206"/>
+  <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A83" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13651,7 +14197,7 @@
       </c>
       <c r="B86" s="4">
         <f>ists_gen!B87</f>
-        <v>499.97500000000002</v>
+        <v>582.97500000000002</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>658</v>
@@ -13675,7 +14221,7 @@
       </c>
       <c r="B87" s="4">
         <f>ists_gen!B88</f>
-        <v>87.724999999999994</v>
+        <v>167</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>660</v>
@@ -13699,7 +14245,7 @@
       </c>
       <c r="B88" s="4">
         <f>ists_gen!B89</f>
-        <v>387.5</v>
+        <v>500</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>662</v>
@@ -13766,38 +14312,43 @@
       </c>
     </row>
     <row r="91" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="11" t="s">
-        <v>613</v>
-      </c>
-      <c r="B91" s="2">
-        <f>ists_gen!B92</f>
-        <v>2150.1999999999998</v>
+      <c r="A91" s="10" t="s">
+        <v>728</v>
+      </c>
+      <c r="B91" s="4">
+        <v>200</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>734</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="E91" s="14" t="s">
         <v>612</v>
       </c>
-      <c r="F91" s="4"/>
-      <c r="G91" s="2"/>
+      <c r="F91" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="92" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
-        <v>689</v>
-      </c>
-      <c r="B92" s="2">
-        <f>ists_gen!B93</f>
-        <v>350</v>
-      </c>
-      <c r="C92" s="18" t="s">
-        <v>694</v>
+        <v>729</v>
+      </c>
+      <c r="B92" s="4">
+        <v>25</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>735</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E92" s="10" t="s">
-        <v>691</v>
+      <c r="E92" s="14" t="s">
+        <v>612</v>
       </c>
       <c r="F92" s="4" t="s">
         <v>210</v>
@@ -13807,103 +14358,142 @@
       </c>
     </row>
     <row r="93" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
-        <v>690</v>
+      <c r="A93" s="11" t="s">
+        <v>613</v>
       </c>
       <c r="B93" s="2">
         <f>ists_gen!B94</f>
+        <v>2649.9749999999999</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>612</v>
+      </c>
+      <c r="F93" s="4"/>
+      <c r="G93" s="2"/>
+    </row>
+    <row r="94" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B94" s="2"/>
+      <c r="D94" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E94" s="14"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="B95" s="2">
+        <f>ists_gen!B96</f>
+        <v>350</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="B96" s="2">
+        <f>ists_gen!B97</f>
         <v>200</v>
       </c>
-      <c r="C93" s="18" t="s">
+      <c r="C96" s="10" t="s">
         <v>692</v>
       </c>
-      <c r="D93" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E93" s="10" t="s">
+      <c r="D96" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E96" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="F93" s="4" t="s">
+      <c r="F96" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G93" s="2" t="s">
+      <c r="G96" s="2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
+    <row r="97" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="B97" s="2">
+        <v>100</v>
+      </c>
+      <c r="C97" s="21" t="s">
+        <v>724</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E97" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="B94" s="2">
-        <f>ists_gen!B95</f>
-        <v>550</v>
-      </c>
-      <c r="D94" s="4" t="s">
+      <c r="F97" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="B98" s="2">
+        <v>55</v>
+      </c>
+      <c r="C98" s="21" t="s">
+        <v>726</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="B99" s="2">
+        <f>ists_gen!B100</f>
+        <v>705</v>
+      </c>
+      <c r="D99" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="E99" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="F94" s="2"/>
-      <c r="G94" s="4"/>
-    </row>
-    <row r="95" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B95" s="2"/>
-      <c r="D95" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E95" s="11"/>
-      <c r="F95" s="4"/>
-      <c r="G95" s="2"/>
-    </row>
-    <row r="96" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B96" s="2"/>
-      <c r="D96" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E96" s="11"/>
-      <c r="F96" s="4"/>
-      <c r="G96" s="2"/>
-    </row>
-    <row r="97" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B97" s="2"/>
-      <c r="D97" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E97" s="4"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="4"/>
-    </row>
-    <row r="98" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B98" s="2"/>
-      <c r="D98" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E98" s="4"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="4"/>
-    </row>
-    <row r="99" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B99" s="2"/>
-      <c r="D99" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E99" s="4"/>
       <c r="F99" s="2"/>
       <c r="G99" s="4"/>
     </row>
@@ -13915,473 +14505,524 @@
       <c r="D100" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E100" s="11"/>
+      <c r="E100" s="4"/>
       <c r="F100" s="2"/>
       <c r="G100" s="4"/>
     </row>
     <row r="101" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B101" s="2"/>
+      <c r="A101" s="10" t="s">
+        <v>753</v>
+      </c>
+      <c r="B101" s="2">
+        <v>170</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>755</v>
+      </c>
       <c r="D101" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E101" s="4"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="102" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B102" s="4"/>
+      <c r="A102" s="10" t="s">
+        <v>754</v>
+      </c>
+      <c r="B102" s="2">
+        <v>160</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>757</v>
+      </c>
       <c r="D102" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E102" s="4"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="103" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B103" s="4"/>
+      <c r="A103" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="B103" s="2">
+        <f>ists_gen!B104</f>
+        <v>330</v>
+      </c>
       <c r="D103" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E103" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="E103" s="10" t="s">
+        <v>752</v>
+      </c>
       <c r="F103" s="2"/>
       <c r="G103" s="4"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="B104" s="4">
-        <f>ists_gen!B103</f>
-        <v>4586.2</v>
-      </c>
+    <row r="104" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B104" s="2"/>
       <c r="D104" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E104" s="4"/>
-      <c r="F104" s="4" t="s">
-        <v>210</v>
-      </c>
+      <c r="F104" s="2"/>
       <c r="G104" s="4"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="B105" s="4">
-        <f>ists_gen!B104</f>
-        <v>4538.7</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B105" s="4"/>
       <c r="D105" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E105" s="4"/>
-      <c r="F105" s="4" t="s">
-        <v>211</v>
-      </c>
+      <c r="F105" s="2"/>
       <c r="G105" s="4"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B106" s="4">
-        <f>ists_gen!B105</f>
-        <v>9124.9</v>
-      </c>
-      <c r="C106" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="B106" s="4"/>
       <c r="D106" s="4" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
-      <c r="G106" s="2" t="s">
-        <v>349</v>
-      </c>
+      <c r="F106" s="2"/>
+      <c r="G106" s="4"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
+        <v>350</v>
+      </c>
+      <c r="B107" s="4">
+        <f>ists_gen!B106</f>
+        <v>5570.9750000000004</v>
+      </c>
       <c r="D107" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
+      <c r="F107" s="4" t="s">
+        <v>210</v>
+      </c>
       <c r="G107" s="4"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B108" s="4">
+        <f>ists_gen!B107</f>
+        <v>4538.7</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G108" s="4"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B109" s="4">
+        <f>ists_gen!B108</f>
+        <v>10109.674999999999</v>
+      </c>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B108" s="4">
+      <c r="B111" s="4">
         <f>state_gen!B6</f>
         <v>11262</v>
       </c>
-      <c r="C108" s="10" t="s">
+      <c r="C111" s="10" t="s">
         <v>711</v>
       </c>
-      <c r="D108" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E108" s="4" t="s">
+      <c r="D111" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E111" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="F111" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="G111" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B109" s="4">
+      <c r="B112" s="4">
         <f>state_gen!B7</f>
         <v>8206</v>
       </c>
-      <c r="C109" s="10" t="s">
+      <c r="C112" s="10" t="s">
         <v>712</v>
       </c>
-      <c r="D109" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E109" s="4" t="s">
+      <c r="D112" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E112" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F109" s="4" t="s">
+      <c r="F112" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="G109" s="2" t="s">
+      <c r="G112" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B110" s="4">
+      <c r="B113" s="4">
         <f>state_gen!B8</f>
         <v>19468</v>
       </c>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4" t="s">
+      <c r="C113" s="4"/>
+      <c r="D113" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E110" s="4" t="s">
+      <c r="E113" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B112" s="4">
+      <c r="B115" s="4">
         <f>state_gen!B10</f>
         <v>4725</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C115" t="s">
         <v>285</v>
       </c>
-      <c r="D112" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E112" s="4" t="s">
+      <c r="D115" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E115" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="F115" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="G112" s="2" t="s">
+      <c r="G115" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B113" s="4">
+      <c r="B116" s="4">
         <f>state_gen!B11</f>
         <v>5268</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C116" t="s">
         <v>286</v>
       </c>
-      <c r="D113" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E113" s="4" t="s">
+      <c r="D116" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E116" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F113" s="4" t="s">
+      <c r="F116" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="G113" s="2" t="s">
+      <c r="G116" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B114" s="4">
+      <c r="B117" s="4">
         <f>state_gen!B12</f>
         <v>9993</v>
       </c>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4" t="s">
+      <c r="C117" s="4"/>
+      <c r="D117" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E114" s="4" t="s">
+      <c r="E117" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F114" s="4"/>
-      <c r="G114" s="4"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B115" s="4"/>
-      <c r="C115" s="4"/>
-      <c r="D115" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E115" s="4"/>
-      <c r="F115" s="4"/>
-      <c r="G115" s="4"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B116" s="4">
+      <c r="B119" s="4">
         <f>state_gen!B14</f>
-        <v>2077</v>
-      </c>
-      <c r="C116" t="s">
+        <v>2082.21</v>
+      </c>
+      <c r="C119" t="s">
         <v>288</v>
       </c>
-      <c r="D116" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E116" s="4" t="s">
+      <c r="D119" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E119" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F116" s="2" t="s">
+      <c r="F119" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="G119" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B117" s="4">
+      <c r="B120" s="4">
         <f>state_gen!B15</f>
         <v>2528.6799999999998</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C120" t="s">
         <v>287</v>
       </c>
-      <c r="D117" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E117" s="4" t="s">
+      <c r="D120" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E120" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F117" s="4" t="s">
+      <c r="F120" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="G117" s="2" t="s">
+      <c r="G120" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="4" t="s">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B118" s="4">
+      <c r="B121" s="4">
         <f>state_gen!B16</f>
-        <v>4605.68</v>
-      </c>
-      <c r="D118" s="4" t="s">
+        <v>4610.8899999999994</v>
+      </c>
+      <c r="D121" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E118" s="4" t="s">
+      <c r="E121" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F118" s="4"/>
-      <c r="G118" s="4"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B119" s="4"/>
-      <c r="D119" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
-      <c r="G119" s="4"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B122" s="4"/>
+      <c r="D122" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B120" s="4">
+      <c r="B123" s="4">
         <f>state_gen!B20</f>
         <v>16002.68</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="D123" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4" t="s">
+      <c r="E123" s="4"/>
+      <c r="F123" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="G120" s="4"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+      <c r="G123" s="4"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B121" s="4">
+      <c r="B124" s="4">
         <f>state_gen!B21</f>
-        <v>18906</v>
-      </c>
-      <c r="D121" s="2" t="s">
+        <v>18911.21</v>
+      </c>
+      <c r="D124" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E121" s="4"/>
-      <c r="F121" s="2" t="s">
+      <c r="E124" s="4"/>
+      <c r="F124" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="G121" s="4"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+      <c r="G124" s="4"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B122" s="4">
+      <c r="B125" s="4">
         <f>state_gen!B22</f>
-        <v>34908.68</v>
-      </c>
-      <c r="D122" s="2" t="s">
+        <v>34913.89</v>
+      </c>
+      <c r="D125" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E122" s="4"/>
-      <c r="F122" s="4"/>
-      <c r="G122" s="2" t="s">
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B123" s="4"/>
-      <c r="D123" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B126" s="4"/>
+      <c r="D126" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B124" s="4">
+      <c r="B127" s="4">
         <f>regional_profile!B9</f>
         <v>20541.38</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C127" t="s">
         <v>283</v>
       </c>
-      <c r="D124" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
+      <c r="D127" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B125" s="4">
+      <c r="B128" s="4">
         <f>regional_profile!B10</f>
-        <v>23492.2</v>
-      </c>
-      <c r="C125" t="s">
+        <v>24482.184999999998</v>
+      </c>
+      <c r="C128" t="s">
         <v>284</v>
       </c>
-      <c r="D125" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
+      <c r="D128" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B126" s="4">
-        <f>B125+B124</f>
-        <v>44033.58</v>
-      </c>
-      <c r="C126" t="s">
+      <c r="B129" s="4">
+        <f>B128+B127</f>
+        <v>45023.565000000002</v>
+      </c>
+      <c r="C129" t="s">
         <v>282</v>
       </c>
-      <c r="D126" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B127" s="4"/>
-      <c r="D127" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="4"/>
-      <c r="D128" s="4"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="4"/>
-      <c r="D129" s="4"/>
+      <c r="D129" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="4"/>
-      <c r="D130" s="4"/>
+      <c r="A130" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B130" s="4"/>
+      <c r="D130" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
@@ -14497,56 +15138,59 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
+      <c r="D159" s="4"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D160" s="4"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D161" s="4"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
@@ -14638,6 +15282,15 @@
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="4"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="4"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15375,10 +16028,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95:F96"/>
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16945,19 +17598,19 @@
       <c r="A89" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="B89" s="21" t="s">
+      <c r="B89" s="20" t="s">
         <v>668</v>
       </c>
-      <c r="C89" s="21" t="s">
+      <c r="C89" s="20" t="s">
         <v>669</v>
       </c>
-      <c r="D89" s="21" t="s">
+      <c r="D89" s="20" t="s">
         <v>670</v>
       </c>
-      <c r="E89" s="21" t="s">
+      <c r="E89" s="20" t="s">
         <v>671</v>
       </c>
-      <c r="F89" s="21" t="s">
+      <c r="F89" s="20" t="s">
         <v>653</v>
       </c>
       <c r="G89" s="10" t="s">
@@ -16971,19 +17624,19 @@
       <c r="A90" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="B90" s="21" t="s">
+      <c r="B90" s="20" t="s">
         <v>672</v>
       </c>
-      <c r="C90" s="21" t="s">
+      <c r="C90" s="20" t="s">
         <v>673</v>
       </c>
-      <c r="D90" s="21" t="s">
+      <c r="D90" s="20" t="s">
         <v>674</v>
       </c>
-      <c r="E90" s="21" t="s">
+      <c r="E90" s="20" t="s">
         <v>675</v>
       </c>
-      <c r="F90" s="21" t="s">
+      <c r="F90" s="20" t="s">
         <v>654</v>
       </c>
       <c r="G90" s="10" t="s">
@@ -16997,19 +17650,19 @@
       <c r="A91" s="10" t="s">
         <v>630</v>
       </c>
-      <c r="B91" s="21" t="s">
+      <c r="B91" s="20" t="s">
         <v>676</v>
       </c>
-      <c r="C91" s="21" t="s">
+      <c r="C91" s="20" t="s">
         <v>677</v>
       </c>
-      <c r="D91" s="21" t="s">
+      <c r="D91" s="20" t="s">
         <v>678</v>
       </c>
-      <c r="E91" s="21" t="s">
+      <c r="E91" s="20" t="s">
         <v>679</v>
       </c>
-      <c r="F91" s="21" t="s">
+      <c r="F91" s="20" t="s">
         <v>657</v>
       </c>
       <c r="G91" s="10" t="s">
@@ -17023,19 +17676,19 @@
       <c r="A92" s="10" t="s">
         <v>632</v>
       </c>
-      <c r="B92" s="21" t="s">
+      <c r="B92" s="20" t="s">
         <v>680</v>
       </c>
-      <c r="C92" s="21" t="s">
+      <c r="C92" s="20" t="s">
         <v>681</v>
       </c>
-      <c r="D92" s="21" t="s">
+      <c r="D92" s="20" t="s">
         <v>682</v>
       </c>
-      <c r="E92" s="21" t="s">
+      <c r="E92" s="20" t="s">
         <v>683</v>
       </c>
-      <c r="F92" s="21" t="s">
+      <c r="F92" s="20" t="s">
         <v>655</v>
       </c>
       <c r="G92" s="10" t="s">
@@ -17049,19 +17702,19 @@
       <c r="A93" s="10" t="s">
         <v>633</v>
       </c>
-      <c r="B93" s="21" t="s">
+      <c r="B93" s="20" t="s">
         <v>684</v>
       </c>
-      <c r="C93" s="21" t="s">
+      <c r="C93" s="20" t="s">
         <v>685</v>
       </c>
-      <c r="D93" s="21" t="s">
+      <c r="D93" s="20" t="s">
         <v>686</v>
       </c>
-      <c r="E93" s="21" t="s">
+      <c r="E93" s="20" t="s">
         <v>687</v>
       </c>
-      <c r="F93" s="21" t="s">
+      <c r="F93" s="20" t="s">
         <v>656</v>
       </c>
       <c r="G93" s="10" t="s">
@@ -17072,16 +17725,26 @@
       </c>
     </row>
     <row r="94" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14" t="s">
-        <v>613</v>
-      </c>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
+      <c r="A94" s="10" t="s">
+        <v>728</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>744</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>745</v>
+      </c>
+      <c r="D94" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="E94" s="20" t="s">
+        <v>747</v>
+      </c>
+      <c r="F94" s="20" t="s">
+        <v>730</v>
+      </c>
       <c r="G94" s="10" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="H94" s="14" t="s">
         <v>612</v>
@@ -17089,235 +17752,343 @@
     </row>
     <row r="95" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>689</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>702</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>703</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>704</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>705</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>706</v>
+        <v>729</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>748</v>
+      </c>
+      <c r="C95" s="20" t="s">
+        <v>749</v>
+      </c>
+      <c r="D95" s="20" t="s">
+        <v>750</v>
+      </c>
+      <c r="E95" s="20" t="s">
+        <v>751</v>
+      </c>
+      <c r="F95" s="20" t="s">
+        <v>731</v>
       </c>
       <c r="G95" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H95" s="10" t="s">
-        <v>691</v>
+      <c r="H95" s="14" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="10" t="s">
-        <v>690</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>698</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>699</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>700</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>701</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>697</v>
-      </c>
+      <c r="A96" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
       <c r="G96" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H96" s="10" t="s">
-        <v>691</v>
+        <v>76</v>
+      </c>
+      <c r="H96" s="14" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="97" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="10" t="s">
-        <v>691</v>
+      <c r="A97" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="10" t="s">
+      <c r="G97" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H97" s="14"/>
+    </row>
+    <row r="98" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H98" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>699</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>700</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H99" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>736</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>738</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>739</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H100" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>741</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>742</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>743</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>723</v>
+      </c>
+      <c r="G101" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H101" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H97" s="10" t="s">
+      <c r="H102" s="10" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
-      <c r="G98" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H98" s="4"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>83</v>
-      </c>
-      <c r="B99" t="s">
-        <v>99</v>
-      </c>
-      <c r="C99" t="s">
-        <v>100</v>
-      </c>
-      <c r="D99" t="s">
-        <v>101</v>
-      </c>
-      <c r="E99" t="s">
-        <v>102</v>
-      </c>
-      <c r="F99" t="s">
-        <v>103</v>
-      </c>
-      <c r="G99" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>84</v>
-      </c>
-      <c r="B100" t="s">
-        <v>94</v>
-      </c>
-      <c r="C100" t="s">
-        <v>95</v>
-      </c>
-      <c r="D100" t="s">
-        <v>96</v>
-      </c>
-      <c r="E100" t="s">
-        <v>97</v>
-      </c>
-      <c r="F100" t="s">
-        <v>98</v>
-      </c>
-      <c r="G100" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>85</v>
-      </c>
-      <c r="B101" t="s">
-        <v>89</v>
-      </c>
-      <c r="C101" t="s">
-        <v>90</v>
-      </c>
-      <c r="D101" t="s">
-        <v>91</v>
-      </c>
-      <c r="E101" t="s">
-        <v>92</v>
-      </c>
-      <c r="F101" t="s">
-        <v>93</v>
-      </c>
-      <c r="G101" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H102" s="4"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
       <c r="G103" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H103" s="4"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H104" s="4"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H105" s="4"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H106" s="4"/>
+    </row>
+    <row r="104" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="s">
+        <v>753</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>763</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="G104" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H104" s="10" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="10" t="s">
+        <v>754</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>766</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>768</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="G105" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H105" s="10" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H106" s="10" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
       <c r="G107" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H107" s="4"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H108" s="4"/>
+      <c r="A108" t="s">
+        <v>83</v>
+      </c>
+      <c r="B108" t="s">
+        <v>99</v>
+      </c>
+      <c r="C108" t="s">
+        <v>100</v>
+      </c>
+      <c r="D108" t="s">
+        <v>101</v>
+      </c>
+      <c r="E108" t="s">
+        <v>102</v>
+      </c>
+      <c r="F108" t="s">
+        <v>103</v>
+      </c>
+      <c r="G108" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H109" s="4"/>
+      <c r="A109" t="s">
+        <v>84</v>
+      </c>
+      <c r="B109" t="s">
+        <v>94</v>
+      </c>
+      <c r="C109" t="s">
+        <v>95</v>
+      </c>
+      <c r="D109" t="s">
+        <v>96</v>
+      </c>
+      <c r="E109" t="s">
+        <v>97</v>
+      </c>
+      <c r="F109" t="s">
+        <v>98</v>
+      </c>
+      <c r="G109" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H110" s="4"/>
+      <c r="A110" t="s">
+        <v>85</v>
+      </c>
+      <c r="B110" t="s">
+        <v>89</v>
+      </c>
+      <c r="C110" t="s">
+        <v>90</v>
+      </c>
+      <c r="D110" t="s">
+        <v>91</v>
+      </c>
+      <c r="E110" t="s">
+        <v>92</v>
+      </c>
+      <c r="F110" t="s">
+        <v>93</v>
+      </c>
+      <c r="G110" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
@@ -17327,6 +18098,87 @@
         <v>17</v>
       </c>
       <c r="H111" s="4"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H112" s="4"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H113" s="4"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H114" s="4"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H115" s="4"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H116" s="4"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H117" s="4"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H118" s="4"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H119" s="4"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H120" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
wbes data fetch start
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.2.100.58\wrldc_remc_reports_generator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\D Drive\POSOCO\IT\Python Projects\wrldc_remc_reports_generator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3490" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="724">
   <si>
     <t>name</t>
   </si>
@@ -2218,6 +2218,12 @@
   </si>
   <si>
     <t>WR-ISTS_COMBINED</t>
+  </si>
+  <si>
+    <t>SIPAT1</t>
+  </si>
+  <si>
+    <t>wbes_acr</t>
   </si>
 </sst>
 </file>
@@ -2680,8 +2686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,10 +2704,11 @@
     <col min="11" max="11" width="45.140625" style="6" customWidth="1"/>
     <col min="12" max="12" width="45.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="38.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="6"/>
+    <col min="14" max="14" width="13.7109375" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2741,8 +2748,11 @@
       <c r="M1" s="6" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="6" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>76</v>
       </c>
@@ -2779,8 +2789,11 @@
       <c r="M2" s="6" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>77</v>
       </c>
@@ -2817,8 +2830,11 @@
       <c r="M3" s="6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -2855,8 +2871,11 @@
       <c r="M4" s="6" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N4" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>531</v>
       </c>
@@ -2896,8 +2915,11 @@
       <c r="M5" s="6" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>524</v>
       </c>
@@ -2937,8 +2959,11 @@
       <c r="M6" s="6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N6" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>532</v>
       </c>
@@ -2978,8 +3003,11 @@
       <c r="M7" s="6" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>318</v>
       </c>
@@ -3019,8 +3047,11 @@
       <c r="M8" s="6" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>319</v>
       </c>
@@ -3060,8 +3091,11 @@
       <c r="M9" s="6" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>317</v>
       </c>
@@ -3101,8 +3135,11 @@
       <c r="M10" s="6" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N10" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>525</v>
       </c>
@@ -3142,8 +3179,11 @@
       <c r="M11" s="6" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>526</v>
       </c>
@@ -3183,8 +3223,11 @@
       <c r="M12" s="6" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>527</v>
       </c>
@@ -3224,8 +3267,11 @@
       <c r="M13" s="6" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N13" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>528</v>
       </c>
@@ -3265,8 +3311,11 @@
       <c r="M14" s="6" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>529</v>
       </c>
@@ -3306,8 +3355,11 @@
       <c r="M15" s="6" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>530</v>
       </c>
@@ -3347,8 +3399,11 @@
       <c r="M16" s="6" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>572</v>
       </c>
@@ -3388,8 +3443,11 @@
       <c r="M17" s="15" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>546</v>
       </c>
@@ -3429,8 +3487,11 @@
       <c r="M18" s="16" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>533</v>
       </c>
@@ -3470,8 +3531,11 @@
       <c r="M19" s="6" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N19" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>534</v>
       </c>
@@ -3511,8 +3575,11 @@
       <c r="M20" s="6" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>473</v>
       </c>
@@ -3552,8 +3619,11 @@
       <c r="M21" s="15" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>417</v>
       </c>
@@ -3593,8 +3663,11 @@
       <c r="M22" s="6" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N22" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>535</v>
       </c>
@@ -3634,8 +3707,11 @@
       <c r="M23" s="15" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>537</v>
       </c>
@@ -3675,8 +3751,11 @@
       <c r="M24" s="17" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N24" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>536</v>
       </c>
@@ -3716,8 +3795,11 @@
       <c r="M25" s="15" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>316</v>
       </c>
@@ -3757,8 +3839,11 @@
       <c r="M26" s="6" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>392</v>
       </c>
@@ -3798,8 +3883,11 @@
       <c r="M27" s="6" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>315</v>
       </c>
@@ -3839,8 +3927,11 @@
       <c r="M28" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>334</v>
       </c>
@@ -3880,8 +3971,11 @@
       <c r="M29" s="8" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>338</v>
       </c>
@@ -3921,8 +4015,11 @@
       <c r="M30" s="8" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>342</v>
       </c>
@@ -3962,8 +4059,11 @@
       <c r="M31" s="8" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="6" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>403</v>
       </c>
@@ -4002,6 +4102,9 @@
       </c>
       <c r="M32" s="8" t="s">
         <v>713</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -4044,6 +4147,9 @@
       <c r="M33" s="24" t="s">
         <v>713</v>
       </c>
+      <c r="N33" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -4085,6 +4191,9 @@
       <c r="M34" s="24" t="s">
         <v>714</v>
       </c>
+      <c r="N34" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -4126,6 +4235,9 @@
       <c r="M35" s="8" t="s">
         <v>715</v>
       </c>
+      <c r="N35" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O35" s="8"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -4168,6 +4280,9 @@
       <c r="M36" s="8" t="s">
         <v>716</v>
       </c>
+      <c r="N36" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O36" s="8"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -4210,6 +4325,9 @@
       <c r="M37" s="7" t="s">
         <v>717</v>
       </c>
+      <c r="N37" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O37" s="8"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -4252,6 +4370,9 @@
       <c r="M38" s="7" t="s">
         <v>718</v>
       </c>
+      <c r="N38" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O38" s="8"/>
     </row>
     <row r="39" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4292,6 +4413,9 @@
         <v>561</v>
       </c>
       <c r="M39" s="15"/>
+      <c r="N39" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="40" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
@@ -4331,6 +4455,9 @@
         <v>672</v>
       </c>
       <c r="M40" s="15"/>
+      <c r="N40" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O40" s="8"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -4370,6 +4497,9 @@
       <c r="L41" s="6" t="s">
         <v>673</v>
       </c>
+      <c r="N41" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O41" s="8"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -4409,6 +4539,9 @@
       <c r="L42" s="15" t="s">
         <v>674</v>
       </c>
+      <c r="N42" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O42" s="8"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -4448,6 +4581,9 @@
       <c r="L43" s="15" t="s">
         <v>675</v>
       </c>
+      <c r="N43" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
@@ -4487,6 +4623,9 @@
         <v>676</v>
       </c>
       <c r="M44" s="18"/>
+      <c r="N44" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O44" s="8"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -4526,6 +4665,9 @@
       <c r="L45" s="15" t="s">
         <v>636</v>
       </c>
+      <c r="N45" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O45" s="8"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -4566,6 +4708,9 @@
         <v>635</v>
       </c>
       <c r="M46" s="18"/>
+      <c r="N46" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O46" s="8"/>
     </row>
     <row r="47" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -4606,6 +4751,9 @@
         <v>636</v>
       </c>
       <c r="M47" s="18"/>
+      <c r="N47" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
@@ -4645,6 +4793,9 @@
         <v>611</v>
       </c>
       <c r="M48" s="15"/>
+      <c r="N48" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O48" s="8"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -4684,6 +4835,9 @@
       <c r="L49" s="6" t="s">
         <v>602</v>
       </c>
+      <c r="N49" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O49" s="8"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -4723,6 +4877,9 @@
       <c r="L50" s="20" t="s">
         <v>627</v>
       </c>
+      <c r="N50" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O50" s="8"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -4762,6 +4919,9 @@
       <c r="L51" s="20" t="s">
         <v>628</v>
       </c>
+      <c r="N51" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
@@ -4800,6 +4960,9 @@
       <c r="L52" s="12" t="s">
         <v>662</v>
       </c>
+      <c r="N52" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O52" s="8"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -4839,6 +5002,9 @@
       <c r="L53" s="12" t="s">
         <v>663</v>
       </c>
+      <c r="N53" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O53" s="8"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -4879,6 +5045,9 @@
       <c r="M54" s="8" t="s">
         <v>704</v>
       </c>
+      <c r="N54" s="6" t="s">
+        <v>722</v>
+      </c>
       <c r="O54" s="8"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -4919,6 +5088,9 @@
       <c r="M55" s="8" t="s">
         <v>703</v>
       </c>
+      <c r="N55" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
@@ -4958,6 +5130,9 @@
       <c r="M56" s="8" t="s">
         <v>706</v>
       </c>
+      <c r="N56" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
@@ -4997,6 +5172,9 @@
       <c r="M57" s="8" t="s">
         <v>705</v>
       </c>
+      <c r="N57" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
@@ -5036,6 +5214,9 @@
       <c r="M58" s="8" t="s">
         <v>708</v>
       </c>
+      <c r="N58" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
@@ -5075,6 +5256,9 @@
       <c r="M59" s="8" t="s">
         <v>707</v>
       </c>
+      <c r="N59" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -5096,6 +5280,9 @@
       <c r="G60" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="N60" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
@@ -5125,6 +5312,9 @@
       <c r="M61" s="8" t="s">
         <v>720</v>
       </c>
+      <c r="N61" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
@@ -5154,6 +5344,9 @@
       <c r="M62" s="8" t="s">
         <v>719</v>
       </c>
+      <c r="N62" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
@@ -5182,6 +5375,9 @@
       </c>
       <c r="M63" s="8" t="s">
         <v>721</v>
+      </c>
+      <c r="N63" s="6" t="s">
+        <v>722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wbes acronyms updated in config
</commit_message>
<xml_diff>
--- a/config/remc_report_config.xlsx
+++ b/config/remc_report_config.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3540" uniqueCount="756">
   <si>
     <t>name</t>
   </si>
@@ -926,9 +926,6 @@
     <t>WR_WR_WIND _AVC</t>
   </si>
   <si>
-    <t>SOLAPUR</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00045839</t>
   </si>
   <si>
@@ -944,9 +941,6 @@
     <t>WR_WR_SOLAR _AVC</t>
   </si>
   <si>
-    <t>SIPAT1</t>
-  </si>
-  <si>
     <t>WREMCPRI.SCADA01.00045841</t>
   </si>
   <si>
@@ -2225,17 +2219,110 @@
     <t>WR-ISTS_COMBINED</t>
   </si>
   <si>
+    <t>OKWPL_RE</t>
+  </si>
+  <si>
+    <t>RPL_SECI_II_RE</t>
+  </si>
+  <si>
+    <t>OEPL</t>
+  </si>
+  <si>
+    <t>GIWEL_SECI_II_RE</t>
+  </si>
+  <si>
+    <t>GIWEL_SECI_III_RE</t>
+  </si>
+  <si>
+    <t>IGESL_DAYAPAR_BHUJ_W</t>
+  </si>
+  <si>
+    <t>AWEK1L</t>
+  </si>
+  <si>
+    <t>AlfanarWind_SECI_III</t>
+  </si>
+  <si>
+    <t>RWE_AP2_SECI_III</t>
+  </si>
+  <si>
+    <t>AWEKFL</t>
+  </si>
+  <si>
+    <t>CPTTNPL</t>
+  </si>
+  <si>
+    <t>ASIPL_BARANDA</t>
+  </si>
+  <si>
+    <t>NETRA_KOTDA_BHUJ_W</t>
+  </si>
+  <si>
+    <t>NTPC_REL_DYPR_BHUJ_W</t>
+  </si>
+  <si>
+    <t>SRIJAN_MORJAR_BHJ2_W</t>
+  </si>
+  <si>
+    <t>SITAC_CHUGGER_BHJ2_W</t>
+  </si>
+  <si>
+    <t>AWEK4L_DEDYA_BHUJ2_W</t>
+  </si>
+  <si>
+    <t>POWERICA</t>
+  </si>
+  <si>
+    <t>APRAAVA_KHKRDA_JAM_W</t>
+  </si>
+  <si>
+    <t>Torrent_Sidpur_Jam_W</t>
+  </si>
+  <si>
+    <t>AWEMP1PL_PTNGR_IDR_W</t>
+  </si>
+  <si>
+    <t>Arinsun_RUMS</t>
+  </si>
+  <si>
+    <t>Athena_RUMS</t>
+  </si>
+  <si>
+    <t>Mahindra_RUMS</t>
+  </si>
+  <si>
+    <t>SGEL_RSP_S</t>
+  </si>
+  <si>
+    <t>KAWAS_SOLAR</t>
+  </si>
+  <si>
+    <t>GANDHAR_SOLAR</t>
+  </si>
+  <si>
+    <t>SHERISHA_RAIPUR_S</t>
+  </si>
+  <si>
+    <t>SOLAPUR_SOLAR</t>
+  </si>
+  <si>
+    <t>MASAYA_BWSPRA_KNDW_S</t>
+  </si>
+  <si>
+    <t>AREH4L_PSS1_KPS1_SF</t>
+  </si>
+  <si>
+    <t>BEEMPOW_AGAR_RUMS_S</t>
+  </si>
+  <si>
     <t>AVAADA_AGAR_RUMS_S</t>
-  </si>
-  <si>
-    <t>BEEMPOW_AGAR_RUMS_S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2267,8 +2354,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2285,8 +2385,14 @@
         <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2331,11 +2437,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2379,15 +2498,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2695,14 +2827,14 @@
   </sheetPr>
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I34" workbookViewId="0">
-      <selection activeCell="N49" sqref="N49"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="90.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="28.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -2713,7 +2845,7 @@
     <col min="11" max="11" width="44.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="44.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="38.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2798,9 +2930,7 @@
       <c r="M2" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>292</v>
-      </c>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2810,10 +2940,10 @@
         <v>25692.21</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>294</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>131</v>
@@ -2822,7 +2952,7 @@
         <v>288</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>30</v>
@@ -2831,17 +2961,15 @@
         <v>32</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>296</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>297</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -2851,19 +2979,19 @@
         <v>46373.59</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>301</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>288</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>24</v>
@@ -2872,17 +3000,15 @@
         <v>26</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -2892,10 +3018,10 @@
         <v>250</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>149</v>
@@ -2904,28 +3030,28 @@
         <v>128</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>298</v>
+      <c r="N5" s="20" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2936,10 +3062,10 @@
         <v>230</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>149</v>
@@ -2948,28 +3074,28 @@
         <v>128</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="M6" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>298</v>
+      <c r="N6" s="20" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2980,10 +3106,10 @@
         <v>50</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>149</v>
@@ -2992,28 +3118,28 @@
         <v>128</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="L7" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="L7" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>298</v>
+      <c r="N7" s="20" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3024,10 +3150,10 @@
         <v>250</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>155</v>
@@ -3036,28 +3162,28 @@
         <v>128</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="L8" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>298</v>
+      <c r="N8" s="20" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3068,10 +3194,10 @@
         <v>300</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>155</v>
@@ -3080,28 +3206,28 @@
         <v>128</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>298</v>
+      <c r="N9" s="20" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3112,10 +3238,10 @@
         <v>250</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>155</v>
@@ -3124,28 +3250,28 @@
         <v>128</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H10" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="L10" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>298</v>
+      <c r="N10" s="20" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3156,10 +3282,10 @@
         <v>425</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>155</v>
@@ -3168,28 +3294,28 @@
         <v>128</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>298</v>
+      <c r="N11" s="20" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3200,10 +3326,10 @@
         <v>300</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>155</v>
@@ -3212,28 +3338,28 @@
         <v>128</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H12" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="L12" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>298</v>
+      <c r="N12" s="20" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3244,10 +3370,10 @@
         <v>300</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>155</v>
@@ -3256,28 +3382,28 @@
         <v>128</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H13" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="L13" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>298</v>
+      <c r="N13" s="20" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3288,10 +3414,10 @@
         <v>131.5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>155</v>
@@ -3300,28 +3426,28 @@
         <v>128</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="M14" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="L14" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>298</v>
+      <c r="N14" s="20" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3332,10 +3458,10 @@
         <v>126</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>155</v>
@@ -3344,28 +3470,28 @@
         <v>128</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H15" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="M15" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>298</v>
+      <c r="N15" s="20" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3376,10 +3502,10 @@
         <v>166</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>155</v>
@@ -3388,28 +3514,28 @@
         <v>128</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H16" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="L16" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="L16" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>298</v>
+      <c r="N16" s="20" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3420,10 +3546,10 @@
         <v>206.5</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>155</v>
@@ -3432,28 +3558,28 @@
         <v>128</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H17" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="K17" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="L17" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="M17" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="L17" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>298</v>
+      <c r="N17" s="20" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3464,10 +3590,10 @@
         <v>140</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>155</v>
@@ -3476,28 +3602,28 @@
         <v>128</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H18" s="14" t="s">
+        <v>410</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="J18" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="K18" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="L18" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="M18" s="17" t="s">
         <v>415</v>
       </c>
-      <c r="L18" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="M18" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>298</v>
+      <c r="N18" s="21" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3508,10 +3634,10 @@
         <v>159.30000000000001</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>168</v>
@@ -3520,28 +3646,28 @@
         <v>128</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H19" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="K19" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="L19" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="M19" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="L19" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>298</v>
+      <c r="N19" s="20" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3552,10 +3678,10 @@
         <v>302.39999999999998</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>168</v>
@@ -3564,28 +3690,28 @@
         <v>128</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H20" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="M20" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="L20" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>298</v>
+      <c r="N20" s="20" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3596,10 +3722,10 @@
         <v>300</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>168</v>
@@ -3608,28 +3734,28 @@
         <v>128</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H21" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="K21" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="M21" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="L21" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>298</v>
+      <c r="N21" s="20" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3640,10 +3766,10 @@
         <v>50.6</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>255</v>
@@ -3652,28 +3778,28 @@
         <v>128</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="K22" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="L22" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="M22" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>298</v>
+      <c r="N22" s="20" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3684,10 +3810,10 @@
         <v>252</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>255</v>
@@ -3696,28 +3822,28 @@
         <v>128</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H23" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="K23" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="L23" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="M23" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="L23" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>298</v>
+      <c r="N23" s="21" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3728,10 +3854,10 @@
         <v>115</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>255</v>
@@ -3740,28 +3866,28 @@
         <v>128</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H24" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="K24" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="L24" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="M24" s="18" t="s">
         <v>463</v>
       </c>
-      <c r="L24" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="M24" s="15" t="s">
-        <v>465</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>298</v>
+      <c r="N24" s="21" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3772,10 +3898,10 @@
         <v>324.39999999999998</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>264</v>
@@ -3784,28 +3910,28 @@
         <v>128</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="L25" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="M25" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="L25" s="4" t="s">
-        <v>472</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>298</v>
+      <c r="N25" s="20" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="26" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3816,10 +3942,10 @@
         <v>250</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>181</v>
@@ -3828,28 +3954,28 @@
         <v>131</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H26" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="L26" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="M26" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="L26" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>298</v>
+      <c r="N26" s="20" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3860,10 +3986,10 @@
         <v>250</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>181</v>
@@ -3872,28 +3998,28 @@
         <v>131</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H27" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="L27" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="M27" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="L27" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="M27" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>298</v>
+      <c r="N27" s="20" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3904,10 +4030,10 @@
         <v>250</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>181</v>
@@ -3916,28 +4042,28 @@
         <v>131</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H28" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="K28" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="L28" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="M28" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="L28" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>298</v>
+      <c r="N28" s="20" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3948,10 +4074,10 @@
         <v>100</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>186</v>
@@ -3960,28 +4086,28 @@
         <v>131</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H29" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="K29" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="L29" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="M29" s="19" t="s">
         <v>503</v>
       </c>
-      <c r="L29" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>298</v>
+      <c r="N29" s="22" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3992,10 +4118,10 @@
         <v>100</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>186</v>
@@ -4004,28 +4130,28 @@
         <v>131</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H30" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="K30" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="L30" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="M30" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="L30" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>298</v>
+      <c r="N30" s="23" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4036,10 +4162,10 @@
         <v>200</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>186</v>
@@ -4048,28 +4174,28 @@
         <v>131</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H31" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="J31" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="L31" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="M31" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="L31" s="4" t="s">
-        <v>520</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>298</v>
+      <c r="N31" s="23" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4080,10 +4206,10 @@
         <v>100</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>186</v>
@@ -4092,28 +4218,28 @@
         <v>131</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H32" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="K32" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="L32" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="M32" s="19" t="s">
         <v>527</v>
       </c>
-      <c r="L32" s="4" t="s">
-        <v>528</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="N32" s="4" t="s">
-        <v>298</v>
+      <c r="N32" s="23" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4124,10 +4250,10 @@
         <v>100</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>186</v>
@@ -4136,28 +4262,28 @@
         <v>131</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H33" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="K33" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="L33" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="K33" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>536</v>
-      </c>
-      <c r="M33" s="15" t="s">
-        <v>529</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>298</v>
+      <c r="M33" s="18" t="s">
+        <v>527</v>
+      </c>
+      <c r="N33" s="23" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4168,10 +4294,10 @@
         <v>100</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>186</v>
@@ -4180,28 +4306,28 @@
         <v>131</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H34" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="K34" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="L34" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="M34" s="18" t="s">
         <v>542</v>
       </c>
-      <c r="L34" s="4" t="s">
-        <v>543</v>
-      </c>
-      <c r="M34" s="15" t="s">
-        <v>544</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>298</v>
+      <c r="N34" s="21" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4212,10 +4338,10 @@
         <v>56</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>194</v>
@@ -4224,28 +4350,28 @@
         <v>131</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H35" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="K35" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="L35" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="M35" s="19" t="s">
         <v>550</v>
       </c>
-      <c r="L35" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>298</v>
+      <c r="N35" s="24" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4256,10 +4382,10 @@
         <v>20</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>197</v>
@@ -4268,28 +4394,28 @@
         <v>131</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H36" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="K36" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="L36" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="M36" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="L36" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="M36" s="3" t="s">
-        <v>560</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>298</v>
+      <c r="N36" s="20" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4300,10 +4426,10 @@
         <v>50</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>200</v>
@@ -4312,28 +4438,28 @@
         <v>131</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H37" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="K37" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="L37" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="M37" s="19" t="s">
         <v>566</v>
       </c>
-      <c r="L37" s="4" t="s">
-        <v>567</v>
-      </c>
-      <c r="M37" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="N37" s="4" t="s">
-        <v>298</v>
+      <c r="N37" s="21" t="s">
+        <v>750</v>
       </c>
     </row>
     <row r="38" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4344,10 +4470,10 @@
         <v>10</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>203</v>
@@ -4356,28 +4482,28 @@
         <v>131</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H38" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="K38" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="L38" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="K38" s="4" t="s">
+      <c r="M38" s="19" t="s">
         <v>574</v>
       </c>
-      <c r="L38" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="M38" s="3" t="s">
-        <v>576</v>
-      </c>
-      <c r="N38" s="4" t="s">
-        <v>298</v>
+      <c r="N38" s="21" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4388,10 +4514,10 @@
         <v>300</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>216</v>
@@ -4400,26 +4526,26 @@
         <v>131</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H39" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="K39" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="L39" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="K39" s="4" t="s">
-        <v>582</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>583</v>
-      </c>
       <c r="M39" s="4"/>
-      <c r="N39" s="4" t="s">
-        <v>298</v>
+      <c r="N39" s="20" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4430,10 +4556,10 @@
         <v>1000</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>218</v>
@@ -4442,26 +4568,26 @@
         <v>131</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H40" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="K40" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="L40" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="K40" s="4" t="s">
-        <v>589</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>590</v>
-      </c>
       <c r="M40" s="4"/>
-      <c r="N40" s="4" t="s">
-        <v>298</v>
+      <c r="N40" s="21" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4472,10 +4598,10 @@
         <v>583</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>218</v>
@@ -4484,25 +4610,26 @@
         <v>131</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H41" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="J41" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="K41" s="4" t="s">
         <v>594</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="L41" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="K41" s="4" t="s">
-        <v>596</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="N41" s="4" t="s">
-        <v>298</v>
+      <c r="M41" s="19"/>
+      <c r="N41" s="23" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4513,10 +4640,10 @@
         <v>167</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>218</v>
@@ -4525,25 +4652,26 @@
         <v>131</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H42" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="J42" s="4" t="s">
         <v>600</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="K42" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="L42" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="K42" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="L42" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="N42" s="4" t="s">
-        <v>298</v>
+      <c r="M42" s="19"/>
+      <c r="N42" s="23" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4554,10 +4682,10 @@
         <v>500</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>218</v>
@@ -4566,25 +4694,26 @@
         <v>131</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H43" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="K43" s="4" t="s">
         <v>608</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="L43" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="L43" s="4" t="s">
-        <v>611</v>
-      </c>
-      <c r="N43" s="4" t="s">
-        <v>298</v>
+      <c r="M43" s="19"/>
+      <c r="N43" s="23" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4595,10 +4724,10 @@
         <v>12.5</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>218</v>
@@ -4607,26 +4736,26 @@
         <v>131</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H44" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="J44" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="K44" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="L44" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="K44" s="4" t="s">
-        <v>617</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>618</v>
-      </c>
       <c r="M44" s="4"/>
-      <c r="N44" s="4" t="s">
-        <v>298</v>
+      <c r="N44" s="23" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4637,10 +4766,10 @@
         <v>162.5</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>218</v>
@@ -4649,25 +4778,26 @@
         <v>131</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H45" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="J45" s="4" t="s">
         <v>621</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="K45" s="4" t="s">
         <v>622</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="L45" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="K45" s="4" t="s">
-        <v>624</v>
-      </c>
-      <c r="L45" s="4" t="s">
-        <v>625</v>
-      </c>
-      <c r="N45" s="4" t="s">
-        <v>298</v>
+      <c r="M45" s="19"/>
+      <c r="N45" s="23" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4678,10 +4808,10 @@
         <v>200</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>218</v>
@@ -4690,26 +4820,26 @@
         <v>131</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H46" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="J46" s="4" t="s">
         <v>628</v>
       </c>
-      <c r="I46" s="4" t="s">
+      <c r="K46" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="L46" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="K46" s="4" t="s">
-        <v>631</v>
-      </c>
-      <c r="L46" s="4" t="s">
-        <v>632</v>
-      </c>
       <c r="M46" s="4"/>
-      <c r="N46" s="4" t="s">
-        <v>298</v>
+      <c r="N46" s="23" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4720,10 +4850,10 @@
         <v>25</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>218</v>
@@ -4732,26 +4862,26 @@
         <v>131</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H47" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="J47" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="K47" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="J47" s="3" t="s">
+      <c r="L47" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="K47" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="L47" s="3" t="s">
-        <v>625</v>
-      </c>
       <c r="M47" s="4"/>
-      <c r="N47" s="4" t="s">
-        <v>298</v>
+      <c r="N47" s="23" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4762,10 +4892,10 @@
         <v>350</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>227</v>
@@ -4774,26 +4904,26 @@
         <v>131</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H48" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="J48" s="4" t="s">
         <v>635</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="K48" s="4" t="s">
         <v>636</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="L48" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="K48" s="4" t="s">
-        <v>638</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>639</v>
-      </c>
       <c r="M48" s="4"/>
-      <c r="N48" s="4" t="s">
-        <v>726</v>
+      <c r="N48" s="23" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="49" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4804,10 +4934,10 @@
         <v>200</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>227</v>
@@ -4816,25 +4946,26 @@
         <v>131</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H49" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="J49" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="I49" s="4" t="s">
+      <c r="K49" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="L49" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="K49" s="4" t="s">
-        <v>645</v>
-      </c>
-      <c r="L49" s="4" t="s">
-        <v>646</v>
-      </c>
-      <c r="N49" s="4" t="s">
-        <v>725</v>
+      <c r="M49" s="19"/>
+      <c r="N49" s="23" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="50" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4844,11 +4975,11 @@
       <c r="B50" s="12">
         <v>100</v>
       </c>
-      <c r="C50" s="16" t="s">
-        <v>647</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>648</v>
+      <c r="C50" s="15" t="s">
+        <v>645</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>646</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>227</v>
@@ -4857,24 +4988,25 @@
         <v>131</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H50" s="14" t="s">
+        <v>647</v>
+      </c>
+      <c r="I50" s="14" t="s">
+        <v>648</v>
+      </c>
+      <c r="J50" s="14" t="s">
         <v>649</v>
       </c>
-      <c r="I50" s="14" t="s">
+      <c r="K50" s="14" t="s">
         <v>650</v>
       </c>
-      <c r="J50" s="14" t="s">
+      <c r="L50" s="15" t="s">
         <v>651</v>
       </c>
-      <c r="K50" s="14" t="s">
-        <v>652</v>
-      </c>
-      <c r="L50" s="16" t="s">
-        <v>653</v>
-      </c>
-      <c r="N50" s="4" t="s">
+      <c r="M50" s="19"/>
+      <c r="N50" s="23" t="s">
         <v>229</v>
       </c>
     </row>
@@ -4885,11 +5017,11 @@
       <c r="B51" s="12">
         <v>105</v>
       </c>
-      <c r="C51" s="16" t="s">
-        <v>654</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>655</v>
+      <c r="C51" s="15" t="s">
+        <v>652</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>653</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>227</v>
@@ -4898,24 +5030,25 @@
         <v>131</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H51" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="J51" s="14" t="s">
         <v>656</v>
       </c>
-      <c r="I51" s="14" t="s">
+      <c r="K51" s="14" t="s">
         <v>657</v>
       </c>
-      <c r="J51" s="14" t="s">
+      <c r="L51" s="15" t="s">
         <v>658</v>
       </c>
-      <c r="K51" s="14" t="s">
-        <v>659</v>
-      </c>
-      <c r="L51" s="16" t="s">
-        <v>660</v>
-      </c>
-      <c r="N51" s="4" t="s">
+      <c r="M51" s="19"/>
+      <c r="N51" s="23" t="s">
         <v>230</v>
       </c>
     </row>
@@ -4927,10 +5060,10 @@
         <v>170</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>232</v>
@@ -4939,24 +5072,25 @@
         <v>131</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H52" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="J52" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="I52" s="4" t="s">
+      <c r="K52" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="L52" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="K52" s="4" t="s">
-        <v>666</v>
-      </c>
-      <c r="L52" s="4" t="s">
-        <v>667</v>
-      </c>
-      <c r="N52" s="4" t="s">
+      <c r="M52" s="19"/>
+      <c r="N52" s="23" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4968,10 +5102,10 @@
         <v>160</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>232</v>
@@ -4980,24 +5114,25 @@
         <v>131</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H53" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="J53" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="K53" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="L53" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="K53" s="4" t="s">
-        <v>673</v>
-      </c>
-      <c r="L53" s="4" t="s">
-        <v>674</v>
-      </c>
-      <c r="N53" s="4" t="s">
+      <c r="M53" s="19"/>
+      <c r="N53" s="23" t="s">
         <v>233</v>
       </c>
     </row>
@@ -5009,10 +5144,10 @@
         <v>12069</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
@@ -5022,7 +5157,7 @@
         <v>120</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>80</v>
@@ -5031,17 +5166,15 @@
         <v>82</v>
       </c>
       <c r="K54" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>677</v>
+      </c>
+      <c r="M54" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="L54" s="4" t="s">
-        <v>679</v>
-      </c>
-      <c r="M54" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="N54" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N54" s="4"/>
     </row>
     <row r="55" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
@@ -5051,10 +5184,10 @@
         <v>8340</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4" t="s">
@@ -5064,7 +5197,7 @@
         <v>120</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>75</v>
@@ -5073,17 +5206,15 @@
         <v>77</v>
       </c>
       <c r="K55" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="M55" s="3" t="s">
         <v>684</v>
       </c>
-      <c r="L55" s="4" t="s">
-        <v>685</v>
-      </c>
-      <c r="M55" s="3" t="s">
-        <v>686</v>
-      </c>
-      <c r="N55" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N55" s="4"/>
     </row>
     <row r="56" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
@@ -5093,10 +5224,10 @@
         <v>5078</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4" t="s">
@@ -5106,7 +5237,7 @@
         <v>120</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>110</v>
@@ -5115,17 +5246,15 @@
         <v>112</v>
       </c>
       <c r="K56" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="M56" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="L56" s="4" t="s">
-        <v>691</v>
-      </c>
-      <c r="M56" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="N56" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N56" s="4"/>
     </row>
     <row r="57" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
@@ -5135,10 +5264,10 @@
         <v>5274</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4" t="s">
@@ -5148,7 +5277,7 @@
         <v>120</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>105</v>
@@ -5157,17 +5286,15 @@
         <v>107</v>
       </c>
       <c r="K57" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="M57" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="L57" s="4" t="s">
-        <v>697</v>
-      </c>
-      <c r="M57" s="3" t="s">
-        <v>698</v>
-      </c>
-      <c r="N57" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N57" s="4"/>
     </row>
     <row r="58" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
@@ -5177,10 +5304,10 @@
         <v>2082.21</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4" t="s">
@@ -5190,7 +5317,7 @@
         <v>120</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>95</v>
@@ -5199,17 +5326,15 @@
         <v>97</v>
       </c>
       <c r="K58" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="M58" s="3" t="s">
         <v>702</v>
       </c>
-      <c r="L58" s="4" t="s">
-        <v>703</v>
-      </c>
-      <c r="M58" s="3" t="s">
-        <v>704</v>
-      </c>
-      <c r="N58" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -5219,10 +5344,10 @@
         <v>2528.6799999999998</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4" t="s">
@@ -5232,7 +5357,7 @@
         <v>120</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>90</v>
@@ -5241,17 +5366,15 @@
         <v>92</v>
       </c>
       <c r="K59" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="M59" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="L59" s="4" t="s">
-        <v>709</v>
-      </c>
-      <c r="M59" s="3" t="s">
-        <v>710</v>
-      </c>
-      <c r="N59" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
@@ -5261,10 +5384,10 @@
         <v>842</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4" t="s">
@@ -5273,23 +5396,21 @@
       <c r="G60" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="N60" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N60" s="4"/>
     </row>
     <row r="61" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B61" s="17"/>
+      <c r="B61" s="16"/>
       <c r="F61" s="4" t="s">
         <v>131</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>45</v>
@@ -5298,31 +5419,29 @@
         <v>47</v>
       </c>
       <c r="K61" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>713</v>
+      </c>
+      <c r="M61" s="3" t="s">
         <v>714</v>
       </c>
-      <c r="L61" s="4" t="s">
-        <v>715</v>
-      </c>
-      <c r="M61" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="N61" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N61" s="4"/>
     </row>
     <row r="62" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B62" s="17"/>
+      <c r="B62" s="16"/>
       <c r="F62" s="4" t="s">
         <v>128</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>50</v>
@@ -5331,31 +5450,29 @@
         <v>52</v>
       </c>
       <c r="K62" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="L62" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="M62" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="L62" s="4" t="s">
-        <v>719</v>
-      </c>
-      <c r="M62" s="3" t="s">
-        <v>720</v>
-      </c>
-      <c r="N62" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N62" s="4"/>
     </row>
     <row r="63" spans="1:14" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B63" s="17"/>
+      <c r="B63" s="16"/>
       <c r="F63" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>40</v>
@@ -5364,19 +5481,18 @@
         <v>42</v>
       </c>
       <c r="K63" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="L63" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="M63" s="3" t="s">
         <v>722</v>
       </c>
-      <c r="L63" s="4" t="s">
-        <v>723</v>
-      </c>
-      <c r="M63" s="3" t="s">
-        <v>724</v>
-      </c>
-      <c r="N63" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="N63" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N63"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11521,7 +11637,9 @@
   </sheetPr>
   <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>